<commit_message>
K4S_DA_A2_GAM_Temporal_Results.xlsx: adding in the GAMs results for A3
</commit_message>
<xml_diff>
--- a/K4S_key_scripts/K4S_DA_Aims/K4S_DA_A2/K4S_DA_A2/K4S_DA_A2_GAM_Temporal_Results.xlsx
+++ b/K4S_key_scripts/K4S_DA_Aims/K4S_DA_A2/K4S_DA_A2/K4S_DA_A2_GAM_Temporal_Results.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoestarkey/Desktop/Honours/Data_Analysis/K_axis_midoc/K4S_key_scripts/K4S_DA_Aims/K4S_DA_A2/K4S_DA_A2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A29D8D23-4E1C-1E46-A6C3-E9377AA5FA41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20759A6-EBCA-F449-B46E-6D12F37C656B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38620" yWindow="500" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{33E5A15D-DBA6-5B40-873E-91FBDBF28531}"/>
+    <workbookView xWindow="5600" yWindow="900" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{33E5A15D-DBA6-5B40-873E-91FBDBF28531}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="GAM_Temporal_Sum" sheetId="1" r:id="rId1"/>
+    <sheet name="GAM_Temporal_Depth" sheetId="2" r:id="rId2"/>
+    <sheet name="GAM_Sat+Insitu_Sum" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="49">
   <si>
     <t>Season</t>
   </si>
@@ -151,10 +152,52 @@
 800-1000</t>
   </si>
   <si>
-    <t>GAM SUMMARY</t>
-  </si>
-  <si>
     <t>GAMM + RE SUMMARY</t>
+  </si>
+  <si>
+    <t>Satellite Factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time since melt </t>
+  </si>
+  <si>
+    <t>Chlorophyll</t>
+  </si>
+  <si>
+    <t>Curent speed</t>
+  </si>
+  <si>
+    <t>Sea surface temperature</t>
+  </si>
+  <si>
+    <t>R-sq. (adj)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n </t>
+  </si>
+  <si>
+    <r>
+      <t>Chlorophyll-</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>a</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ALL TAXA </t>
+  </si>
+  <si>
+    <t>CEPHALOPODS</t>
+  </si>
+  <si>
+    <t>KRILL</t>
   </si>
 </sst>
 </file>
@@ -165,7 +208,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -195,6 +238,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
@@ -347,7 +397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -363,8 +413,12 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -628,6 +682,7 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -643,6 +698,9 @@
     <xf numFmtId="164" fontId="2" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -654,81 +712,57 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEBA8"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEBA8"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEBA8"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEBA8"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <b/>
@@ -1105,7 +1139,7 @@
   <dimension ref="B3:H17"/>
   <sheetViews>
     <sheetView zoomScale="169" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B12"/>
+      <selection activeCell="B4" sqref="B4:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1155,19 +1189,19 @@
       <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="11">
-        <v>1</v>
-      </c>
-      <c r="E5" s="11">
-        <v>1</v>
-      </c>
-      <c r="F5" s="11">
+      <c r="D5" s="13">
+        <v>1</v>
+      </c>
+      <c r="E5" s="13">
+        <v>1</v>
+      </c>
+      <c r="F5" s="13">
         <v>0.877</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="15">
         <v>0.35599999999999998</v>
       </c>
-      <c r="H5" s="10" t="str">
+      <c r="H5" s="11" t="str">
         <f>IF(G5&lt;0.05, G5, "&gt;0.05")</f>
         <v>&gt;0.05</v>
       </c>
@@ -1177,19 +1211,19 @@
       <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="11">
-        <v>1</v>
-      </c>
-      <c r="E6" s="11">
-        <v>1</v>
-      </c>
-      <c r="F6" s="11">
+      <c r="D6" s="13">
+        <v>1</v>
+      </c>
+      <c r="E6" s="13">
+        <v>1</v>
+      </c>
+      <c r="F6" s="13">
         <v>0.24399999999999999</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="15">
         <v>0.63900000000000001</v>
       </c>
-      <c r="H6" s="10" t="str">
+      <c r="H6" s="11" t="str">
         <f>IF(G6&lt;0.05, G6, "&gt;0.05")</f>
         <v>&gt;0.05</v>
       </c>
@@ -1199,19 +1233,19 @@
       <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="13">
         <v>1.65</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="13">
         <v>2.048</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="13">
         <v>0.86699999999999999</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="15">
         <v>0.41899999999999998</v>
       </c>
-      <c r="H7" s="10" t="str">
+      <c r="H7" s="11" t="str">
         <f>IF(G7&lt;0.05, G7, "&gt;0.05")</f>
         <v>&gt;0.05</v>
       </c>
@@ -1221,19 +1255,19 @@
       <c r="C8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="14">
         <v>6.8639999999999999</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="14">
         <v>7.9480000000000004</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="14">
         <v>4.625</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8" s="16">
         <v>2.3999999999999998E-3</v>
       </c>
-      <c r="H8" s="15">
+      <c r="H8" s="17">
         <f>IF(G8&lt;0.05, G8, "&gt;0.05")</f>
         <v>2.3999999999999998E-3</v>
       </c>
@@ -1245,19 +1279,19 @@
       <c r="C9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="11">
-        <v>1</v>
-      </c>
-      <c r="E9" s="11">
-        <v>1</v>
-      </c>
-      <c r="F9" s="11">
+      <c r="D9" s="13">
+        <v>1</v>
+      </c>
+      <c r="E9" s="13">
+        <v>1</v>
+      </c>
+      <c r="F9" s="13">
         <v>0.57699999999999996</v>
       </c>
-      <c r="G9" s="13">
+      <c r="G9" s="15">
         <v>0.45300000000000001</v>
       </c>
-      <c r="H9" s="16" t="str">
+      <c r="H9" s="18" t="str">
         <f>IF(G9&lt;0.05, G9, "&gt;0.05")</f>
         <v>&gt;0.05</v>
       </c>
@@ -1267,19 +1301,19 @@
       <c r="C10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="11">
-        <v>1</v>
-      </c>
-      <c r="E10" s="11">
-        <v>1</v>
-      </c>
-      <c r="F10" s="11">
+      <c r="D10" s="13">
+        <v>1</v>
+      </c>
+      <c r="E10" s="13">
+        <v>1</v>
+      </c>
+      <c r="F10" s="13">
         <v>0.66900000000000004</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="15">
         <v>0.41899999999999998</v>
       </c>
-      <c r="H10" s="10" t="str">
+      <c r="H10" s="11" t="str">
         <f>IF(G10&lt;0.05, G10, "&gt;0.05")</f>
         <v>&gt;0.05</v>
       </c>
@@ -1289,19 +1323,19 @@
       <c r="C11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="11">
-        <v>1</v>
-      </c>
-      <c r="E11" s="11">
-        <v>1</v>
-      </c>
-      <c r="F11" s="11">
+      <c r="D11" s="13">
+        <v>1</v>
+      </c>
+      <c r="E11" s="13">
+        <v>1</v>
+      </c>
+      <c r="F11" s="13">
         <v>0.56599999999999995</v>
       </c>
-      <c r="G11" s="13">
+      <c r="G11" s="15">
         <v>0.45700000000000002</v>
       </c>
-      <c r="H11" s="10" t="str">
+      <c r="H11" s="11" t="str">
         <f>IF(G11&lt;0.05, G11, "&gt;0.05")</f>
         <v>&gt;0.05</v>
       </c>
@@ -1311,19 +1345,19 @@
       <c r="C12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="14">
         <v>2.1059999999999999</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="14">
         <v>2.6280000000000001</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="14">
         <v>2.4089999999999998</v>
       </c>
-      <c r="G12" s="14">
+      <c r="G12" s="16">
         <v>0.106</v>
       </c>
-      <c r="H12" s="14" t="str">
+      <c r="H12" s="16" t="str">
         <f>IF(G12&lt;0.05, G12, "&gt;0.05")</f>
         <v>&gt;0.05</v>
       </c>
@@ -1335,19 +1369,19 @@
       <c r="C13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="13">
         <v>1.625</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="13">
         <v>1.9890000000000001</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="13">
         <v>1.0920000000000001</v>
       </c>
-      <c r="G13" s="13">
+      <c r="G13" s="15">
         <v>0.374</v>
       </c>
-      <c r="H13" s="10" t="str">
+      <c r="H13" s="11" t="str">
         <f>IF(G13&lt;0.05, G13, "&gt;0.05")</f>
         <v>&gt;0.05</v>
       </c>
@@ -1357,19 +1391,19 @@
       <c r="C14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="11">
-        <v>1</v>
-      </c>
-      <c r="E14" s="11">
-        <v>1</v>
-      </c>
-      <c r="F14" s="11">
+      <c r="D14" s="13">
+        <v>1</v>
+      </c>
+      <c r="E14" s="13">
+        <v>1</v>
+      </c>
+      <c r="F14" s="13">
         <v>0.54400000000000004</v>
       </c>
-      <c r="G14" s="13">
+      <c r="G14" s="15">
         <v>0.46600000000000003</v>
       </c>
-      <c r="H14" s="10" t="str">
+      <c r="H14" s="11" t="str">
         <f>IF(G14&lt;0.05, G14, "&gt;0.05")</f>
         <v>&gt;0.05</v>
       </c>
@@ -1379,19 +1413,19 @@
       <c r="C15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="11">
-        <v>1</v>
-      </c>
-      <c r="E15" s="11">
-        <v>1</v>
-      </c>
-      <c r="F15" s="11">
+      <c r="D15" s="13">
+        <v>1</v>
+      </c>
+      <c r="E15" s="13">
+        <v>1</v>
+      </c>
+      <c r="F15" s="13">
         <v>0.96399999999999997</v>
       </c>
-      <c r="G15" s="13">
+      <c r="G15" s="15">
         <v>0.33300000000000002</v>
       </c>
-      <c r="H15" s="10" t="str">
+      <c r="H15" s="11" t="str">
         <f>IF(G15&lt;0.05, G15, "&gt;0.05")</f>
         <v>&gt;0.05</v>
       </c>
@@ -1401,19 +1435,19 @@
       <c r="C16" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D16" s="14">
         <v>3.4529999999999998</v>
       </c>
-      <c r="E16" s="12">
+      <c r="E16" s="14">
         <v>4.2610000000000001</v>
       </c>
-      <c r="F16" s="12">
+      <c r="F16" s="14">
         <v>1.004</v>
       </c>
-      <c r="G16" s="14">
+      <c r="G16" s="16">
         <v>0.38800000000000001</v>
       </c>
-      <c r="H16" s="14" t="str">
+      <c r="H16" s="16" t="str">
         <f>IF(G16&lt;0.05, G16, "&gt;0.05")</f>
         <v>&gt;0.05</v>
       </c>
@@ -1433,7 +1467,7 @@
     <mergeCell ref="B13:B16"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:H16">
-    <cfRule type="cellIs" dxfId="5" priority="2" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1446,8 +1480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC0FF2A1-C6A7-6249-9809-08DF6541B68E}">
   <dimension ref="B4:N126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="109" zoomScaleNormal="117" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView topLeftCell="A20" zoomScale="109" zoomScaleNormal="117" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27:K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1489,105 +1523,105 @@
       <c r="C6" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="19" t="s">
         <v>15</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="10"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="11"/>
     </row>
     <row r="7" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C7" s="6"/>
-      <c r="D7" s="18"/>
+      <c r="D7" s="20"/>
       <c r="E7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="10"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="11"/>
     </row>
     <row r="8" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C8" s="6"/>
-      <c r="D8" s="18"/>
+      <c r="D8" s="20"/>
       <c r="E8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="10"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="11"/>
     </row>
     <row r="9" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9" s="6"/>
-      <c r="D9" s="18"/>
+      <c r="D9" s="20"/>
       <c r="E9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="10"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="11"/>
     </row>
     <row r="10" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="6"/>
-      <c r="D10" s="18"/>
+      <c r="D10" s="20"/>
       <c r="E10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="10"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="11"/>
     </row>
     <row r="11" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C11" s="6"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="10"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="11"/>
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C12" s="6"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="10"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="11"/>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C13" s="6"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="10"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="11"/>
     </row>
     <row r="14" spans="3:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C14" s="7"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="15"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="17"/>
     </row>
     <row r="15" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C15" s="6" t="s">
@@ -1595,41 +1629,41 @@
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="16"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="18"/>
     </row>
     <row r="16" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C16" s="6"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="10"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="11"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="10"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="11"/>
     </row>
     <row r="18" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C18" s="7"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C19" s="6" t="s">
@@ -1637,70 +1671,68 @@
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="10"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="11"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C20" s="6"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="10"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="11"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C21" s="6"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="10"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="11"/>
     </row>
     <row r="22" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C22" s="7"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B26" s="84"/>
-      <c r="C26" s="84"/>
-      <c r="D26" s="84"/>
-      <c r="E26" s="84"/>
-      <c r="F26" s="84"/>
-      <c r="G26" s="84"/>
-      <c r="H26" s="84"/>
-      <c r="I26" s="84"/>
-      <c r="J26" s="84"/>
-      <c r="K26" s="84"/>
+      <c r="B26" s="86"/>
+      <c r="C26" s="86"/>
+      <c r="D26" s="86"/>
+      <c r="E26" s="86"/>
+      <c r="F26" s="86"/>
+      <c r="G26" s="86"/>
+      <c r="H26" s="86"/>
+      <c r="I26" s="86"/>
+      <c r="J26" s="86"/>
+      <c r="K26" s="86"/>
     </row>
     <row r="27" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="84"/>
-      <c r="C27" s="106" t="s">
-        <v>37</v>
-      </c>
-      <c r="D27" s="106"/>
-      <c r="E27" s="106"/>
-      <c r="F27" s="106"/>
-      <c r="G27" s="106"/>
-      <c r="H27" s="106"/>
-      <c r="I27" s="106"/>
-      <c r="J27" s="105"/>
-      <c r="K27" s="84"/>
+      <c r="B27" s="86"/>
+      <c r="C27" s="109"/>
+      <c r="D27" s="109"/>
+      <c r="E27" s="109"/>
+      <c r="F27" s="109"/>
+      <c r="G27" s="109"/>
+      <c r="H27" s="109"/>
+      <c r="I27" s="109"/>
+      <c r="J27" s="107"/>
+      <c r="K27" s="86"/>
     </row>
     <row r="28" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="84"/>
+      <c r="B28" s="86"/>
       <c r="C28" s="2" t="s">
         <v>10</v>
       </c>
@@ -1723,281 +1755,281 @@
         <v>9</v>
       </c>
       <c r="J28" s="2"/>
-      <c r="K28" s="84"/>
+      <c r="K28" s="86"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B29" s="84"/>
-      <c r="C29" s="49" t="s">
+      <c r="B29" s="86"/>
+      <c r="C29" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="D29" s="44" t="s">
+      <c r="D29" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="E29" s="45" t="s">
+      <c r="E29" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="F29" s="46">
-        <v>1</v>
-      </c>
-      <c r="G29" s="46">
-        <v>1</v>
-      </c>
-      <c r="H29" s="46">
+      <c r="F29" s="48">
+        <v>1</v>
+      </c>
+      <c r="G29" s="48">
+        <v>1</v>
+      </c>
+      <c r="H29" s="48">
         <v>3.63</v>
       </c>
-      <c r="I29" s="47">
+      <c r="I29" s="49">
         <v>5.8599999999999999E-2</v>
       </c>
-      <c r="J29" s="107" t="str">
+      <c r="J29" s="110" t="str">
         <f>IF(I29&lt;0.05, "&lt;0.05", IF(I29&lt;0.1, "&lt;0.1", ""))</f>
         <v>&lt;0.1</v>
       </c>
-      <c r="K29" s="84"/>
+      <c r="K29" s="86"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B30" s="84"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="44" t="s">
+      <c r="B30" s="86"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="E30" s="45" t="s">
+      <c r="E30" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="F30" s="46">
-        <v>1</v>
-      </c>
-      <c r="G30" s="46">
-        <v>1</v>
-      </c>
-      <c r="H30" s="46">
+      <c r="F30" s="48">
+        <v>1</v>
+      </c>
+      <c r="G30" s="48">
+        <v>1</v>
+      </c>
+      <c r="H30" s="48">
         <v>3.165</v>
       </c>
-      <c r="I30" s="47">
+      <c r="I30" s="49">
         <v>7.7100000000000002E-2</v>
       </c>
-      <c r="J30" s="107" t="str">
+      <c r="J30" s="110" t="str">
         <f t="shared" ref="J30:J43" si="0">IF(I30&lt;0.05, "&lt;0.05", IF(I30&lt;0.1, "&lt;0.1", ""))</f>
         <v>&lt;0.1</v>
       </c>
-      <c r="K30" s="84"/>
+      <c r="K30" s="86"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B31" s="84"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="44" t="s">
+      <c r="B31" s="86"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E31" s="45" t="s">
+      <c r="E31" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="F31" s="46">
+      <c r="F31" s="48">
         <v>1.3680000000000001</v>
       </c>
-      <c r="G31" s="46">
+      <c r="G31" s="48">
         <v>1.647</v>
       </c>
-      <c r="H31" s="46">
+      <c r="H31" s="48">
         <v>4.798</v>
       </c>
-      <c r="I31" s="47">
+      <c r="I31" s="49">
         <v>3.0700000000000002E-2</v>
       </c>
-      <c r="J31" s="107" t="str">
+      <c r="J31" s="110" t="str">
         <f t="shared" si="0"/>
         <v>&lt;0.05</v>
       </c>
-      <c r="K31" s="84"/>
+      <c r="K31" s="86"/>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B32" s="84"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31" t="s">
+      <c r="B32" s="86"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33" t="s">
         <v>24</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F32" s="11">
+      <c r="F32" s="13">
         <v>3.988</v>
       </c>
-      <c r="G32" s="11">
+      <c r="G32" s="13">
         <v>4.923</v>
       </c>
-      <c r="H32" s="11">
+      <c r="H32" s="13">
         <v>3.2639999999999998</v>
       </c>
-      <c r="I32" s="22">
+      <c r="I32" s="24">
         <v>9.5999999999999992E-3</v>
       </c>
-      <c r="J32" s="108" t="str">
+      <c r="J32" s="111" t="str">
         <f t="shared" si="0"/>
         <v>&lt;0.05</v>
       </c>
-      <c r="K32" s="84"/>
+      <c r="K32" s="86"/>
     </row>
     <row r="33" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="84"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
+      <c r="B33" s="86"/>
+      <c r="C33" s="33"/>
+      <c r="D33" s="33"/>
       <c r="E33" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F33" s="11">
+      <c r="F33" s="13">
         <v>7.6529999999999996</v>
       </c>
-      <c r="G33" s="11">
+      <c r="G33" s="13">
         <v>8.1969999999999992</v>
       </c>
-      <c r="H33" s="11">
+      <c r="H33" s="13">
         <v>4.9729999999999999</v>
       </c>
-      <c r="I33" s="21">
+      <c r="I33" s="23">
         <v>2.6400000000000001E-5</v>
       </c>
       <c r="J33" s="8" t="str">
         <f t="shared" si="0"/>
         <v>&lt;0.05</v>
       </c>
-      <c r="K33" s="11"/>
-      <c r="L33" s="11"/>
-      <c r="M33" s="11"/>
-      <c r="N33" s="22"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+      <c r="N33" s="24"/>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B34" s="84"/>
-      <c r="C34" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="D34" s="29" t="s">
+      <c r="B34" s="86"/>
+      <c r="C34" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="E34" s="32" t="s">
+      <c r="E34" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="F34" s="33">
-        <v>1</v>
-      </c>
-      <c r="G34" s="33">
-        <v>1</v>
-      </c>
-      <c r="H34" s="33">
+      <c r="F34" s="35">
+        <v>1</v>
+      </c>
+      <c r="G34" s="35">
+        <v>1</v>
+      </c>
+      <c r="H34" s="35">
         <v>4.298</v>
       </c>
-      <c r="I34" s="34">
+      <c r="I34" s="36">
         <v>3.9699999999999999E-2</v>
       </c>
-      <c r="J34" s="80" t="str">
+      <c r="J34" s="82" t="str">
         <f t="shared" si="0"/>
         <v>&lt;0.05</v>
       </c>
-      <c r="K34" s="84"/>
+      <c r="K34" s="86"/>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B35" s="84"/>
-      <c r="C35" s="30"/>
-      <c r="D35" s="35"/>
-      <c r="E35" s="36" t="s">
+      <c r="B35" s="86"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="37"/>
+      <c r="E35" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="F35" s="37">
+      <c r="F35" s="39">
         <v>3.1549999999999998</v>
       </c>
-      <c r="G35" s="37">
+      <c r="G35" s="39">
         <v>3.8809999999999998</v>
       </c>
-      <c r="H35" s="37">
+      <c r="H35" s="39">
         <v>3.484</v>
       </c>
-      <c r="I35" s="38">
+      <c r="I35" s="40">
         <v>1.35E-2</v>
       </c>
-      <c r="J35" s="109" t="str">
+      <c r="J35" s="112" t="str">
         <f t="shared" si="0"/>
         <v>&lt;0.05</v>
       </c>
-      <c r="K35" s="84"/>
+      <c r="K35" s="86"/>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B36" s="84"/>
-      <c r="C36" s="30"/>
-      <c r="D36" s="39" t="s">
+      <c r="B36" s="86"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="E36" s="40" t="s">
+      <c r="E36" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="F36" s="41">
+      <c r="F36" s="43">
         <v>3.2080000000000002</v>
       </c>
-      <c r="G36" s="41">
+      <c r="G36" s="43">
         <v>3.9460000000000002</v>
       </c>
-      <c r="H36" s="41">
+      <c r="H36" s="43">
         <v>2.09</v>
       </c>
-      <c r="I36" s="42">
+      <c r="I36" s="44">
         <v>9.4799999999999995E-2</v>
       </c>
-      <c r="J36" s="73" t="str">
+      <c r="J36" s="75" t="str">
         <f t="shared" si="0"/>
         <v>&lt;0.1</v>
       </c>
-      <c r="K36" s="84"/>
+      <c r="K36" s="86"/>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B37" s="84"/>
-      <c r="C37" s="30"/>
-      <c r="D37" s="35"/>
-      <c r="E37" s="43" t="s">
+      <c r="B37" s="86"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="37"/>
+      <c r="E37" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="F37" s="37">
+      <c r="F37" s="39">
         <v>2.7349999999999999</v>
       </c>
-      <c r="G37" s="37">
+      <c r="G37" s="39">
         <v>3.363</v>
       </c>
-      <c r="H37" s="37">
+      <c r="H37" s="39">
         <v>2.6469999999999998</v>
       </c>
-      <c r="I37" s="38">
+      <c r="I37" s="40">
         <v>5.57E-2</v>
       </c>
-      <c r="J37" s="109" t="str">
+      <c r="J37" s="112" t="str">
         <f t="shared" si="0"/>
         <v>&lt;0.1</v>
       </c>
-      <c r="K37" s="84"/>
+      <c r="K37" s="86"/>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B38" s="84"/>
-      <c r="C38" s="30"/>
-      <c r="D38" s="44" t="s">
+      <c r="B38" s="86"/>
+      <c r="C38" s="32"/>
+      <c r="D38" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E38" s="45" t="s">
+      <c r="E38" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="F38" s="46">
+      <c r="F38" s="48">
         <v>1.8720000000000001</v>
       </c>
-      <c r="G38" s="46">
+      <c r="G38" s="48">
         <v>2.323</v>
       </c>
-      <c r="H38" s="46">
+      <c r="H38" s="48">
         <v>2.855</v>
       </c>
-      <c r="I38" s="47">
+      <c r="I38" s="49">
         <v>5.1299999999999998E-2</v>
       </c>
-      <c r="J38" s="107" t="str">
+      <c r="J38" s="110" t="str">
         <f t="shared" si="0"/>
         <v>&lt;0.1</v>
       </c>
-      <c r="K38" s="84"/>
+      <c r="K38" s="86"/>
     </row>
     <row r="39" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="84"/>
+      <c r="B39" s="86"/>
       <c r="C39" s="7"/>
       <c r="D39" s="5" t="s">
         <v>24</v>
@@ -2011,91 +2043,91 @@
       <c r="G39" s="5">
         <v>8.7089999999999996</v>
       </c>
-      <c r="H39" s="12">
+      <c r="H39" s="14">
         <v>2.903</v>
       </c>
-      <c r="I39" s="23">
+      <c r="I39" s="25">
         <v>4.1599999999999996E-3</v>
       </c>
-      <c r="J39" s="83" t="str">
+      <c r="J39" s="85" t="str">
         <f t="shared" si="0"/>
         <v>&lt;0.05</v>
       </c>
-      <c r="K39" s="84"/>
+      <c r="K39" s="86"/>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B40" s="84"/>
-      <c r="C40" s="17" t="s">
+      <c r="B40" s="86"/>
+      <c r="C40" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="D40" s="44" t="s">
+      <c r="D40" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="E40" s="45" t="s">
+      <c r="E40" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="F40" s="46">
+      <c r="F40" s="48">
         <v>1.907</v>
       </c>
-      <c r="G40" s="46">
-        <v>1</v>
-      </c>
-      <c r="H40" s="46">
+      <c r="G40" s="48">
+        <v>1</v>
+      </c>
+      <c r="H40" s="48">
         <v>4.5350000000000001</v>
       </c>
-      <c r="I40" s="47">
+      <c r="I40" s="49">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="J40" s="107" t="str">
+      <c r="J40" s="110" t="str">
         <f t="shared" si="0"/>
         <v>&lt;0.05</v>
       </c>
-      <c r="K40" s="84"/>
+      <c r="K40" s="86"/>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B41" s="84"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="44" t="s">
+      <c r="B41" s="86"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="E41" s="45" t="s">
+      <c r="E41" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="F41" s="46">
+      <c r="F41" s="48">
         <v>2.0150000000000001</v>
       </c>
-      <c r="G41" s="46">
+      <c r="G41" s="48">
         <v>2.4649999999999999</v>
       </c>
-      <c r="H41" s="46">
+      <c r="H41" s="48">
         <v>9.3629999999999995</v>
       </c>
-      <c r="I41" s="47">
+      <c r="I41" s="49">
         <v>7.2399999999999998E-5</v>
       </c>
-      <c r="J41" s="107" t="str">
+      <c r="J41" s="110" t="str">
         <f t="shared" si="0"/>
         <v>&lt;0.05</v>
       </c>
-      <c r="K41" s="84"/>
+      <c r="K41" s="86"/>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B42" s="84"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="44" t="s">
+      <c r="B42" s="86"/>
+      <c r="C42" s="32"/>
+      <c r="D42" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E42" s="53"/>
-      <c r="F42" s="54"/>
-      <c r="G42" s="54"/>
-      <c r="H42" s="54"/>
-      <c r="I42" s="55"/>
-      <c r="J42" s="110"/>
-      <c r="K42" s="84"/>
+      <c r="E42" s="55"/>
+      <c r="F42" s="56"/>
+      <c r="G42" s="56"/>
+      <c r="H42" s="56"/>
+      <c r="I42" s="57"/>
+      <c r="J42" s="113"/>
+      <c r="K42" s="86"/>
     </row>
     <row r="43" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="84"/>
-      <c r="C43" s="24"/>
+      <c r="B43" s="86"/>
+      <c r="C43" s="7"/>
       <c r="D43" s="5" t="s">
         <v>24</v>
       </c>
@@ -2111,69 +2143,69 @@
       <c r="H43" s="5">
         <v>2.371</v>
       </c>
-      <c r="I43" s="9">
+      <c r="I43" s="10">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="J43" s="111" t="str">
+      <c r="J43" s="115" t="str">
         <f t="shared" si="0"/>
         <v>&lt;0.1</v>
       </c>
-      <c r="K43" s="84"/>
+      <c r="K43" s="86"/>
     </row>
     <row r="44" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="84"/>
-      <c r="C44" s="50"/>
-      <c r="D44" s="84"/>
-      <c r="E44" s="84"/>
-      <c r="F44" s="84"/>
-      <c r="G44" s="84"/>
-      <c r="H44" s="84"/>
-      <c r="I44" s="84"/>
-      <c r="J44" s="84"/>
-      <c r="K44" s="84"/>
+      <c r="B44" s="86"/>
+      <c r="C44" s="52"/>
+      <c r="D44" s="86"/>
+      <c r="E44" s="86"/>
+      <c r="F44" s="86"/>
+      <c r="G44" s="86"/>
+      <c r="H44" s="86"/>
+      <c r="I44" s="86"/>
+      <c r="J44" s="86"/>
+      <c r="K44" s="86"/>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B45" s="84"/>
-      <c r="C45" s="84"/>
-      <c r="D45" s="84"/>
-      <c r="E45" s="84"/>
-      <c r="F45" s="84"/>
-      <c r="G45" s="84"/>
-      <c r="H45" s="84"/>
-      <c r="I45" s="84"/>
-      <c r="J45" s="84"/>
-      <c r="K45" s="84"/>
+      <c r="B45" s="86"/>
+      <c r="C45" s="86"/>
+      <c r="D45" s="86"/>
+      <c r="E45" s="86"/>
+      <c r="F45" s="86"/>
+      <c r="G45" s="86"/>
+      <c r="H45" s="86"/>
+      <c r="I45" s="86"/>
+      <c r="J45" s="86"/>
+      <c r="K45" s="86"/>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="K46" s="84"/>
-    </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="C47" s="84"/>
-      <c r="D47" s="84"/>
-      <c r="E47" s="84"/>
-      <c r="F47" s="84"/>
-      <c r="G47" s="84"/>
-      <c r="H47" s="84"/>
-      <c r="I47" s="84"/>
-      <c r="J47" s="84"/>
-      <c r="K47" s="84"/>
+      <c r="K46" s="86"/>
+    </row>
+    <row r="47" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C47" s="86"/>
+      <c r="D47" s="109" t="s">
+        <v>37</v>
+      </c>
+      <c r="E47" s="109"/>
+      <c r="F47" s="109"/>
+      <c r="G47" s="109"/>
+      <c r="H47" s="109"/>
+      <c r="I47" s="109"/>
+      <c r="J47" s="109"/>
+      <c r="K47" s="86"/>
     </row>
     <row r="48" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="84"/>
-      <c r="C48" s="106" t="s">
-        <v>38</v>
-      </c>
-      <c r="D48" s="106"/>
-      <c r="E48" s="106"/>
-      <c r="F48" s="106"/>
-      <c r="G48" s="106"/>
-      <c r="H48" s="106"/>
-      <c r="I48" s="106"/>
-      <c r="J48" s="105"/>
-      <c r="K48" s="84"/>
+      <c r="B48" s="86"/>
+      <c r="C48" s="86"/>
+      <c r="D48" s="86"/>
+      <c r="E48" s="86"/>
+      <c r="F48" s="86"/>
+      <c r="G48" s="86"/>
+      <c r="H48" s="86"/>
+      <c r="I48" s="86"/>
+      <c r="J48" s="107"/>
+      <c r="K48" s="86"/>
     </row>
     <row r="49" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="84"/>
+      <c r="B49" s="86"/>
       <c r="C49" s="2" t="s">
         <v>10</v>
       </c>
@@ -2196,417 +2228,417 @@
         <v>9</v>
       </c>
       <c r="J49" s="2"/>
-      <c r="K49" s="84"/>
+      <c r="K49" s="86"/>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B50" s="84"/>
-      <c r="C50" s="49" t="s">
+      <c r="B50" s="86"/>
+      <c r="C50" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="D50" s="44" t="s">
+      <c r="D50" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="E50" s="45" t="s">
+      <c r="E50" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="F50" s="46">
-        <v>1</v>
-      </c>
-      <c r="G50" s="46">
-        <v>1</v>
-      </c>
-      <c r="H50" s="46">
+      <c r="F50" s="48">
+        <v>1</v>
+      </c>
+      <c r="G50" s="48">
+        <v>1</v>
+      </c>
+      <c r="H50" s="48">
         <v>3.5569999999999999</v>
       </c>
-      <c r="I50" s="47">
+      <c r="I50" s="49">
         <v>6.1100000000000002E-2</v>
       </c>
-      <c r="J50" s="107" t="str">
+      <c r="J50" s="110" t="str">
         <f>IF(I50&lt;0.05, "&lt;0.05", IF(I50&lt;0.1, "&lt;0.1", ""))</f>
         <v>&lt;0.1</v>
       </c>
-      <c r="K50" s="84"/>
+      <c r="K50" s="86"/>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B51" s="84"/>
-      <c r="C51" s="31"/>
-      <c r="D51" s="44" t="s">
+      <c r="B51" s="86"/>
+      <c r="C51" s="33"/>
+      <c r="D51" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="E51" s="45" t="s">
+      <c r="E51" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="F51" s="46">
-        <v>1</v>
-      </c>
-      <c r="G51" s="46">
-        <v>1</v>
-      </c>
-      <c r="H51" s="46">
+      <c r="F51" s="48">
+        <v>1</v>
+      </c>
+      <c r="G51" s="48">
+        <v>1</v>
+      </c>
+      <c r="H51" s="48">
         <v>3.1829999999999998</v>
       </c>
-      <c r="I51" s="47">
+      <c r="I51" s="49">
         <v>7.6300000000000007E-2</v>
       </c>
-      <c r="J51" s="107" t="str">
+      <c r="J51" s="110" t="str">
         <f t="shared" ref="J51:J64" si="1">IF(I51&lt;0.05, "&lt;0.05", IF(I51&lt;0.1, "&lt;0.1", ""))</f>
         <v>&lt;0.1</v>
       </c>
-      <c r="K51" s="84"/>
+      <c r="K51" s="86"/>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B52" s="84"/>
-      <c r="C52" s="31"/>
-      <c r="D52" s="44" t="s">
+      <c r="B52" s="86"/>
+      <c r="C52" s="33"/>
+      <c r="D52" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E52" s="45" t="s">
+      <c r="E52" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="F52" s="46">
-        <v>1</v>
-      </c>
-      <c r="G52" s="46">
-        <v>1</v>
-      </c>
-      <c r="H52" s="46">
+      <c r="F52" s="48">
+        <v>1</v>
+      </c>
+      <c r="G52" s="48">
+        <v>1</v>
+      </c>
+      <c r="H52" s="48">
         <v>6.492</v>
       </c>
-      <c r="I52" s="47">
+      <c r="I52" s="49">
         <v>1.18E-2</v>
       </c>
-      <c r="J52" s="107" t="str">
+      <c r="J52" s="110" t="str">
         <f t="shared" si="1"/>
         <v>&lt;0.05</v>
       </c>
-      <c r="K52" s="84"/>
+      <c r="K52" s="86"/>
     </row>
     <row r="53" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="84"/>
-      <c r="C53" s="31"/>
-      <c r="D53" s="21" t="s">
+      <c r="B53" s="86"/>
+      <c r="C53" s="33"/>
+      <c r="D53" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="E53" s="59" t="s">
+      <c r="E53" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="F53" s="60"/>
-      <c r="G53" s="60"/>
-      <c r="H53" s="60"/>
-      <c r="I53" s="61"/>
-      <c r="J53" s="112"/>
-      <c r="K53" s="84"/>
+      <c r="F53" s="62"/>
+      <c r="G53" s="62"/>
+      <c r="H53" s="62"/>
+      <c r="I53" s="63"/>
+      <c r="J53" s="116"/>
+      <c r="K53" s="86"/>
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B54" s="84"/>
-      <c r="C54" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="D54" s="49" t="s">
+      <c r="B54" s="86"/>
+      <c r="C54" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="D54" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="E54" s="32" t="s">
+      <c r="E54" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="F54" s="33">
-        <v>1</v>
-      </c>
-      <c r="G54" s="33">
-        <v>1</v>
-      </c>
-      <c r="H54" s="33">
+      <c r="F54" s="35">
+        <v>1</v>
+      </c>
+      <c r="G54" s="35">
+        <v>1</v>
+      </c>
+      <c r="H54" s="35">
         <v>4.4020000000000001</v>
       </c>
-      <c r="I54" s="34">
+      <c r="I54" s="36">
         <v>3.7449999999999997E-2</v>
       </c>
-      <c r="J54" s="80" t="str">
+      <c r="J54" s="82" t="str">
         <f t="shared" si="1"/>
         <v>&lt;0.05</v>
       </c>
-      <c r="K54" s="84"/>
+      <c r="K54" s="86"/>
     </row>
     <row r="55" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="84"/>
-      <c r="C55" s="30"/>
-      <c r="D55" s="57"/>
-      <c r="E55" s="36" t="s">
+      <c r="B55" s="86"/>
+      <c r="C55" s="32"/>
+      <c r="D55" s="59"/>
+      <c r="E55" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="F55" s="37">
+      <c r="F55" s="39">
         <v>2.6040000000000001</v>
       </c>
-      <c r="G55" s="37">
+      <c r="G55" s="39">
         <v>2.6040000000000001</v>
       </c>
-      <c r="H55" s="37">
+      <c r="H55" s="39">
         <v>5.57</v>
       </c>
-      <c r="I55" s="38">
+      <c r="I55" s="40">
         <v>9.8700000000000003E-3</v>
       </c>
-      <c r="J55" s="109" t="str">
+      <c r="J55" s="112" t="str">
         <f t="shared" si="1"/>
         <v>&lt;0.05</v>
       </c>
-      <c r="K55" s="84"/>
+      <c r="K55" s="86"/>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B56" s="84"/>
-      <c r="C56" s="30"/>
-      <c r="D56" s="58" t="s">
+      <c r="B56" s="86"/>
+      <c r="C56" s="32"/>
+      <c r="D56" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="E56" s="40" t="s">
+      <c r="E56" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="F56" s="41">
-        <v>1</v>
-      </c>
-      <c r="G56" s="41">
-        <v>1</v>
-      </c>
-      <c r="H56" s="41">
+      <c r="F56" s="43">
+        <v>1</v>
+      </c>
+      <c r="G56" s="43">
+        <v>1</v>
+      </c>
+      <c r="H56" s="43">
         <v>4.1509999999999998</v>
       </c>
-      <c r="I56" s="34">
+      <c r="I56" s="36">
         <v>4.3200000000000002E-2</v>
       </c>
-      <c r="J56" s="80" t="str">
+      <c r="J56" s="82" t="str">
         <f t="shared" si="1"/>
         <v>&lt;0.05</v>
       </c>
-      <c r="K56" s="84"/>
+      <c r="K56" s="86"/>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B57" s="84"/>
-      <c r="C57" s="30"/>
-      <c r="D57" s="57"/>
-      <c r="E57" s="43" t="s">
+      <c r="B57" s="86"/>
+      <c r="C57" s="32"/>
+      <c r="D57" s="59"/>
+      <c r="E57" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="F57" s="37">
+      <c r="F57" s="39">
         <v>2.036</v>
       </c>
-      <c r="G57" s="37">
+      <c r="G57" s="39">
         <v>2.036</v>
       </c>
-      <c r="H57" s="37">
+      <c r="H57" s="39">
         <v>3.661</v>
       </c>
-      <c r="I57" s="38">
+      <c r="I57" s="40">
         <v>3.4200000000000001E-2</v>
       </c>
-      <c r="J57" s="109" t="str">
+      <c r="J57" s="112" t="str">
         <f t="shared" si="1"/>
         <v>&lt;0.05</v>
       </c>
-      <c r="K57" s="84"/>
+      <c r="K57" s="86"/>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B58" s="84"/>
-      <c r="C58" s="30"/>
-      <c r="D58" s="44" t="s">
+      <c r="B58" s="86"/>
+      <c r="C58" s="32"/>
+      <c r="D58" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E58" s="45" t="s">
+      <c r="E58" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="F58" s="46">
+      <c r="F58" s="48">
         <v>0.99990000000000001</v>
       </c>
-      <c r="G58" s="46">
+      <c r="G58" s="48">
         <v>0.99990000000000001</v>
       </c>
-      <c r="H58" s="46">
+      <c r="H58" s="48">
         <v>4.51</v>
       </c>
-      <c r="I58" s="47">
+      <c r="I58" s="49">
         <v>3.5299999999999998E-2</v>
       </c>
-      <c r="J58" s="107" t="str">
+      <c r="J58" s="110" t="str">
         <f t="shared" si="1"/>
         <v>&lt;0.05</v>
       </c>
-      <c r="K58" s="84"/>
+      <c r="K58" s="86"/>
     </row>
     <row r="59" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="84"/>
+      <c r="B59" s="86"/>
       <c r="C59" s="7"/>
       <c r="D59" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E59" s="59" t="s">
+      <c r="E59" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="F59" s="60"/>
-      <c r="G59" s="60"/>
-      <c r="H59" s="60"/>
-      <c r="I59" s="61"/>
-      <c r="J59" s="112"/>
-      <c r="K59" s="84"/>
+      <c r="F59" s="62"/>
+      <c r="G59" s="62"/>
+      <c r="H59" s="62"/>
+      <c r="I59" s="63"/>
+      <c r="J59" s="116"/>
+      <c r="K59" s="86"/>
     </row>
     <row r="60" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B60" s="84"/>
-      <c r="C60" s="17" t="s">
+      <c r="B60" s="86"/>
+      <c r="C60" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D60" s="44" t="s">
+      <c r="D60" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="E60" s="45" t="s">
+      <c r="E60" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="F60" s="46">
-        <v>1</v>
-      </c>
-      <c r="G60" s="46">
-        <v>1</v>
-      </c>
-      <c r="H60" s="46">
+      <c r="F60" s="48">
+        <v>1</v>
+      </c>
+      <c r="G60" s="48">
+        <v>1</v>
+      </c>
+      <c r="H60" s="48">
         <v>6.9820000000000002</v>
       </c>
-      <c r="I60" s="47">
+      <c r="I60" s="49">
         <v>9.0399999999999994E-3</v>
       </c>
-      <c r="J60" s="107" t="str">
+      <c r="J60" s="110" t="str">
         <f t="shared" si="1"/>
         <v>&lt;0.05</v>
       </c>
-      <c r="K60" s="84"/>
+      <c r="K60" s="86"/>
     </row>
     <row r="61" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B61" s="84"/>
-      <c r="C61" s="19"/>
-      <c r="D61" s="58" t="s">
+      <c r="B61" s="86"/>
+      <c r="C61" s="21"/>
+      <c r="D61" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="E61" s="40" t="s">
+      <c r="E61" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="F61" s="41">
+      <c r="F61" s="43">
         <v>1.8480000000000001</v>
       </c>
-      <c r="G61" s="41">
+      <c r="G61" s="43">
         <v>1.8480000000000001</v>
       </c>
-      <c r="H61" s="41">
+      <c r="H61" s="43">
         <v>13.904999999999999</v>
       </c>
-      <c r="I61" s="42">
+      <c r="I61" s="44">
         <v>1.9599999999999999E-4</v>
       </c>
-      <c r="J61" s="73" t="str">
+      <c r="J61" s="75" t="str">
         <f t="shared" si="1"/>
         <v>&lt;0.05</v>
       </c>
-      <c r="K61" s="84"/>
+      <c r="K61" s="86"/>
     </row>
     <row r="62" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B62" s="84"/>
-      <c r="C62" s="19"/>
-      <c r="D62" s="57"/>
-      <c r="E62" s="43" t="s">
+      <c r="B62" s="86"/>
+      <c r="C62" s="21"/>
+      <c r="D62" s="59"/>
+      <c r="E62" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="F62" s="37">
-        <v>1</v>
-      </c>
-      <c r="G62" s="37">
-        <v>1</v>
-      </c>
-      <c r="H62" s="37">
+      <c r="F62" s="39">
+        <v>1</v>
+      </c>
+      <c r="G62" s="39">
+        <v>1</v>
+      </c>
+      <c r="H62" s="39">
         <v>3.633</v>
       </c>
-      <c r="I62" s="38">
+      <c r="I62" s="40">
         <v>5.842E-2</v>
       </c>
-      <c r="J62" s="109" t="str">
+      <c r="J62" s="112" t="str">
         <f t="shared" si="1"/>
         <v>&lt;0.1</v>
       </c>
-      <c r="K62" s="84"/>
+      <c r="K62" s="86"/>
     </row>
     <row r="63" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B63" s="84"/>
-      <c r="C63" s="19"/>
-      <c r="D63" s="21" t="s">
+      <c r="B63" s="86"/>
+      <c r="C63" s="21"/>
+      <c r="D63" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="E63" s="53"/>
-      <c r="F63" s="54"/>
-      <c r="G63" s="54"/>
-      <c r="H63" s="54"/>
-      <c r="I63" s="55"/>
-      <c r="J63" s="55"/>
-      <c r="K63" s="84"/>
+      <c r="E63" s="55"/>
+      <c r="F63" s="56"/>
+      <c r="G63" s="56"/>
+      <c r="H63" s="56"/>
+      <c r="I63" s="57"/>
+      <c r="J63" s="57"/>
+      <c r="K63" s="86"/>
     </row>
     <row r="64" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="84"/>
-      <c r="C64" s="24"/>
+      <c r="B64" s="86"/>
+      <c r="C64" s="26"/>
       <c r="D64" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E64" s="113" t="s">
+      <c r="E64" s="117" t="s">
         <v>27</v>
       </c>
-      <c r="F64" s="114"/>
-      <c r="G64" s="114"/>
-      <c r="H64" s="114"/>
-      <c r="I64" s="115"/>
-      <c r="J64" s="115"/>
-      <c r="K64" s="84"/>
+      <c r="F64" s="118"/>
+      <c r="G64" s="118"/>
+      <c r="H64" s="118"/>
+      <c r="I64" s="119"/>
+      <c r="J64" s="119"/>
+      <c r="K64" s="86"/>
     </row>
     <row r="65" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B65" s="84"/>
-      <c r="C65" s="84"/>
-      <c r="D65" s="84"/>
-      <c r="E65" s="84"/>
-      <c r="F65" s="84"/>
-      <c r="G65" s="84"/>
-      <c r="H65" s="84"/>
-      <c r="I65" s="84"/>
-      <c r="J65" s="84"/>
-      <c r="K65" s="84"/>
-      <c r="L65" s="84"/>
+      <c r="B65" s="86"/>
+      <c r="C65" s="86"/>
+      <c r="D65" s="86"/>
+      <c r="E65" s="86"/>
+      <c r="F65" s="86"/>
+      <c r="G65" s="86"/>
+      <c r="H65" s="86"/>
+      <c r="I65" s="86"/>
+      <c r="J65" s="86"/>
+      <c r="K65" s="86"/>
+      <c r="L65" s="86"/>
     </row>
     <row r="66" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B66" s="84"/>
-      <c r="C66" s="84"/>
-      <c r="D66" s="84"/>
-      <c r="E66" s="84"/>
-      <c r="F66" s="84"/>
-      <c r="G66" s="84"/>
-      <c r="H66" s="84"/>
-      <c r="I66" s="84"/>
-      <c r="J66" s="84"/>
-      <c r="K66" s="84"/>
-      <c r="L66" s="84"/>
+      <c r="B66" s="86"/>
+      <c r="C66" s="86"/>
+      <c r="D66" s="86"/>
+      <c r="E66" s="86"/>
+      <c r="F66" s="86"/>
+      <c r="G66" s="86"/>
+      <c r="H66" s="86"/>
+      <c r="I66" s="86"/>
+      <c r="J66" s="86"/>
+      <c r="K66" s="86"/>
+      <c r="L66" s="86"/>
     </row>
     <row r="68" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B68" s="84"/>
-      <c r="C68" s="84" t="s">
+      <c r="B68" s="86"/>
+      <c r="C68" s="86" t="s">
         <v>31</v>
       </c>
-      <c r="D68" s="84"/>
-      <c r="E68" s="84"/>
-      <c r="F68" s="84"/>
-      <c r="G68" s="84"/>
-      <c r="H68" s="84"/>
-      <c r="I68" s="84"/>
+      <c r="D68" s="86"/>
+      <c r="E68" s="86"/>
+      <c r="F68" s="86"/>
+      <c r="G68" s="86"/>
+      <c r="H68" s="86"/>
+      <c r="I68" s="86"/>
     </row>
     <row r="69" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="84"/>
-      <c r="C69" s="84"/>
-      <c r="D69" s="84"/>
-      <c r="E69" s="84"/>
-      <c r="F69" s="84"/>
-      <c r="G69" s="84"/>
-      <c r="H69" s="84"/>
-      <c r="I69" s="84"/>
+      <c r="B69" s="86"/>
+      <c r="C69" s="86"/>
+      <c r="D69" s="86"/>
+      <c r="E69" s="86"/>
+      <c r="F69" s="86"/>
+      <c r="G69" s="86"/>
+      <c r="H69" s="86"/>
+      <c r="I69" s="86"/>
     </row>
     <row r="70" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="84"/>
+      <c r="B70" s="86"/>
       <c r="C70" s="2" t="s">
         <v>10</v>
       </c>
@@ -2620,215 +2652,215 @@
         <v>9</v>
       </c>
       <c r="G70" s="2"/>
-      <c r="H70" s="84"/>
-      <c r="I70" s="84"/>
+      <c r="H70" s="86"/>
+      <c r="I70" s="86"/>
     </row>
     <row r="71" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B71" s="84"/>
-      <c r="C71" s="49" t="s">
+      <c r="B71" s="86"/>
+      <c r="C71" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="D71" s="65" t="s">
+      <c r="D71" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="E71" s="26" t="s">
+      <c r="E71" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="F71" s="66">
+      <c r="F71" s="68">
         <v>5.8599999999999999E-2</v>
       </c>
-      <c r="G71" s="27" t="s">
+      <c r="G71" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="H71" s="84"/>
-      <c r="I71" s="84"/>
+      <c r="H71" s="86"/>
+      <c r="I71" s="86"/>
     </row>
     <row r="72" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="84"/>
-      <c r="C72" s="31"/>
-      <c r="D72" s="25" t="s">
+      <c r="B72" s="86"/>
+      <c r="C72" s="33"/>
+      <c r="D72" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="E72" s="25" t="s">
+      <c r="E72" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="F72" s="67">
+      <c r="F72" s="69">
         <v>6.1100000000000002E-2</v>
       </c>
-      <c r="G72" s="12" t="s">
+      <c r="G72" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="H72" s="84"/>
-      <c r="I72" s="84"/>
+      <c r="H72" s="86"/>
+      <c r="I72" s="86"/>
     </row>
     <row r="73" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B73" s="84"/>
-      <c r="C73" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="D73" s="29" t="s">
+      <c r="B73" s="86"/>
+      <c r="C73" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="D73" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="E73" s="68" t="s">
+      <c r="E73" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="F73" s="69">
+      <c r="F73" s="71">
         <v>3.9699999999999999E-2</v>
       </c>
-      <c r="G73" s="27" t="s">
+      <c r="G73" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="H73" s="84"/>
-      <c r="I73" s="84"/>
+      <c r="H73" s="86"/>
+      <c r="I73" s="86"/>
     </row>
     <row r="74" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B74" s="84"/>
-      <c r="C74" s="30"/>
-      <c r="D74" s="35"/>
-      <c r="E74" s="72" t="s">
+      <c r="B74" s="86"/>
+      <c r="C74" s="32"/>
+      <c r="D74" s="37"/>
+      <c r="E74" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="F74" s="70">
+      <c r="F74" s="72">
         <v>1.35E-2</v>
       </c>
-      <c r="G74" s="27" t="s">
+      <c r="G74" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="H74" s="84"/>
-      <c r="I74" s="84"/>
+      <c r="H74" s="86"/>
+      <c r="I74" s="86"/>
     </row>
     <row r="75" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B75" s="84"/>
-      <c r="C75" s="30"/>
-      <c r="D75" s="39" t="s">
+      <c r="B75" s="86"/>
+      <c r="C75" s="32"/>
+      <c r="D75" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="E75" s="73" t="s">
+      <c r="E75" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="F75" s="74">
+      <c r="F75" s="76">
         <v>3.7449999999999997E-2</v>
       </c>
-      <c r="G75" s="27" t="s">
+      <c r="G75" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="H75" s="84"/>
-      <c r="I75" s="84"/>
+      <c r="H75" s="86"/>
+      <c r="I75" s="86"/>
     </row>
     <row r="76" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="84"/>
-      <c r="C76" s="30"/>
+      <c r="B76" s="86"/>
+      <c r="C76" s="32"/>
       <c r="D76" s="7"/>
-      <c r="E76" s="75" t="s">
+      <c r="E76" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="F76" s="76">
+      <c r="F76" s="78">
         <v>9.8700000000000003E-3</v>
       </c>
-      <c r="G76" s="12" t="s">
+      <c r="G76" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="H76" s="84"/>
-      <c r="I76" s="84"/>
+      <c r="H76" s="86"/>
+      <c r="I76" s="86"/>
     </row>
     <row r="77" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B77" s="84"/>
-      <c r="C77" s="79" t="s">
+      <c r="B77" s="86"/>
+      <c r="C77" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="D77" s="80" t="s">
+      <c r="D77" s="82" t="s">
         <v>21</v>
       </c>
-      <c r="E77" s="26" t="s">
+      <c r="E77" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="F77" s="71">
+      <c r="F77" s="73">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="G77" s="27" t="s">
+      <c r="G77" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="H77" s="84"/>
-      <c r="I77" s="84"/>
+      <c r="H77" s="86"/>
+      <c r="I77" s="86"/>
     </row>
     <row r="78" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="84"/>
-      <c r="C78" s="82"/>
-      <c r="D78" s="83" t="s">
+      <c r="B78" s="86"/>
+      <c r="C78" s="84"/>
+      <c r="D78" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="E78" s="25" t="s">
+      <c r="E78" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="F78" s="76">
+      <c r="F78" s="78">
         <v>9.0399999999999994E-3</v>
       </c>
-      <c r="G78" s="12" t="s">
+      <c r="G78" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="H78" s="84"/>
-      <c r="I78" s="84"/>
+      <c r="H78" s="86"/>
+      <c r="I78" s="86"/>
     </row>
     <row r="79" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="84"/>
-      <c r="C79" s="77"/>
-      <c r="D79" s="85"/>
-      <c r="E79" s="85"/>
-      <c r="F79" s="85"/>
-      <c r="G79" s="85"/>
-      <c r="H79" s="85"/>
-      <c r="I79" s="85"/>
-      <c r="J79" s="85"/>
-      <c r="K79" s="84"/>
+      <c r="B79" s="86"/>
+      <c r="C79" s="79"/>
+      <c r="D79" s="87"/>
+      <c r="E79" s="87"/>
+      <c r="F79" s="87"/>
+      <c r="G79" s="87"/>
+      <c r="H79" s="87"/>
+      <c r="I79" s="87"/>
+      <c r="J79" s="87"/>
+      <c r="K79" s="86"/>
     </row>
     <row r="80" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B80" s="84"/>
-      <c r="C80" s="77"/>
-      <c r="D80" s="28"/>
-      <c r="E80" s="28"/>
-      <c r="F80" s="28"/>
-      <c r="G80" s="28"/>
-      <c r="H80" s="84"/>
-      <c r="I80" s="84"/>
-      <c r="J80" s="84"/>
-      <c r="K80" s="84"/>
+      <c r="B80" s="86"/>
+      <c r="C80" s="79"/>
+      <c r="D80" s="30"/>
+      <c r="E80" s="30"/>
+      <c r="F80" s="30"/>
+      <c r="G80" s="30"/>
+      <c r="H80" s="86"/>
+      <c r="I80" s="86"/>
+      <c r="J80" s="86"/>
+      <c r="K80" s="86"/>
     </row>
     <row r="81" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="84"/>
-      <c r="C81" s="78"/>
-      <c r="D81" s="28"/>
-      <c r="E81" s="28"/>
-      <c r="F81" s="28"/>
-      <c r="G81" s="28"/>
-      <c r="H81" s="84"/>
-      <c r="I81" s="84"/>
-      <c r="J81" s="84"/>
-      <c r="K81" s="84"/>
+      <c r="B81" s="86"/>
+      <c r="C81" s="80"/>
+      <c r="D81" s="30"/>
+      <c r="E81" s="30"/>
+      <c r="F81" s="30"/>
+      <c r="G81" s="30"/>
+      <c r="H81" s="86"/>
+      <c r="I81" s="86"/>
+      <c r="J81" s="86"/>
+      <c r="K81" s="86"/>
     </row>
     <row r="85" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B85" s="84"/>
-      <c r="C85" s="84" t="s">
+      <c r="B85" s="86"/>
+      <c r="C85" s="86" t="s">
         <v>32</v>
       </c>
-      <c r="D85" s="84"/>
-      <c r="E85" s="84"/>
-      <c r="F85" s="84"/>
-      <c r="G85" s="84"/>
-      <c r="H85" s="84"/>
-      <c r="I85" s="84"/>
+      <c r="D85" s="86"/>
+      <c r="E85" s="86"/>
+      <c r="F85" s="86"/>
+      <c r="G85" s="86"/>
+      <c r="H85" s="86"/>
+      <c r="I85" s="86"/>
     </row>
     <row r="86" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="84"/>
-      <c r="C86" s="84"/>
-      <c r="D86" s="84"/>
-      <c r="E86" s="84"/>
-      <c r="F86" s="84"/>
-      <c r="G86" s="84"/>
-      <c r="H86" s="84"/>
-      <c r="I86" s="84"/>
+      <c r="B86" s="86"/>
+      <c r="C86" s="86"/>
+      <c r="D86" s="86"/>
+      <c r="E86" s="86"/>
+      <c r="F86" s="86"/>
+      <c r="G86" s="86"/>
+      <c r="H86" s="86"/>
+      <c r="I86" s="86"/>
     </row>
     <row r="87" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="84"/>
+      <c r="B87" s="86"/>
       <c r="C87" s="2" t="s">
         <v>10</v>
       </c>
@@ -2842,196 +2874,196 @@
         <v>9</v>
       </c>
       <c r="G87" s="2"/>
-      <c r="H87" s="84"/>
-      <c r="I87" s="84"/>
+      <c r="H87" s="86"/>
+      <c r="I87" s="86"/>
     </row>
     <row r="88" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B88" s="84"/>
-      <c r="C88" s="49" t="s">
+      <c r="B88" s="86"/>
+      <c r="C88" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="D88" s="65" t="s">
+      <c r="D88" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="E88" s="45" t="s">
+      <c r="E88" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="F88" s="66">
+      <c r="F88" s="68">
         <v>7.7100000000000002E-2</v>
       </c>
-      <c r="G88" s="27" t="s">
+      <c r="G88" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="H88" s="84"/>
-      <c r="I88" s="84"/>
+      <c r="H88" s="86"/>
+      <c r="I88" s="86"/>
     </row>
     <row r="89" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="84"/>
-      <c r="C89" s="31"/>
-      <c r="D89" s="25" t="s">
+      <c r="B89" s="86"/>
+      <c r="C89" s="33"/>
+      <c r="D89" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="E89" s="45" t="s">
+      <c r="E89" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="F89" s="67">
+      <c r="F89" s="69">
         <v>7.6300000000000007E-2</v>
       </c>
-      <c r="G89" s="12" t="s">
+      <c r="G89" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="H89" s="84"/>
-      <c r="I89" s="84"/>
+      <c r="H89" s="86"/>
+      <c r="I89" s="86"/>
     </row>
     <row r="90" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B90" s="84"/>
-      <c r="C90" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="D90" s="29" t="s">
+      <c r="B90" s="86"/>
+      <c r="C90" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="D90" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="E90" s="40" t="s">
+      <c r="E90" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="F90" s="87">
+      <c r="F90" s="89">
         <v>0.94799999999999995</v>
       </c>
-      <c r="G90" s="27" t="s">
+      <c r="G90" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="H90" s="84"/>
-      <c r="I90" s="84"/>
+      <c r="H90" s="86"/>
+      <c r="I90" s="86"/>
     </row>
     <row r="91" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B91" s="84"/>
-      <c r="C91" s="30"/>
-      <c r="D91" s="35"/>
-      <c r="E91" s="43" t="s">
+      <c r="B91" s="86"/>
+      <c r="C91" s="32"/>
+      <c r="D91" s="37"/>
+      <c r="E91" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="F91" s="64">
+      <c r="F91" s="66">
         <v>5.57E-2</v>
       </c>
-      <c r="G91" s="27" t="s">
+      <c r="G91" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="H91" s="84"/>
-      <c r="I91" s="84"/>
+      <c r="H91" s="86"/>
+      <c r="I91" s="86"/>
     </row>
     <row r="92" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B92" s="84"/>
-      <c r="C92" s="30"/>
-      <c r="D92" s="39" t="s">
+      <c r="B92" s="86"/>
+      <c r="C92" s="32"/>
+      <c r="D92" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="E92" s="40" t="s">
+      <c r="E92" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="F92" s="74">
+      <c r="F92" s="76">
         <v>4.3200000000000002E-2</v>
       </c>
-      <c r="G92" s="27" t="s">
+      <c r="G92" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="H92" s="84"/>
-      <c r="I92" s="84"/>
+      <c r="H92" s="86"/>
+      <c r="I92" s="86"/>
     </row>
     <row r="93" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B93" s="84"/>
+      <c r="B93" s="86"/>
       <c r="C93" s="7"/>
       <c r="D93" s="7"/>
-      <c r="E93" s="25" t="s">
+      <c r="E93" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="F93" s="76">
+      <c r="F93" s="78">
         <v>3.4200000000000001E-2</v>
       </c>
-      <c r="G93" s="12" t="s">
+      <c r="G93" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="H93" s="84"/>
-      <c r="I93" s="84"/>
+      <c r="H93" s="86"/>
+      <c r="I93" s="86"/>
     </row>
     <row r="94" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B94" s="84"/>
-      <c r="C94" s="29" t="s">
+      <c r="B94" s="86"/>
+      <c r="C94" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="D94" s="80" t="s">
+      <c r="D94" s="82" t="s">
         <v>21</v>
       </c>
-      <c r="E94" s="81" t="s">
+      <c r="E94" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="F94" s="88">
+      <c r="F94" s="90">
         <v>7.2399999999999998E-5</v>
       </c>
-      <c r="G94" s="33" t="s">
+      <c r="G94" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="H94" s="84"/>
-      <c r="I94" s="84"/>
+      <c r="H94" s="86"/>
+      <c r="I94" s="86"/>
     </row>
     <row r="95" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B95" s="84"/>
-      <c r="C95" s="30"/>
-      <c r="D95" s="68" t="s">
+      <c r="B95" s="86"/>
+      <c r="C95" s="32"/>
+      <c r="D95" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="E95" s="40" t="s">
+      <c r="E95" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="F95" s="74">
+      <c r="F95" s="76">
         <v>1.9599999999999999E-4</v>
       </c>
-      <c r="G95" s="27" t="s">
+      <c r="G95" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="H95" s="84"/>
-      <c r="I95" s="84"/>
+      <c r="H95" s="86"/>
+      <c r="I95" s="86"/>
     </row>
     <row r="96" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B96" s="84"/>
+      <c r="B96" s="86"/>
       <c r="C96" s="7"/>
-      <c r="D96" s="86"/>
-      <c r="E96" s="25" t="s">
+      <c r="D96" s="88"/>
+      <c r="E96" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F96" s="67">
+      <c r="F96" s="69">
         <v>5.842E-2</v>
       </c>
-      <c r="G96" s="89" t="s">
+      <c r="G96" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="H96" s="86"/>
-      <c r="I96" s="86"/>
-      <c r="J96" s="86"/>
+      <c r="H96" s="88"/>
+      <c r="I96" s="88"/>
+      <c r="J96" s="88"/>
     </row>
     <row r="99" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B99" s="84"/>
-      <c r="C99" s="84" t="s">
+      <c r="B99" s="86"/>
+      <c r="C99" s="86" t="s">
         <v>33</v>
       </c>
-      <c r="D99" s="84"/>
-      <c r="E99" s="84"/>
-      <c r="F99" s="84"/>
-      <c r="G99" s="84"/>
-      <c r="H99" s="84"/>
-      <c r="I99" s="84"/>
+      <c r="D99" s="86"/>
+      <c r="E99" s="86"/>
+      <c r="F99" s="86"/>
+      <c r="G99" s="86"/>
+      <c r="H99" s="86"/>
+      <c r="I99" s="86"/>
     </row>
     <row r="100" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B100" s="84"/>
-      <c r="C100" s="84"/>
-      <c r="D100" s="84"/>
-      <c r="E100" s="84"/>
-      <c r="F100" s="84"/>
-      <c r="G100" s="84"/>
-      <c r="H100" s="84"/>
-      <c r="I100" s="84"/>
+      <c r="B100" s="86"/>
+      <c r="C100" s="86"/>
+      <c r="D100" s="86"/>
+      <c r="E100" s="86"/>
+      <c r="F100" s="86"/>
+      <c r="G100" s="86"/>
+      <c r="H100" s="86"/>
+      <c r="I100" s="86"/>
     </row>
     <row r="101" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B101" s="84"/>
+      <c r="B101" s="86"/>
       <c r="C101" s="2" t="s">
         <v>10</v>
       </c>
@@ -3045,295 +3077,295 @@
         <v>9</v>
       </c>
       <c r="G101" s="2"/>
-      <c r="H101" s="84"/>
-      <c r="I101" s="84"/>
+      <c r="H101" s="86"/>
+      <c r="I101" s="86"/>
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B102" s="84"/>
-      <c r="C102" s="49" t="s">
+      <c r="B102" s="86"/>
+      <c r="C102" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="D102" s="65" t="s">
+      <c r="D102" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="E102" s="90" t="s">
+      <c r="E102" s="92" t="s">
         <v>17</v>
       </c>
-      <c r="F102" s="91">
+      <c r="F102" s="93">
         <v>3.0700000000000002E-2</v>
       </c>
-      <c r="G102" s="27" t="s">
+      <c r="G102" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="H102" s="84"/>
-      <c r="I102" s="84"/>
+      <c r="H102" s="86"/>
+      <c r="I102" s="86"/>
     </row>
     <row r="103" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B103" s="84"/>
-      <c r="C103" s="31"/>
-      <c r="D103" s="25" t="s">
+      <c r="B103" s="86"/>
+      <c r="C103" s="33"/>
+      <c r="D103" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="E103" s="25" t="s">
+      <c r="E103" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="F103" s="76">
+      <c r="F103" s="78">
         <v>1.18E-2</v>
       </c>
-      <c r="G103" s="12" t="s">
+      <c r="G103" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="H103" s="84"/>
-      <c r="I103" s="84"/>
+      <c r="H103" s="86"/>
+      <c r="I103" s="86"/>
     </row>
     <row r="104" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B104" s="84"/>
-      <c r="C104" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="D104" s="20" t="s">
+      <c r="B104" s="86"/>
+      <c r="C104" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="D104" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E104" s="45" t="s">
+      <c r="E104" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="F104" s="62">
+      <c r="F104" s="64">
         <v>5.1299999999999998E-2</v>
       </c>
-      <c r="G104" s="27" t="s">
+      <c r="G104" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="H104" s="84"/>
-      <c r="I104" s="84"/>
+      <c r="H104" s="86"/>
+      <c r="I104" s="86"/>
     </row>
     <row r="105" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B105" s="84"/>
-      <c r="C105" s="30"/>
-      <c r="D105" s="56" t="s">
+      <c r="B105" s="86"/>
+      <c r="C105" s="32"/>
+      <c r="D105" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="E105" s="45" t="s">
+      <c r="E105" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="F105" s="91">
+      <c r="F105" s="93">
         <v>3.5299999999999998E-2</v>
       </c>
-      <c r="G105" s="27" t="s">
+      <c r="G105" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="H105" s="84"/>
-      <c r="I105" s="84"/>
+      <c r="H105" s="86"/>
+      <c r="I105" s="86"/>
     </row>
     <row r="106" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B106" s="84"/>
-      <c r="C106" s="29" t="s">
+      <c r="B106" s="86"/>
+      <c r="C106" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="D106" s="80" t="s">
+      <c r="D106" s="82" t="s">
         <v>21</v>
       </c>
-      <c r="E106" s="80"/>
-      <c r="F106" s="92" t="s">
+      <c r="E106" s="82"/>
+      <c r="F106" s="94" t="s">
         <v>34</v>
       </c>
-      <c r="G106" s="34" t="s">
+      <c r="G106" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="H106" s="84"/>
-      <c r="I106" s="84"/>
+      <c r="H106" s="86"/>
+      <c r="I106" s="86"/>
     </row>
     <row r="107" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B107" s="84"/>
+      <c r="B107" s="86"/>
       <c r="C107" s="7"/>
-      <c r="D107" s="83" t="s">
+      <c r="D107" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="E107" s="83"/>
-      <c r="F107" s="93" t="s">
+      <c r="E107" s="85"/>
+      <c r="F107" s="95" t="s">
         <v>35</v>
       </c>
-      <c r="G107" s="23" t="s">
+      <c r="G107" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="H107" s="84"/>
-      <c r="I107" s="84"/>
+      <c r="H107" s="86"/>
+      <c r="I107" s="86"/>
     </row>
     <row r="108" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B108" s="84"/>
-      <c r="C108" s="84"/>
-      <c r="D108" s="84"/>
-      <c r="E108" s="84"/>
-      <c r="F108" s="84"/>
-      <c r="G108" s="84"/>
-      <c r="H108" s="84"/>
-      <c r="I108" s="84"/>
+      <c r="B108" s="86"/>
+      <c r="C108" s="86"/>
+      <c r="D108" s="86"/>
+      <c r="E108" s="86"/>
+      <c r="F108" s="86"/>
+      <c r="G108" s="86"/>
+      <c r="H108" s="86"/>
+      <c r="I108" s="86"/>
     </row>
     <row r="109" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B109" s="84"/>
-      <c r="C109" s="84"/>
-      <c r="D109" s="84"/>
-      <c r="E109" s="84"/>
-      <c r="F109" s="84"/>
-      <c r="G109" s="84"/>
-      <c r="H109" s="84"/>
-      <c r="I109" s="84"/>
+      <c r="B109" s="86"/>
+      <c r="C109" s="86"/>
+      <c r="D109" s="86"/>
+      <c r="E109" s="86"/>
+      <c r="F109" s="86"/>
+      <c r="G109" s="86"/>
+      <c r="H109" s="86"/>
+      <c r="I109" s="86"/>
     </row>
     <row r="110" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B110" s="84"/>
-      <c r="C110" s="84"/>
-      <c r="D110" s="84"/>
-      <c r="E110" s="84"/>
-      <c r="F110" s="84"/>
-      <c r="G110" s="84"/>
-      <c r="H110" s="84"/>
-      <c r="I110" s="84"/>
+      <c r="B110" s="86"/>
+      <c r="C110" s="86"/>
+      <c r="D110" s="86"/>
+      <c r="E110" s="86"/>
+      <c r="F110" s="86"/>
+      <c r="G110" s="86"/>
+      <c r="H110" s="86"/>
+      <c r="I110" s="86"/>
     </row>
     <row r="111" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B111" s="84"/>
-      <c r="C111" s="84"/>
-      <c r="D111" s="84"/>
-      <c r="E111" s="84"/>
-      <c r="F111" s="84"/>
-      <c r="G111" s="84"/>
-      <c r="H111" s="84"/>
-      <c r="I111" s="84"/>
+      <c r="B111" s="86"/>
+      <c r="C111" s="86"/>
+      <c r="D111" s="86"/>
+      <c r="E111" s="86"/>
+      <c r="F111" s="86"/>
+      <c r="G111" s="86"/>
+      <c r="H111" s="86"/>
+      <c r="I111" s="86"/>
     </row>
     <row r="113" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B113" s="84"/>
-      <c r="C113" s="84"/>
-      <c r="D113" s="84"/>
-      <c r="E113" s="84"/>
-      <c r="F113" s="84"/>
-      <c r="G113" s="84"/>
-      <c r="H113" s="84"/>
+      <c r="B113" s="86"/>
+      <c r="C113" s="86"/>
+      <c r="D113" s="86"/>
+      <c r="E113" s="86"/>
+      <c r="F113" s="86"/>
+      <c r="G113" s="86"/>
+      <c r="H113" s="86"/>
     </row>
     <row r="114" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B114" s="84"/>
-      <c r="C114" s="63" t="s">
+      <c r="B114" s="86"/>
+      <c r="C114" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="D114" s="63" t="s">
+      <c r="D114" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="E114" s="63" t="s">
+      <c r="E114" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="F114" s="63" t="s">
+      <c r="F114" s="65" t="s">
         <v>9</v>
       </c>
       <c r="G114" s="2"/>
-      <c r="H114" s="84"/>
+      <c r="H114" s="86"/>
     </row>
     <row r="115" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B115" s="84"/>
-      <c r="C115" s="21" t="s">
+      <c r="B115" s="86"/>
+      <c r="C115" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="D115" s="96" t="s">
+      <c r="D115" s="98" t="s">
         <v>21</v>
       </c>
-      <c r="E115" s="97" t="s">
+      <c r="E115" s="99" t="s">
         <v>16</v>
       </c>
-      <c r="F115" s="71">
+      <c r="F115" s="73">
         <v>9.5999999999999992E-3</v>
       </c>
-      <c r="G115" s="27" t="s">
+      <c r="G115" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="H115" s="84"/>
+      <c r="H115" s="86"/>
     </row>
     <row r="116" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B116" s="84"/>
-      <c r="C116" s="48"/>
-      <c r="D116" s="95"/>
-      <c r="E116" s="101" t="s">
+      <c r="B116" s="86"/>
+      <c r="C116" s="50"/>
+      <c r="D116" s="97"/>
+      <c r="E116" s="103" t="s">
         <v>20</v>
       </c>
-      <c r="F116" s="102">
+      <c r="F116" s="104">
         <v>2.6400000000000001E-5</v>
       </c>
-      <c r="G116" s="12" t="s">
+      <c r="G116" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="H116" s="84"/>
+      <c r="H116" s="86"/>
     </row>
     <row r="117" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B117" s="84"/>
-      <c r="C117" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="D117" s="52" t="s">
+      <c r="B117" s="86"/>
+      <c r="C117" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="D117" s="54" t="s">
         <v>21</v>
       </c>
       <c r="E117" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F117" s="76">
+      <c r="F117" s="78">
         <v>4.1599999999999996E-3</v>
       </c>
-      <c r="G117" s="104" t="s">
+      <c r="G117" s="106" t="s">
         <v>29</v>
       </c>
-      <c r="H117" s="84"/>
+      <c r="H117" s="86"/>
     </row>
     <row r="118" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B118" s="84"/>
-      <c r="C118" s="98" t="s">
+      <c r="B118" s="86"/>
+      <c r="C118" s="100" t="s">
         <v>2</v>
       </c>
-      <c r="D118" s="99" t="s">
+      <c r="D118" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="E118" s="100" t="s">
+      <c r="E118" s="102" t="s">
         <v>20</v>
       </c>
-      <c r="F118" s="103">
+      <c r="F118" s="105">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="G118" s="104" t="s">
+      <c r="G118" s="106" t="s">
         <v>30</v>
       </c>
-      <c r="H118" s="84"/>
+      <c r="H118" s="86"/>
     </row>
     <row r="119" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B119" s="84"/>
-      <c r="C119" s="84"/>
-      <c r="D119" s="84"/>
-      <c r="E119" s="84"/>
-      <c r="F119" s="84"/>
-      <c r="G119" s="84"/>
-      <c r="H119" s="84"/>
+      <c r="B119" s="86"/>
+      <c r="C119" s="86"/>
+      <c r="D119" s="86"/>
+      <c r="E119" s="86"/>
+      <c r="F119" s="86"/>
+      <c r="G119" s="86"/>
+      <c r="H119" s="86"/>
     </row>
     <row r="120" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B120" s="84"/>
-      <c r="C120" s="84"/>
-      <c r="D120" s="84"/>
-      <c r="E120" s="84"/>
-      <c r="F120" s="84"/>
-      <c r="G120" s="84"/>
-      <c r="H120" s="84"/>
+      <c r="B120" s="86"/>
+      <c r="C120" s="86"/>
+      <c r="D120" s="86"/>
+      <c r="E120" s="86"/>
+      <c r="F120" s="86"/>
+      <c r="G120" s="86"/>
+      <c r="H120" s="86"/>
     </row>
     <row r="121" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B121" s="84"/>
-      <c r="C121" s="84"/>
-      <c r="D121" s="84"/>
-      <c r="E121" s="84"/>
-      <c r="F121" s="84"/>
-      <c r="G121" s="84"/>
-      <c r="H121" s="84"/>
+      <c r="B121" s="86"/>
+      <c r="C121" s="86"/>
+      <c r="D121" s="86"/>
+      <c r="E121" s="86"/>
+      <c r="F121" s="86"/>
+      <c r="G121" s="86"/>
+      <c r="H121" s="86"/>
     </row>
     <row r="122" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B122" s="84"/>
-      <c r="C122" s="84"/>
-      <c r="D122" s="84"/>
-      <c r="E122" s="84"/>
-      <c r="F122" s="84"/>
-      <c r="G122" s="84"/>
-      <c r="H122" s="84"/>
+      <c r="B122" s="86"/>
+      <c r="C122" s="86"/>
+      <c r="D122" s="86"/>
+      <c r="E122" s="86"/>
+      <c r="F122" s="86"/>
+      <c r="G122" s="86"/>
+      <c r="H122" s="86"/>
     </row>
     <row r="126" spans="2:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="B126" s="94" t="s">
+      <c r="B126" s="96" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3356,7 +3388,7 @@
     <mergeCell ref="C71:C72"/>
     <mergeCell ref="C73:C76"/>
     <mergeCell ref="D75:D76"/>
-    <mergeCell ref="C48:I48"/>
+    <mergeCell ref="D47:J47"/>
     <mergeCell ref="C50:C53"/>
     <mergeCell ref="C54:C59"/>
     <mergeCell ref="D54:D55"/>
@@ -3375,11 +3407,1017 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="J6:J22">
-    <cfRule type="cellIs" dxfId="1" priority="3" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="3" stopIfTrue="1" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8F6DB0D-2B41-A146-8989-239E41193B1F}">
+  <dimension ref="B1:M53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B38" zoomScale="200" workbookViewId="0">
+      <selection activeCell="K48" sqref="K48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="25.5" customWidth="1"/>
+    <col min="5" max="10" width="9.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C1" s="86"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="86"/>
+      <c r="K1" s="86"/>
+      <c r="L1" s="86"/>
+    </row>
+    <row r="2" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+    </row>
+    <row r="3" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="86"/>
+      <c r="K3" s="108"/>
+      <c r="L3" s="86"/>
+      <c r="M3" s="86"/>
+    </row>
+    <row r="4" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="86"/>
+      <c r="D4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="107"/>
+      <c r="L4" s="86"/>
+      <c r="M4" s="86"/>
+    </row>
+    <row r="5" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C5" s="86"/>
+      <c r="D5" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="13">
+        <v>2.7719999999999998</v>
+      </c>
+      <c r="G5" s="13">
+        <v>3.45</v>
+      </c>
+      <c r="H5" s="13">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="I5" s="15"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="120"/>
+      <c r="L5" s="86"/>
+      <c r="M5" s="86"/>
+    </row>
+    <row r="6" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C6" s="86"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="70"/>
+      <c r="L6" s="86"/>
+      <c r="M6" s="86"/>
+    </row>
+    <row r="7" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C7" s="86"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="70"/>
+      <c r="L7" s="86"/>
+      <c r="M7" s="86"/>
+    </row>
+    <row r="8" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="86"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="70"/>
+      <c r="L8" s="86"/>
+      <c r="M8" s="86"/>
+    </row>
+    <row r="9" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C9" s="86"/>
+      <c r="D9" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="70"/>
+      <c r="L9" s="86"/>
+      <c r="M9" s="86"/>
+    </row>
+    <row r="10" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C10" s="86"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="86"/>
+    </row>
+    <row r="11" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C11" s="86"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="70"/>
+      <c r="L11" s="86"/>
+      <c r="M11" s="86"/>
+    </row>
+    <row r="12" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="86"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="70"/>
+      <c r="L12" s="86"/>
+      <c r="M12" s="86"/>
+    </row>
+    <row r="13" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C13" s="86"/>
+      <c r="D13" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="70"/>
+      <c r="L13" s="86"/>
+      <c r="M13" s="86"/>
+    </row>
+    <row r="14" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C14" s="86"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="70"/>
+      <c r="L14" s="86"/>
+      <c r="M14" s="86"/>
+    </row>
+    <row r="15" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C15" s="86"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="70"/>
+      <c r="L15" s="86"/>
+      <c r="M15" s="86"/>
+    </row>
+    <row r="16" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C16" s="86"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="122"/>
+      <c r="J16" s="122"/>
+      <c r="K16" s="70"/>
+      <c r="L16" s="86"/>
+      <c r="M16" s="86"/>
+    </row>
+    <row r="17" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C17" s="108"/>
+      <c r="D17" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="70"/>
+      <c r="L17" s="86"/>
+      <c r="M17" s="86"/>
+    </row>
+    <row r="18" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C18" s="108"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="70"/>
+      <c r="L18" s="86"/>
+      <c r="M18" s="86"/>
+    </row>
+    <row r="19" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C19" s="108"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="70"/>
+      <c r="L19" s="86"/>
+      <c r="M19" s="86"/>
+    </row>
+    <row r="20" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C20" s="108"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="122"/>
+      <c r="J20" s="122"/>
+      <c r="K20" s="121"/>
+      <c r="L20" s="86"/>
+      <c r="M20" s="86"/>
+    </row>
+    <row r="21" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C21" s="108"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="108"/>
+      <c r="F21" s="108"/>
+      <c r="G21" s="108"/>
+      <c r="H21" s="108"/>
+      <c r="I21" s="108"/>
+      <c r="J21" s="108"/>
+      <c r="K21" s="108"/>
+      <c r="L21" s="86"/>
+      <c r="M21" s="86"/>
+    </row>
+    <row r="22" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C22" s="86"/>
+      <c r="D22" s="67" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="67"/>
+      <c r="F22" s="67"/>
+      <c r="G22" s="67"/>
+      <c r="H22" s="67"/>
+      <c r="I22" s="67"/>
+      <c r="J22" s="67"/>
+      <c r="K22" s="108"/>
+      <c r="L22" s="86"/>
+      <c r="M22" s="86"/>
+    </row>
+    <row r="23" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="86"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="108"/>
+      <c r="F23" s="108"/>
+      <c r="G23" s="108"/>
+      <c r="H23" s="108"/>
+      <c r="I23" s="108"/>
+      <c r="J23" s="108"/>
+      <c r="K23" s="108"/>
+      <c r="L23" s="86"/>
+      <c r="M23" s="86"/>
+    </row>
+    <row r="24" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="86"/>
+      <c r="D24" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" s="124" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="124" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="124" t="s">
+        <v>8</v>
+      </c>
+      <c r="H24" s="124" t="s">
+        <v>9</v>
+      </c>
+      <c r="I24" s="124" t="s">
+        <v>43</v>
+      </c>
+      <c r="J24" s="124" t="s">
+        <v>44</v>
+      </c>
+      <c r="K24" s="107"/>
+      <c r="L24" s="86"/>
+      <c r="M24" s="86"/>
+    </row>
+    <row r="25" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C25" s="86"/>
+      <c r="D25" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" s="13">
+        <v>2.7719999999999998</v>
+      </c>
+      <c r="F25" s="13">
+        <v>3.45</v>
+      </c>
+      <c r="G25" s="13">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="H25" s="15">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="I25" s="15">
+        <v>3.6799999999999999E-2</v>
+      </c>
+      <c r="J25" s="125">
+        <v>32</v>
+      </c>
+      <c r="K25" s="120"/>
+      <c r="L25" s="86"/>
+      <c r="M25" s="86"/>
+    </row>
+    <row r="26" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C26" s="86"/>
+      <c r="D26" s="123" t="s">
+        <v>41</v>
+      </c>
+      <c r="E26" s="13">
+        <v>1</v>
+      </c>
+      <c r="F26" s="13">
+        <v>1</v>
+      </c>
+      <c r="G26" s="13">
+        <v>0.182</v>
+      </c>
+      <c r="H26" s="15">
+        <v>0.67200000000000004</v>
+      </c>
+      <c r="I26" s="15">
+        <v>-2.5399999999999999E-2</v>
+      </c>
+      <c r="J26" s="125">
+        <v>34</v>
+      </c>
+      <c r="K26" s="70"/>
+      <c r="L26" s="86"/>
+      <c r="M26" s="86"/>
+    </row>
+    <row r="27" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C27" s="86"/>
+      <c r="D27" s="123" t="s">
+        <v>45</v>
+      </c>
+      <c r="E27" s="13">
+        <v>1</v>
+      </c>
+      <c r="F27" s="13">
+        <v>1</v>
+      </c>
+      <c r="G27" s="13">
+        <v>2.077</v>
+      </c>
+      <c r="H27" s="15">
+        <v>0.161</v>
+      </c>
+      <c r="I27" s="11">
+        <v>3.5799999999999998E-2</v>
+      </c>
+      <c r="J27" s="125">
+        <v>30</v>
+      </c>
+      <c r="K27" s="8"/>
+    </row>
+    <row r="28" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C28" s="86"/>
+      <c r="D28" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="E28" s="14">
+        <v>5.5380000000000003</v>
+      </c>
+      <c r="F28" s="14">
+        <v>6.4260000000000002</v>
+      </c>
+      <c r="G28" s="14">
+        <v>6.1020000000000003</v>
+      </c>
+      <c r="H28" s="132">
+        <v>3.4900000000000003E-4</v>
+      </c>
+      <c r="I28" s="12">
+        <v>0.52100000000000002</v>
+      </c>
+      <c r="J28" s="126">
+        <v>34</v>
+      </c>
+      <c r="K28" s="70"/>
+    </row>
+    <row r="29" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C29" s="86"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="130"/>
+      <c r="I29" s="114"/>
+      <c r="J29" s="131"/>
+      <c r="K29" s="70"/>
+    </row>
+    <row r="30" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C30" s="86"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="G30" s="29"/>
+      <c r="H30" s="130"/>
+      <c r="I30" s="114"/>
+      <c r="J30" s="131"/>
+      <c r="K30" s="70"/>
+    </row>
+    <row r="31" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C31" s="86"/>
+      <c r="D31" s="86"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="127"/>
+      <c r="K31" s="70"/>
+    </row>
+    <row r="32" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C32" s="86"/>
+      <c r="D32" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32" s="124" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="124" t="s">
+        <v>11</v>
+      </c>
+      <c r="G32" s="124" t="s">
+        <v>8</v>
+      </c>
+      <c r="H32" s="124" t="s">
+        <v>9</v>
+      </c>
+      <c r="I32" s="124" t="s">
+        <v>43</v>
+      </c>
+      <c r="J32" s="128" t="s">
+        <v>44</v>
+      </c>
+      <c r="K32" s="120"/>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C33" s="86"/>
+      <c r="D33" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E33" s="13">
+        <v>3.81</v>
+      </c>
+      <c r="F33" s="13">
+        <v>4.6059999999999999</v>
+      </c>
+      <c r="G33" s="13">
+        <v>1.6559999999999999</v>
+      </c>
+      <c r="H33" s="15">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="I33" s="15">
+        <v>0.151</v>
+      </c>
+      <c r="J33" s="125">
+        <v>32</v>
+      </c>
+      <c r="K33" s="70"/>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C34" s="108"/>
+      <c r="D34" s="123" t="s">
+        <v>41</v>
+      </c>
+      <c r="E34" s="13">
+        <v>1</v>
+      </c>
+      <c r="F34" s="13">
+        <v>1</v>
+      </c>
+      <c r="G34" s="13">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="H34" s="15">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="I34" s="15">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="J34" s="125">
+        <v>34</v>
+      </c>
+      <c r="K34" s="8"/>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C35" s="108"/>
+      <c r="D35" s="123" t="s">
+        <v>45</v>
+      </c>
+      <c r="E35" s="13">
+        <v>1</v>
+      </c>
+      <c r="F35" s="13">
+        <v>1</v>
+      </c>
+      <c r="G35" s="13">
+        <v>3.3260000000000001</v>
+      </c>
+      <c r="H35" s="134">
+        <v>7.8899999999999998E-2</v>
+      </c>
+      <c r="I35" s="11">
+        <v>7.4300000000000005E-2</v>
+      </c>
+      <c r="J35" s="125">
+        <v>30</v>
+      </c>
+      <c r="K35" s="120"/>
+    </row>
+    <row r="36" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C36" s="108"/>
+      <c r="D36" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="E36" s="14">
+        <v>3.101</v>
+      </c>
+      <c r="F36" s="14">
+        <v>3.8519999999999999</v>
+      </c>
+      <c r="G36" s="14">
+        <v>3.5990000000000002</v>
+      </c>
+      <c r="H36" s="133">
+        <v>0.02</v>
+      </c>
+      <c r="I36" s="12">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="J36" s="126">
+        <v>34</v>
+      </c>
+      <c r="K36" s="70"/>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C37" s="108"/>
+      <c r="D37" s="123"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="120"/>
+      <c r="K37" s="8"/>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C38" s="108"/>
+      <c r="D38" s="123"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="G38" s="13"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="11"/>
+      <c r="J38" s="120"/>
+      <c r="K38" s="8"/>
+    </row>
+    <row r="39" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="23"/>
+      <c r="C39" s="86"/>
+      <c r="D39" s="86"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="127"/>
+      <c r="K39" s="70"/>
+    </row>
+    <row r="40" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C40" s="86"/>
+      <c r="D40" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E40" s="124" t="s">
+        <v>7</v>
+      </c>
+      <c r="F40" s="124" t="s">
+        <v>11</v>
+      </c>
+      <c r="G40" s="124" t="s">
+        <v>8</v>
+      </c>
+      <c r="H40" s="124" t="s">
+        <v>9</v>
+      </c>
+      <c r="I40" s="124" t="s">
+        <v>43</v>
+      </c>
+      <c r="J40" s="128" t="s">
+        <v>44</v>
+      </c>
+      <c r="K40" s="120"/>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C41" s="86"/>
+      <c r="D41" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E41" s="13">
+        <v>3.8519999999999999</v>
+      </c>
+      <c r="F41" s="13">
+        <v>4.6539999999999999</v>
+      </c>
+      <c r="G41" s="13">
+        <v>1.4690000000000001</v>
+      </c>
+      <c r="H41" s="15">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="I41" s="15">
+        <v>0.161</v>
+      </c>
+      <c r="J41" s="125">
+        <v>32</v>
+      </c>
+      <c r="K41" s="70"/>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C42" s="108"/>
+      <c r="D42" s="123" t="s">
+        <v>41</v>
+      </c>
+      <c r="E42" s="13">
+        <v>1.704</v>
+      </c>
+      <c r="F42" s="13">
+        <v>2.1019999999999999</v>
+      </c>
+      <c r="G42" s="13">
+        <v>1.0329999999999999</v>
+      </c>
+      <c r="H42" s="15">
+        <v>0.36299999999999999</v>
+      </c>
+      <c r="I42" s="15">
+        <v>3.95E-2</v>
+      </c>
+      <c r="J42" s="125">
+        <v>34</v>
+      </c>
+      <c r="K42" s="8"/>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C43" s="108"/>
+      <c r="D43" s="123" t="s">
+        <v>45</v>
+      </c>
+      <c r="E43" s="13">
+        <v>1.258</v>
+      </c>
+      <c r="F43" s="13">
+        <v>1.47</v>
+      </c>
+      <c r="G43" s="13">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="H43" s="15">
+        <v>0.83799999999999997</v>
+      </c>
+      <c r="I43" s="11">
+        <v>-2.07E-2</v>
+      </c>
+      <c r="J43" s="125">
+        <v>30</v>
+      </c>
+      <c r="K43" s="120"/>
+    </row>
+    <row r="44" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C44" s="108"/>
+      <c r="D44" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="E44" s="14">
+        <v>1.8839999999999999</v>
+      </c>
+      <c r="F44" s="14">
+        <v>2.3580000000000001</v>
+      </c>
+      <c r="G44" s="14">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="H44" s="129">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="I44" s="12">
+        <v>2.3E-2</v>
+      </c>
+      <c r="J44" s="126">
+        <v>34</v>
+      </c>
+      <c r="K44" s="70"/>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C45" s="108"/>
+      <c r="D45" s="123"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="15"/>
+      <c r="I45" s="11"/>
+      <c r="J45" s="120"/>
+      <c r="K45" s="8"/>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C46" s="108"/>
+      <c r="D46" s="123"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G46" s="13"/>
+      <c r="H46" s="15"/>
+      <c r="I46" s="11"/>
+      <c r="J46" s="120"/>
+      <c r="K46" s="8"/>
+    </row>
+    <row r="47" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C47" s="86"/>
+      <c r="D47" s="86"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="15"/>
+      <c r="I47" s="11"/>
+      <c r="J47" s="127"/>
+      <c r="K47" s="70"/>
+    </row>
+    <row r="48" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C48" s="86"/>
+      <c r="D48" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E48" s="124" t="s">
+        <v>7</v>
+      </c>
+      <c r="F48" s="124" t="s">
+        <v>11</v>
+      </c>
+      <c r="G48" s="124" t="s">
+        <v>8</v>
+      </c>
+      <c r="H48" s="124" t="s">
+        <v>9</v>
+      </c>
+      <c r="I48" s="124" t="s">
+        <v>43</v>
+      </c>
+      <c r="J48" s="128" t="s">
+        <v>44</v>
+      </c>
+      <c r="K48" s="120"/>
+    </row>
+    <row r="49" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C49" s="86"/>
+      <c r="D49" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E49" s="13">
+        <v>1</v>
+      </c>
+      <c r="F49" s="13">
+        <v>1</v>
+      </c>
+      <c r="G49" s="13">
+        <v>6.3959999999999999</v>
+      </c>
+      <c r="H49" s="135">
+        <v>1.8100000000000002E-2</v>
+      </c>
+      <c r="I49" s="15">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="J49" s="125">
+        <v>27</v>
+      </c>
+      <c r="K49" s="70"/>
+    </row>
+    <row r="50" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C50" s="108"/>
+      <c r="D50" s="123" t="s">
+        <v>41</v>
+      </c>
+      <c r="E50" s="13">
+        <v>1</v>
+      </c>
+      <c r="F50" s="13">
+        <v>1</v>
+      </c>
+      <c r="G50" s="13">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="H50" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="I50" s="15">
+        <v>-9.6699999999999998E-3</v>
+      </c>
+      <c r="J50" s="125">
+        <v>29</v>
+      </c>
+      <c r="K50" s="8"/>
+    </row>
+    <row r="51" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C51" s="108"/>
+      <c r="D51" s="123" t="s">
+        <v>45</v>
+      </c>
+      <c r="E51" s="13">
+        <v>1.76</v>
+      </c>
+      <c r="F51" s="13">
+        <v>2.19</v>
+      </c>
+      <c r="G51" s="13">
+        <v>0.78300000000000003</v>
+      </c>
+      <c r="H51" s="15">
+        <v>0.44900000000000001</v>
+      </c>
+      <c r="I51" s="11">
+        <v>4.0500000000000001E-2</v>
+      </c>
+      <c r="J51" s="125">
+        <v>26</v>
+      </c>
+      <c r="K51" s="120"/>
+    </row>
+    <row r="52" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C52" s="108"/>
+      <c r="D52" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="E52" s="14">
+        <v>1.8240000000000001</v>
+      </c>
+      <c r="F52" s="14">
+        <v>2.2730000000000001</v>
+      </c>
+      <c r="G52" s="14">
+        <v>8.5969999999999995</v>
+      </c>
+      <c r="H52" s="132">
+        <v>1.0200000000000001E-3</v>
+      </c>
+      <c r="I52" s="12">
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="J52" s="126">
+        <v>29</v>
+      </c>
+      <c r="K52" s="70"/>
+    </row>
+    <row r="53" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C53" s="108"/>
+      <c r="D53" s="123"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="13"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="15"/>
+      <c r="I53" s="11"/>
+      <c r="J53" s="120"/>
+      <c r="K53" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="D17:D20"/>
+    <mergeCell ref="D5:D8"/>
+    <mergeCell ref="D9:D12"/>
+    <mergeCell ref="D13:D16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updating the excel spread sheet and testing out new ways to plot the heatmaps
</commit_message>
<xml_diff>
--- a/K4S_key_scripts/K4S_DA_Aims/K4S_DA_A2/K4S_DA_A2/K4S_DA_A2_GAM_Temporal_Results.xlsx
+++ b/K4S_key_scripts/K4S_DA_Aims/K4S_DA_A2/K4S_DA_A2/K4S_DA_A2_GAM_Temporal_Results.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoestarkey/Desktop/Honours/Data_Analysis/K_axis_midoc/K4S_key_scripts/K4S_DA_Aims/K4S_DA_A2/K4S_DA_A2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2406DD-FE75-0B46-814F-9F23E46CCEF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9037F72-2DE6-6849-8957-AD33B46C82E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5600" yWindow="900" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{33E5A15D-DBA6-5B40-873E-91FBDBF28531}"/>
+    <workbookView xWindow="5600" yWindow="880" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{33E5A15D-DBA6-5B40-873E-91FBDBF28531}"/>
   </bookViews>
   <sheets>
     <sheet name="GAM_Temporal_Sum" sheetId="1" r:id="rId1"/>
-    <sheet name="GAM_Temporal_Depth" sheetId="2" r:id="rId2"/>
-    <sheet name="GAM_Sat+Insitu_Sum" sheetId="3" r:id="rId3"/>
+    <sheet name="GAM_Temporal_Depth_Before_Refit" sheetId="2" r:id="rId2"/>
+    <sheet name="GAM_Temporal_Depth_After_Refit" sheetId="4" r:id="rId3"/>
+    <sheet name="GAM_Sat+Insitu_Sum" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="51">
   <si>
     <t>Season</t>
   </si>
@@ -152,9 +153,6 @@
 800-1000</t>
   </si>
   <si>
-    <t>GAMM + RE SUMMARY</t>
-  </si>
-  <si>
     <t>Satellite Factor</t>
   </si>
   <si>
@@ -200,7 +198,13 @@
     <t>KRILL</t>
   </si>
   <si>
-    <t>GAM SUMMARY</t>
+    <t xml:space="preserve"> Before Refit GAMM + RE SUMMARY</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Before Refit GAM SUMMARY</t>
+  </si>
+  <si>
+    <t>After  Refit GAMM + RE SUMMARY</t>
   </si>
 </sst>
 </file>
@@ -400,7 +404,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -679,56 +683,87 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1450,10 +1485,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC0FF2A1-C6A7-6249-9809-08DF6541B68E}">
-  <dimension ref="B4:N126"/>
+  <dimension ref="B4:X126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="91" zoomScaleNormal="117" workbookViewId="0">
-      <selection activeCell="J68" sqref="J68"/>
+    <sheetView topLeftCell="L39" zoomScale="116" zoomScaleNormal="117" workbookViewId="0">
+      <selection activeCell="P47" sqref="P47:X66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1495,7 +1530,7 @@
       <c r="C6" s="104" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="115" t="s">
+      <c r="D6" s="107" t="s">
         <v>15</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -1509,7 +1544,7 @@
     </row>
     <row r="7" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C7" s="104"/>
-      <c r="D7" s="116"/>
+      <c r="D7" s="108"/>
       <c r="E7" s="3" t="s">
         <v>17</v>
       </c>
@@ -1521,7 +1556,7 @@
     </row>
     <row r="8" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C8" s="104"/>
-      <c r="D8" s="116"/>
+      <c r="D8" s="108"/>
       <c r="E8" s="3" t="s">
         <v>18</v>
       </c>
@@ -1533,7 +1568,7 @@
     </row>
     <row r="9" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9" s="104"/>
-      <c r="D9" s="116"/>
+      <c r="D9" s="108"/>
       <c r="E9" s="3" t="s">
         <v>19</v>
       </c>
@@ -1545,7 +1580,7 @@
     </row>
     <row r="10" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="104"/>
-      <c r="D10" s="116"/>
+      <c r="D10" s="108"/>
       <c r="E10" s="3" t="s">
         <v>20</v>
       </c>
@@ -1682,26 +1717,26 @@
     <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B26" s="66"/>
       <c r="C26" s="66"/>
-      <c r="D26" s="122" t="s">
+      <c r="D26" s="109" t="s">
         <v>49</v>
       </c>
-      <c r="E26" s="122"/>
-      <c r="F26" s="122"/>
-      <c r="G26" s="122"/>
-      <c r="H26" s="122"/>
-      <c r="I26" s="122"/>
-      <c r="J26" s="122"/>
+      <c r="E26" s="109"/>
+      <c r="F26" s="109"/>
+      <c r="G26" s="109"/>
+      <c r="H26" s="109"/>
+      <c r="I26" s="109"/>
+      <c r="J26" s="109"/>
       <c r="K26" s="66"/>
     </row>
     <row r="27" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" s="66"/>
-      <c r="C27" s="121"/>
-      <c r="D27" s="121"/>
-      <c r="E27" s="121"/>
-      <c r="F27" s="121"/>
-      <c r="G27" s="121"/>
-      <c r="H27" s="121"/>
-      <c r="I27" s="121"/>
+      <c r="C27" s="106"/>
+      <c r="D27" s="106"/>
+      <c r="E27" s="106"/>
+      <c r="F27" s="106"/>
+      <c r="G27" s="106"/>
+      <c r="H27" s="106"/>
+      <c r="I27" s="106"/>
       <c r="J27" s="66"/>
       <c r="K27" s="66"/>
     </row>
@@ -1733,7 +1768,7 @@
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B29" s="66"/>
-      <c r="C29" s="109" t="s">
+      <c r="C29" s="114" t="s">
         <v>0</v>
       </c>
       <c r="D29" s="33" t="s">
@@ -1762,7 +1797,7 @@
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B30" s="66"/>
-      <c r="C30" s="110"/>
+      <c r="C30" s="113"/>
       <c r="D30" s="33" t="s">
         <v>22</v>
       </c>
@@ -1789,7 +1824,7 @@
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B31" s="66"/>
-      <c r="C31" s="110"/>
+      <c r="C31" s="113"/>
       <c r="D31" s="33" t="s">
         <v>6</v>
       </c>
@@ -1816,8 +1851,8 @@
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B32" s="66"/>
-      <c r="C32" s="110"/>
-      <c r="D32" s="110" t="s">
+      <c r="C32" s="113"/>
+      <c r="D32" s="113" t="s">
         <v>24</v>
       </c>
       <c r="E32" s="3" t="s">
@@ -1841,10 +1876,10 @@
       </c>
       <c r="K32" s="66"/>
     </row>
-    <row r="33" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B33" s="66"/>
-      <c r="C33" s="110"/>
-      <c r="D33" s="110"/>
+      <c r="C33" s="113"/>
+      <c r="D33" s="113"/>
       <c r="E33" s="3" t="s">
         <v>20</v>
       </c>
@@ -1869,12 +1904,12 @@
       <c r="M33" s="10"/>
       <c r="N33" s="18"/>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B34" s="66"/>
-      <c r="C34" s="106" t="s">
-        <v>1</v>
-      </c>
-      <c r="D34" s="106" t="s">
+      <c r="C34" s="110" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" s="110" t="s">
         <v>15</v>
       </c>
       <c r="E34" s="22" t="s">
@@ -1898,7 +1933,7 @@
       </c>
       <c r="K34" s="66"/>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B35" s="66"/>
       <c r="C35" s="104"/>
       <c r="D35" s="111"/>
@@ -1923,10 +1958,10 @@
       </c>
       <c r="K35" s="66"/>
     </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B36" s="66"/>
       <c r="C36" s="104"/>
-      <c r="D36" s="114" t="s">
+      <c r="D36" s="112" t="s">
         <v>22</v>
       </c>
       <c r="E36" s="29" t="s">
@@ -1950,7 +1985,7 @@
       </c>
       <c r="K36" s="66"/>
     </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B37" s="66"/>
       <c r="C37" s="104"/>
       <c r="D37" s="111"/>
@@ -1975,7 +2010,7 @@
       </c>
       <c r="K37" s="66"/>
     </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B38" s="66"/>
       <c r="C38" s="104"/>
       <c r="D38" s="33" t="s">
@@ -2002,7 +2037,7 @@
       </c>
       <c r="K38" s="66"/>
     </row>
-    <row r="39" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B39" s="66"/>
       <c r="C39" s="105"/>
       <c r="D39" s="5" t="s">
@@ -2029,9 +2064,9 @@
       </c>
       <c r="K39" s="66"/>
     </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B40" s="66"/>
-      <c r="C40" s="106" t="s">
+      <c r="C40" s="110" t="s">
         <v>2</v>
       </c>
       <c r="D40" s="33" t="s">
@@ -2058,7 +2093,7 @@
       </c>
       <c r="K40" s="66"/>
     </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B41" s="66"/>
       <c r="C41" s="104"/>
       <c r="D41" s="33" t="s">
@@ -2085,7 +2120,7 @@
       </c>
       <c r="K41" s="66"/>
     </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B42" s="66"/>
       <c r="C42" s="104"/>
       <c r="D42" s="33" t="s">
@@ -2099,7 +2134,7 @@
       <c r="J42" s="86"/>
       <c r="K42" s="66"/>
     </row>
-    <row r="43" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B43" s="66"/>
       <c r="C43" s="105"/>
       <c r="D43" s="5" t="s">
@@ -2126,7 +2161,7 @@
       </c>
       <c r="K43" s="66"/>
     </row>
-    <row r="44" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B44" s="66"/>
       <c r="C44" s="38"/>
       <c r="D44" s="66"/>
@@ -2138,7 +2173,7 @@
       <c r="J44" s="66"/>
       <c r="K44" s="66"/>
     </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B45" s="66"/>
       <c r="C45" s="66"/>
       <c r="D45" s="66"/>
@@ -2150,23 +2185,34 @@
       <c r="J45" s="66"/>
       <c r="K45" s="66"/>
     </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:24" x14ac:dyDescent="0.2">
       <c r="K46" s="66"/>
     </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C47" s="66"/>
-      <c r="D47" s="122" t="s">
-        <v>37</v>
-      </c>
-      <c r="E47" s="122"/>
-      <c r="F47" s="122"/>
-      <c r="G47" s="122"/>
-      <c r="H47" s="122"/>
-      <c r="I47" s="122"/>
-      <c r="J47" s="122"/>
+      <c r="D47" s="109" t="s">
+        <v>48</v>
+      </c>
+      <c r="E47" s="109"/>
+      <c r="F47" s="109"/>
+      <c r="G47" s="109"/>
+      <c r="H47" s="109"/>
+      <c r="I47" s="109"/>
+      <c r="J47" s="109"/>
       <c r="K47" s="66"/>
-    </row>
-    <row r="48" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P47" s="66"/>
+      <c r="Q47" s="109" t="s">
+        <v>50</v>
+      </c>
+      <c r="R47" s="109"/>
+      <c r="S47" s="109"/>
+      <c r="T47" s="109"/>
+      <c r="U47" s="109"/>
+      <c r="V47" s="109"/>
+      <c r="W47" s="109"/>
+      <c r="X47" s="66"/>
+    </row>
+    <row r="48" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B48" s="66"/>
       <c r="C48" s="66"/>
       <c r="D48" s="66"/>
@@ -2177,8 +2223,18 @@
       <c r="I48" s="66"/>
       <c r="J48" s="66"/>
       <c r="K48" s="66"/>
-    </row>
-    <row r="49" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="O48" s="66"/>
+      <c r="P48" s="66"/>
+      <c r="Q48" s="66"/>
+      <c r="R48" s="66"/>
+      <c r="S48" s="66"/>
+      <c r="T48" s="66"/>
+      <c r="U48" s="66"/>
+      <c r="V48" s="66"/>
+      <c r="W48" s="66"/>
+      <c r="X48" s="66"/>
+    </row>
+    <row r="49" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B49" s="66"/>
       <c r="C49" s="2" t="s">
         <v>10</v>
@@ -2203,10 +2259,34 @@
       </c>
       <c r="J49" s="2"/>
       <c r="K49" s="66"/>
-    </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="O49" s="66"/>
+      <c r="P49" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q49" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="R49" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="S49" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="T49" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="U49" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="V49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="W49" s="2"/>
+      <c r="X49" s="66"/>
+    </row>
+    <row r="50" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B50" s="66"/>
-      <c r="C50" s="109" t="s">
+      <c r="C50" s="114" t="s">
         <v>0</v>
       </c>
       <c r="D50" s="33" t="s">
@@ -2232,10 +2312,37 @@
         <v>&lt;0.1</v>
       </c>
       <c r="K50" s="66"/>
-    </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="O50" s="66"/>
+      <c r="P50" s="114" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q50" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="R50" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="S50" s="35">
+        <v>1</v>
+      </c>
+      <c r="T50" s="35">
+        <v>1</v>
+      </c>
+      <c r="U50" s="35">
+        <v>3.5569999999999999</v>
+      </c>
+      <c r="V50" s="36">
+        <v>6.1100000000000002E-2</v>
+      </c>
+      <c r="W50" s="84" t="str">
+        <f>IF(V50&lt;0.05, "&lt;0.05", IF(V50&lt;0.1, "&lt;0.1", ""))</f>
+        <v>&lt;0.1</v>
+      </c>
+      <c r="X50" s="66"/>
+    </row>
+    <row r="51" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B51" s="66"/>
-      <c r="C51" s="110"/>
+      <c r="C51" s="113"/>
       <c r="D51" s="33" t="s">
         <v>5</v>
       </c>
@@ -2259,10 +2366,35 @@
         <v>&lt;0.1</v>
       </c>
       <c r="K51" s="66"/>
-    </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="O51" s="66"/>
+      <c r="P51" s="113"/>
+      <c r="Q51" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="R51" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="S51" s="35">
+        <v>1</v>
+      </c>
+      <c r="T51" s="35">
+        <v>1</v>
+      </c>
+      <c r="U51" s="35">
+        <v>3.1829999999999998</v>
+      </c>
+      <c r="V51" s="36">
+        <v>7.6300000000000007E-2</v>
+      </c>
+      <c r="W51" s="84" t="str">
+        <f t="shared" ref="W51:W62" si="2">IF(V51&lt;0.05, "&lt;0.05", IF(V51&lt;0.1, "&lt;0.1", ""))</f>
+        <v>&lt;0.1</v>
+      </c>
+      <c r="X51" s="66"/>
+    </row>
+    <row r="52" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B52" s="66"/>
-      <c r="C52" s="110"/>
+      <c r="C52" s="113"/>
       <c r="D52" s="33" t="s">
         <v>6</v>
       </c>
@@ -2286,10 +2418,35 @@
         <v>&lt;0.05</v>
       </c>
       <c r="K52" s="66"/>
-    </row>
-    <row r="53" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="O52" s="66"/>
+      <c r="P52" s="113"/>
+      <c r="Q52" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="R52" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="S52" s="35">
+        <v>1</v>
+      </c>
+      <c r="T52" s="35">
+        <v>1</v>
+      </c>
+      <c r="U52" s="35">
+        <v>6.492</v>
+      </c>
+      <c r="V52" s="36">
+        <v>1.18E-2</v>
+      </c>
+      <c r="W52" s="84" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;0.05</v>
+      </c>
+      <c r="X52" s="66"/>
+    </row>
+    <row r="53" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B53" s="66"/>
-      <c r="C53" s="110"/>
+      <c r="C53" s="113"/>
       <c r="D53" s="17" t="s">
         <v>24</v>
       </c>
@@ -2302,13 +2459,27 @@
       <c r="I53" s="46"/>
       <c r="J53" s="88"/>
       <c r="K53" s="66"/>
-    </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="O53" s="66"/>
+      <c r="P53" s="113"/>
+      <c r="Q53" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="R53" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="S53" s="45"/>
+      <c r="T53" s="45"/>
+      <c r="U53" s="45"/>
+      <c r="V53" s="46"/>
+      <c r="W53" s="88"/>
+      <c r="X53" s="66"/>
+    </row>
+    <row r="54" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B54" s="66"/>
-      <c r="C54" s="106" t="s">
-        <v>1</v>
-      </c>
-      <c r="D54" s="109" t="s">
+      <c r="C54" s="110" t="s">
+        <v>1</v>
+      </c>
+      <c r="D54" s="114" t="s">
         <v>25</v>
       </c>
       <c r="E54" s="22" t="s">
@@ -2331,11 +2502,38 @@
         <v>&lt;0.05</v>
       </c>
       <c r="K54" s="66"/>
-    </row>
-    <row r="55" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="O54" s="66"/>
+      <c r="P54" s="110" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q54" s="114" t="s">
+        <v>25</v>
+      </c>
+      <c r="R54" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="S54" s="23">
+        <v>1</v>
+      </c>
+      <c r="T54" s="23">
+        <v>1</v>
+      </c>
+      <c r="U54" s="23">
+        <v>4.4020000000000001</v>
+      </c>
+      <c r="V54" s="24">
+        <v>3.7449999999999997E-2</v>
+      </c>
+      <c r="W54" s="63" t="str">
+        <f t="shared" ref="W54:W65" si="3">IF(V54&lt;0.05, "&lt;0.05", IF(V54&lt;0.1, "&lt;0.1", ""))</f>
+        <v>&lt;0.05</v>
+      </c>
+      <c r="X54" s="66"/>
+    </row>
+    <row r="55" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B55" s="66"/>
       <c r="C55" s="104"/>
-      <c r="D55" s="119"/>
+      <c r="D55" s="115"/>
       <c r="E55" s="26" t="s">
         <v>26</v>
       </c>
@@ -2356,11 +2554,34 @@
         <v>&lt;0.05</v>
       </c>
       <c r="K55" s="66"/>
-    </row>
-    <row r="56" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="O55" s="66"/>
+      <c r="P55" s="104"/>
+      <c r="Q55" s="115"/>
+      <c r="R55" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="S55" s="27">
+        <v>2.6040000000000001</v>
+      </c>
+      <c r="T55" s="27">
+        <v>2.6040000000000001</v>
+      </c>
+      <c r="U55" s="27">
+        <v>5.57</v>
+      </c>
+      <c r="V55" s="28">
+        <v>9.8700000000000003E-3</v>
+      </c>
+      <c r="W55" s="85" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;0.05</v>
+      </c>
+      <c r="X55" s="66"/>
+    </row>
+    <row r="56" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B56" s="66"/>
       <c r="C56" s="104"/>
-      <c r="D56" s="118" t="s">
+      <c r="D56" s="116" t="s">
         <v>5</v>
       </c>
       <c r="E56" s="29" t="s">
@@ -2383,11 +2604,36 @@
         <v>&lt;0.05</v>
       </c>
       <c r="K56" s="66"/>
-    </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="O56" s="66"/>
+      <c r="P56" s="104"/>
+      <c r="Q56" s="116" t="s">
+        <v>5</v>
+      </c>
+      <c r="R56" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="S56" s="30">
+        <v>1</v>
+      </c>
+      <c r="T56" s="30">
+        <v>1</v>
+      </c>
+      <c r="U56" s="30">
+        <v>4.1509999999999998</v>
+      </c>
+      <c r="V56" s="24">
+        <v>4.3200000000000002E-2</v>
+      </c>
+      <c r="W56" s="63" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;0.05</v>
+      </c>
+      <c r="X56" s="66"/>
+    </row>
+    <row r="57" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B57" s="66"/>
       <c r="C57" s="104"/>
-      <c r="D57" s="119"/>
+      <c r="D57" s="115"/>
       <c r="E57" s="32" t="s">
         <v>20</v>
       </c>
@@ -2408,8 +2654,31 @@
         <v>&lt;0.05</v>
       </c>
       <c r="K57" s="66"/>
-    </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="O57" s="66"/>
+      <c r="P57" s="104"/>
+      <c r="Q57" s="115"/>
+      <c r="R57" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="S57" s="27">
+        <v>2.036</v>
+      </c>
+      <c r="T57" s="27">
+        <v>2.036</v>
+      </c>
+      <c r="U57" s="27">
+        <v>3.661</v>
+      </c>
+      <c r="V57" s="28">
+        <v>3.4200000000000001E-2</v>
+      </c>
+      <c r="W57" s="85" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;0.05</v>
+      </c>
+      <c r="X57" s="66"/>
+    </row>
+    <row r="58" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B58" s="66"/>
       <c r="C58" s="104"/>
       <c r="D58" s="33" t="s">
@@ -2435,8 +2704,33 @@
         <v>&lt;0.05</v>
       </c>
       <c r="K58" s="66"/>
-    </row>
-    <row r="59" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="O58" s="66"/>
+      <c r="P58" s="104"/>
+      <c r="Q58" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="R58" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="S58" s="35">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="T58" s="35">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="U58" s="35">
+        <v>4.51</v>
+      </c>
+      <c r="V58" s="36">
+        <v>3.5299999999999998E-2</v>
+      </c>
+      <c r="W58" s="84" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;0.05</v>
+      </c>
+      <c r="X58" s="66"/>
+    </row>
+    <row r="59" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B59" s="66"/>
       <c r="C59" s="105"/>
       <c r="D59" s="5" t="s">
@@ -2451,10 +2745,24 @@
       <c r="I59" s="46"/>
       <c r="J59" s="88"/>
       <c r="K59" s="66"/>
-    </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="O59" s="66"/>
+      <c r="P59" s="105"/>
+      <c r="Q59" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="R59" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="S59" s="45"/>
+      <c r="T59" s="45"/>
+      <c r="U59" s="45"/>
+      <c r="V59" s="46"/>
+      <c r="W59" s="88"/>
+      <c r="X59" s="66"/>
+    </row>
+    <row r="60" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B60" s="66"/>
-      <c r="C60" s="115" t="s">
+      <c r="C60" s="107" t="s">
         <v>2</v>
       </c>
       <c r="D60" s="33" t="s">
@@ -2480,11 +2788,38 @@
         <v>&lt;0.05</v>
       </c>
       <c r="K60" s="66"/>
-    </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="O60" s="66"/>
+      <c r="P60" s="107" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q60" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="R60" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="S60" s="35">
+        <v>1</v>
+      </c>
+      <c r="T60" s="35">
+        <v>1</v>
+      </c>
+      <c r="U60" s="35">
+        <v>6.9820000000000002</v>
+      </c>
+      <c r="V60" s="36">
+        <v>9.0399999999999994E-3</v>
+      </c>
+      <c r="W60" s="84" t="str">
+        <f t="shared" ref="W60:W65" si="4">IF(V60&lt;0.05, "&lt;0.05", IF(V60&lt;0.1, "&lt;0.1", ""))</f>
+        <v>&lt;0.05</v>
+      </c>
+      <c r="X60" s="66"/>
+    </row>
+    <row r="61" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B61" s="66"/>
-      <c r="C61" s="116"/>
-      <c r="D61" s="118" t="s">
+      <c r="C61" s="108"/>
+      <c r="D61" s="116" t="s">
         <v>5</v>
       </c>
       <c r="E61" s="29" t="s">
@@ -2507,11 +2842,36 @@
         <v>&lt;0.05</v>
       </c>
       <c r="K61" s="66"/>
-    </row>
-    <row r="62" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="O61" s="66"/>
+      <c r="P61" s="108"/>
+      <c r="Q61" s="116" t="s">
+        <v>5</v>
+      </c>
+      <c r="R61" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="S61" s="30">
+        <v>1.8480000000000001</v>
+      </c>
+      <c r="T61" s="30">
+        <v>1.8480000000000001</v>
+      </c>
+      <c r="U61" s="30">
+        <v>13.904999999999999</v>
+      </c>
+      <c r="V61" s="31">
+        <v>1.9599999999999999E-4</v>
+      </c>
+      <c r="W61" s="57" t="str">
+        <f t="shared" si="4"/>
+        <v>&lt;0.05</v>
+      </c>
+      <c r="X61" s="66"/>
+    </row>
+    <row r="62" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B62" s="66"/>
-      <c r="C62" s="116"/>
-      <c r="D62" s="119"/>
+      <c r="C62" s="108"/>
+      <c r="D62" s="115"/>
       <c r="E62" s="32" t="s">
         <v>18</v>
       </c>
@@ -2532,10 +2892,33 @@
         <v>&lt;0.1</v>
       </c>
       <c r="K62" s="66"/>
-    </row>
-    <row r="63" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="O62" s="66"/>
+      <c r="P62" s="108"/>
+      <c r="Q62" s="115"/>
+      <c r="R62" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="S62" s="27">
+        <v>1</v>
+      </c>
+      <c r="T62" s="27">
+        <v>1</v>
+      </c>
+      <c r="U62" s="27">
+        <v>3.633</v>
+      </c>
+      <c r="V62" s="28">
+        <v>5.842E-2</v>
+      </c>
+      <c r="W62" s="85" t="str">
+        <f t="shared" si="4"/>
+        <v>&lt;0.1</v>
+      </c>
+      <c r="X62" s="66"/>
+    </row>
+    <row r="63" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B63" s="66"/>
-      <c r="C63" s="116"/>
+      <c r="C63" s="108"/>
       <c r="D63" s="17" t="s">
         <v>6</v>
       </c>
@@ -2546,8 +2929,20 @@
       <c r="I63" s="42"/>
       <c r="J63" s="42"/>
       <c r="K63" s="66"/>
-    </row>
-    <row r="64" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="O63" s="66"/>
+      <c r="P63" s="108"/>
+      <c r="Q63" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="R63" s="40"/>
+      <c r="S63" s="41"/>
+      <c r="T63" s="41"/>
+      <c r="U63" s="41"/>
+      <c r="V63" s="42"/>
+      <c r="W63" s="42"/>
+      <c r="X63" s="66"/>
+    </row>
+    <row r="64" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B64" s="66"/>
       <c r="C64" s="117"/>
       <c r="D64" s="5" t="s">
@@ -2562,8 +2957,22 @@
       <c r="I64" s="91"/>
       <c r="J64" s="91"/>
       <c r="K64" s="66"/>
-    </row>
-    <row r="65" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="O64" s="66"/>
+      <c r="P64" s="117"/>
+      <c r="Q64" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="R64" s="89" t="s">
+        <v>27</v>
+      </c>
+      <c r="S64" s="90"/>
+      <c r="T64" s="90"/>
+      <c r="U64" s="90"/>
+      <c r="V64" s="91"/>
+      <c r="W64" s="91"/>
+      <c r="X64" s="66"/>
+    </row>
+    <row r="65" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B65" s="66"/>
       <c r="C65" s="66"/>
       <c r="D65" s="66"/>
@@ -2575,8 +2984,18 @@
       <c r="J65" s="66"/>
       <c r="K65" s="66"/>
       <c r="L65" s="66"/>
-    </row>
-    <row r="66" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="O65" s="66"/>
+      <c r="P65" s="66"/>
+      <c r="Q65" s="66"/>
+      <c r="R65" s="66"/>
+      <c r="S65" s="66"/>
+      <c r="T65" s="66"/>
+      <c r="U65" s="66"/>
+      <c r="V65" s="66"/>
+      <c r="W65" s="66"/>
+      <c r="X65" s="66"/>
+    </row>
+    <row r="66" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B66" s="66"/>
       <c r="C66" s="66"/>
       <c r="D66" s="66"/>
@@ -2589,7 +3008,7 @@
       <c r="K66" s="66"/>
       <c r="L66" s="66"/>
     </row>
-    <row r="68" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B68" s="66"/>
       <c r="C68" s="66" t="s">
         <v>31</v>
@@ -2601,7 +3020,7 @@
       <c r="H68" s="66"/>
       <c r="I68" s="66"/>
     </row>
-    <row r="69" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B69" s="66"/>
       <c r="C69" s="66"/>
       <c r="D69" s="66"/>
@@ -2611,7 +3030,7 @@
       <c r="H69" s="66"/>
       <c r="I69" s="66"/>
     </row>
-    <row r="70" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B70" s="66"/>
       <c r="C70" s="2" t="s">
         <v>10</v>
@@ -2629,9 +3048,9 @@
       <c r="H70" s="66"/>
       <c r="I70" s="66"/>
     </row>
-    <row r="71" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B71" s="66"/>
-      <c r="C71" s="109" t="s">
+      <c r="C71" s="114" t="s">
         <v>0</v>
       </c>
       <c r="D71" t="s">
@@ -2649,9 +3068,9 @@
       <c r="H71" s="66"/>
       <c r="I71" s="66"/>
     </row>
-    <row r="72" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B72" s="66"/>
-      <c r="C72" s="110"/>
+      <c r="C72" s="113"/>
       <c r="D72" s="20" t="s">
         <v>28</v>
       </c>
@@ -2667,12 +3086,12 @@
       <c r="H72" s="66"/>
       <c r="I72" s="66"/>
     </row>
-    <row r="73" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B73" s="66"/>
-      <c r="C73" s="106" t="s">
-        <v>1</v>
-      </c>
-      <c r="D73" s="106" t="s">
+      <c r="C73" s="110" t="s">
+        <v>1</v>
+      </c>
+      <c r="D73" s="110" t="s">
         <v>21</v>
       </c>
       <c r="E73" s="52" t="s">
@@ -2687,7 +3106,7 @@
       <c r="H73" s="66"/>
       <c r="I73" s="66"/>
     </row>
-    <row r="74" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B74" s="66"/>
       <c r="C74" s="104"/>
       <c r="D74" s="111"/>
@@ -2703,10 +3122,10 @@
       <c r="H74" s="66"/>
       <c r="I74" s="66"/>
     </row>
-    <row r="75" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B75" s="66"/>
       <c r="C75" s="104"/>
-      <c r="D75" s="114" t="s">
+      <c r="D75" s="112" t="s">
         <v>28</v>
       </c>
       <c r="E75" s="57" t="s">
@@ -2721,7 +3140,7 @@
       <c r="H75" s="66"/>
       <c r="I75" s="66"/>
     </row>
-    <row r="76" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B76" s="66"/>
       <c r="C76" s="104"/>
       <c r="D76" s="105"/>
@@ -2737,9 +3156,9 @@
       <c r="H76" s="66"/>
       <c r="I76" s="66"/>
     </row>
-    <row r="77" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B77" s="66"/>
-      <c r="C77" s="112" t="s">
+      <c r="C77" s="119" t="s">
         <v>2</v>
       </c>
       <c r="D77" s="63" t="s">
@@ -2757,9 +3176,9 @@
       <c r="H77" s="66"/>
       <c r="I77" s="66"/>
     </row>
-    <row r="78" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B78" s="66"/>
-      <c r="C78" s="113"/>
+      <c r="C78" s="120"/>
       <c r="D78" s="65" t="s">
         <v>28</v>
       </c>
@@ -2775,19 +3194,19 @@
       <c r="H78" s="66"/>
       <c r="I78" s="66"/>
     </row>
-    <row r="79" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B79" s="66"/>
       <c r="C79" s="61"/>
-      <c r="D79" s="120"/>
-      <c r="E79" s="120"/>
-      <c r="F79" s="120"/>
-      <c r="G79" s="120"/>
-      <c r="H79" s="120"/>
-      <c r="I79" s="120"/>
-      <c r="J79" s="120"/>
+      <c r="D79" s="118"/>
+      <c r="E79" s="118"/>
+      <c r="F79" s="118"/>
+      <c r="G79" s="118"/>
+      <c r="H79" s="118"/>
+      <c r="I79" s="118"/>
+      <c r="J79" s="118"/>
       <c r="K79" s="66"/>
     </row>
-    <row r="80" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B80" s="66"/>
       <c r="C80" s="61"/>
       <c r="D80" s="18"/>
@@ -2853,7 +3272,7 @@
     </row>
     <row r="88" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B88" s="66"/>
-      <c r="C88" s="109" t="s">
+      <c r="C88" s="114" t="s">
         <v>0</v>
       </c>
       <c r="D88" t="s">
@@ -2873,7 +3292,7 @@
     </row>
     <row r="89" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B89" s="66"/>
-      <c r="C89" s="110"/>
+      <c r="C89" s="113"/>
       <c r="D89" s="20" t="s">
         <v>28</v>
       </c>
@@ -2891,10 +3310,10 @@
     </row>
     <row r="90" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B90" s="66"/>
-      <c r="C90" s="106" t="s">
-        <v>1</v>
-      </c>
-      <c r="D90" s="106" t="s">
+      <c r="C90" s="110" t="s">
+        <v>1</v>
+      </c>
+      <c r="D90" s="110" t="s">
         <v>21</v>
       </c>
       <c r="E90" s="29" t="s">
@@ -2928,7 +3347,7 @@
     <row r="92" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B92" s="66"/>
       <c r="C92" s="104"/>
-      <c r="D92" s="114" t="s">
+      <c r="D92" s="112" t="s">
         <v>28</v>
       </c>
       <c r="E92" s="29" t="s">
@@ -2961,7 +3380,7 @@
     </row>
     <row r="94" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B94" s="66"/>
-      <c r="C94" s="106" t="s">
+      <c r="C94" s="110" t="s">
         <v>2</v>
       </c>
       <c r="D94" s="63" t="s">
@@ -3056,7 +3475,7 @@
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B102" s="66"/>
-      <c r="C102" s="109" t="s">
+      <c r="C102" s="114" t="s">
         <v>0</v>
       </c>
       <c r="D102" t="s">
@@ -3076,7 +3495,7 @@
     </row>
     <row r="103" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B103" s="66"/>
-      <c r="C103" s="110"/>
+      <c r="C103" s="113"/>
       <c r="D103" s="20" t="s">
         <v>28</v>
       </c>
@@ -3094,7 +3513,7 @@
     </row>
     <row r="104" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B104" s="66"/>
-      <c r="C104" s="106" t="s">
+      <c r="C104" s="110" t="s">
         <v>1</v>
       </c>
       <c r="D104" s="16" t="s">
@@ -3132,7 +3551,7 @@
     </row>
     <row r="106" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B106" s="66"/>
-      <c r="C106" s="106" t="s">
+      <c r="C106" s="110" t="s">
         <v>2</v>
       </c>
       <c r="D106" s="63" t="s">
@@ -3235,7 +3654,7 @@
       <c r="C115" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D115" s="107" t="s">
+      <c r="D115" s="121" t="s">
         <v>21</v>
       </c>
       <c r="E115" s="76" t="s">
@@ -3252,7 +3671,7 @@
     <row r="116" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B116" s="66"/>
       <c r="C116" s="37"/>
-      <c r="D116" s="108"/>
+      <c r="D116" s="122"/>
       <c r="E116" s="80" t="s">
         <v>20</v>
       </c>
@@ -3344,24 +3763,23 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="C27:I27"/>
-    <mergeCell ref="C6:C14"/>
-    <mergeCell ref="C15:C18"/>
-    <mergeCell ref="C19:C22"/>
-    <mergeCell ref="D6:D10"/>
-    <mergeCell ref="D26:J26"/>
-    <mergeCell ref="C40:C43"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="C29:C33"/>
-    <mergeCell ref="C34:C39"/>
-    <mergeCell ref="D47:J47"/>
-    <mergeCell ref="C50:C53"/>
-    <mergeCell ref="C54:C59"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="D56:D57"/>
+  <mergeCells count="41">
+    <mergeCell ref="Q47:W47"/>
+    <mergeCell ref="P50:P53"/>
+    <mergeCell ref="P54:P59"/>
+    <mergeCell ref="Q54:Q55"/>
+    <mergeCell ref="Q56:Q57"/>
+    <mergeCell ref="P60:P64"/>
+    <mergeCell ref="Q61:Q62"/>
+    <mergeCell ref="D115:D116"/>
+    <mergeCell ref="C94:C96"/>
+    <mergeCell ref="C102:C103"/>
+    <mergeCell ref="C104:C105"/>
+    <mergeCell ref="C88:C89"/>
+    <mergeCell ref="C90:C93"/>
+    <mergeCell ref="D90:D91"/>
+    <mergeCell ref="D92:D93"/>
+    <mergeCell ref="C106:C107"/>
     <mergeCell ref="C60:C64"/>
     <mergeCell ref="D61:D62"/>
     <mergeCell ref="D79:J79"/>
@@ -3370,15 +3788,23 @@
     <mergeCell ref="D75:D76"/>
     <mergeCell ref="D73:D74"/>
     <mergeCell ref="C77:C78"/>
-    <mergeCell ref="C88:C89"/>
-    <mergeCell ref="C90:C93"/>
-    <mergeCell ref="D90:D91"/>
-    <mergeCell ref="D92:D93"/>
-    <mergeCell ref="C106:C107"/>
-    <mergeCell ref="D115:D116"/>
-    <mergeCell ref="C94:C96"/>
-    <mergeCell ref="C102:C103"/>
-    <mergeCell ref="C104:C105"/>
+    <mergeCell ref="D47:J47"/>
+    <mergeCell ref="C50:C53"/>
+    <mergeCell ref="C54:C59"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="C40:C43"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="C29:C33"/>
+    <mergeCell ref="C34:C39"/>
+    <mergeCell ref="C27:I27"/>
+    <mergeCell ref="C6:C14"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="C19:C22"/>
+    <mergeCell ref="D6:D10"/>
+    <mergeCell ref="D26:J26"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="J6:J22">
@@ -3392,6 +3818,987 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11EC7562-B833-6E47-893A-48CC2F5000AD}">
+  <dimension ref="C6:K53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="88" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C6" s="66"/>
+      <c r="D6" s="109" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="109"/>
+      <c r="F6" s="109"/>
+      <c r="G6" s="109"/>
+      <c r="H6" s="109"/>
+      <c r="I6" s="109"/>
+      <c r="J6" s="109"/>
+      <c r="K6" s="66"/>
+    </row>
+    <row r="7" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="66"/>
+      <c r="I7" s="66"/>
+      <c r="J7" s="66"/>
+      <c r="K7" s="66"/>
+    </row>
+    <row r="8" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="2"/>
+      <c r="K8" s="66"/>
+    </row>
+    <row r="9" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C9" s="114" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="110" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="35">
+        <v>1</v>
+      </c>
+      <c r="G9" s="35">
+        <v>1</v>
+      </c>
+      <c r="H9" s="35">
+        <v>5.0339999999999998</v>
+      </c>
+      <c r="I9" s="36">
+        <v>2.63E-2</v>
+      </c>
+      <c r="J9" s="84" t="s">
+        <v>29</v>
+      </c>
+      <c r="K9" s="66"/>
+    </row>
+    <row r="10" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C10" s="123"/>
+      <c r="D10" s="111"/>
+      <c r="E10" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="35">
+        <v>5.0149999999999997</v>
+      </c>
+      <c r="G10" s="35">
+        <v>5.0149999999999997</v>
+      </c>
+      <c r="H10" s="35">
+        <v>3.165</v>
+      </c>
+      <c r="I10" s="36">
+        <v>1.12E-2</v>
+      </c>
+      <c r="J10" s="84" t="s">
+        <v>29</v>
+      </c>
+      <c r="K10" s="66"/>
+    </row>
+    <row r="11" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C11" s="123"/>
+      <c r="D11" s="112" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="35">
+        <v>1</v>
+      </c>
+      <c r="G11" s="35">
+        <v>1</v>
+      </c>
+      <c r="H11" s="35">
+        <v>4.6680000000000001</v>
+      </c>
+      <c r="I11" s="36">
+        <v>3.2199999999999999E-2</v>
+      </c>
+      <c r="J11" s="84" t="s">
+        <v>29</v>
+      </c>
+      <c r="K11" s="66"/>
+    </row>
+    <row r="12" spans="3:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C12" s="113"/>
+      <c r="D12" s="111"/>
+      <c r="E12" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="35">
+        <v>4.3049999999999997</v>
+      </c>
+      <c r="G12" s="35">
+        <v>4.3049999999999997</v>
+      </c>
+      <c r="H12" s="35">
+        <v>1.7689999999999999</v>
+      </c>
+      <c r="I12" s="36">
+        <v>9.9299999999999999E-2</v>
+      </c>
+      <c r="J12" s="84" t="s">
+        <v>30</v>
+      </c>
+      <c r="K12" s="66"/>
+    </row>
+    <row r="13" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C13" s="113"/>
+      <c r="D13" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="35">
+        <v>1</v>
+      </c>
+      <c r="G13" s="35">
+        <v>1</v>
+      </c>
+      <c r="H13" s="35">
+        <v>8.7590000000000003</v>
+      </c>
+      <c r="I13" s="36">
+        <v>3.5899999999999999E-3</v>
+      </c>
+      <c r="J13" s="84" t="s">
+        <v>29</v>
+      </c>
+      <c r="K13" s="66"/>
+    </row>
+    <row r="14" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="113"/>
+      <c r="D14" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="46"/>
+      <c r="J14" s="88"/>
+      <c r="K14" s="66"/>
+    </row>
+    <row r="15" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C15" s="110" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="114" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="23">
+        <v>1</v>
+      </c>
+      <c r="G15" s="23">
+        <v>1</v>
+      </c>
+      <c r="H15" s="23">
+        <v>5.9320000000000004</v>
+      </c>
+      <c r="I15" s="24">
+        <v>1.5991999999999999E-2</v>
+      </c>
+      <c r="J15" s="63" t="s">
+        <v>29</v>
+      </c>
+      <c r="K15" s="66"/>
+    </row>
+    <row r="16" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="104"/>
+      <c r="D16" s="115"/>
+      <c r="E16" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="27">
+        <v>3.6259999999999999</v>
+      </c>
+      <c r="G16" s="27">
+        <v>3.6259999999999999</v>
+      </c>
+      <c r="H16" s="27">
+        <v>7.492</v>
+      </c>
+      <c r="I16" s="28">
+        <v>1.84E-4</v>
+      </c>
+      <c r="J16" s="85" t="s">
+        <v>29</v>
+      </c>
+      <c r="K16" s="66"/>
+    </row>
+    <row r="17" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C17" s="104"/>
+      <c r="D17" s="116" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="30">
+        <v>1</v>
+      </c>
+      <c r="G17" s="30">
+        <v>1</v>
+      </c>
+      <c r="H17" s="30">
+        <v>5.9649999999999999</v>
+      </c>
+      <c r="I17" s="24">
+        <v>1.5706000000000001E-2</v>
+      </c>
+      <c r="J17" s="63" t="s">
+        <v>29</v>
+      </c>
+      <c r="K17" s="66"/>
+    </row>
+    <row r="18" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C18" s="104"/>
+      <c r="D18" s="115"/>
+      <c r="E18" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="27">
+        <v>3.6829999999999998</v>
+      </c>
+      <c r="G18" s="27">
+        <v>3.6829999999999998</v>
+      </c>
+      <c r="H18" s="27">
+        <v>6.6989999999999998</v>
+      </c>
+      <c r="I18" s="28">
+        <v>5.5900000000000004E-4</v>
+      </c>
+      <c r="J18" s="85" t="s">
+        <v>29</v>
+      </c>
+      <c r="K18" s="66"/>
+    </row>
+    <row r="19" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C19" s="104"/>
+      <c r="D19" s="112" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="27">
+        <v>2.0539999999999998</v>
+      </c>
+      <c r="G19" s="27">
+        <v>2.0550000000000002</v>
+      </c>
+      <c r="H19" s="27">
+        <v>5.3840000000000003</v>
+      </c>
+      <c r="I19" s="28">
+        <v>5.3699999999999998E-3</v>
+      </c>
+      <c r="J19" s="85" t="s">
+        <v>29</v>
+      </c>
+      <c r="K19" s="66"/>
+    </row>
+    <row r="20" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C20" s="104"/>
+      <c r="D20" s="124"/>
+      <c r="E20" s="125" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="35">
+        <v>1</v>
+      </c>
+      <c r="G20" s="35">
+        <v>1</v>
+      </c>
+      <c r="H20" s="35">
+        <v>3.15</v>
+      </c>
+      <c r="I20" s="36">
+        <v>7.7990000000000004E-2</v>
+      </c>
+      <c r="J20" s="84" t="s">
+        <v>30</v>
+      </c>
+      <c r="K20" s="66"/>
+    </row>
+    <row r="21" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="105"/>
+      <c r="D21" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" s="45"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="45"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="88"/>
+      <c r="K21" s="66"/>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C22" s="110" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="110" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="35">
+        <v>1</v>
+      </c>
+      <c r="G22" s="35">
+        <v>1</v>
+      </c>
+      <c r="H22" s="35">
+        <v>3.472</v>
+      </c>
+      <c r="I22" s="36">
+        <v>6.4299999999999996E-2</v>
+      </c>
+      <c r="J22" s="84" t="s">
+        <v>30</v>
+      </c>
+      <c r="K22" s="66"/>
+    </row>
+    <row r="23" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C23" s="124"/>
+      <c r="D23" s="124"/>
+      <c r="E23" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="30">
+        <v>1.5589999999999999</v>
+      </c>
+      <c r="G23" s="30">
+        <v>1.5589999999999999</v>
+      </c>
+      <c r="H23" s="30">
+        <v>8.6859999999999999</v>
+      </c>
+      <c r="I23" s="31">
+        <v>9.4000000000000004E-3</v>
+      </c>
+      <c r="J23" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="K23" s="66"/>
+    </row>
+    <row r="24" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C24" s="124"/>
+      <c r="D24" s="111"/>
+      <c r="E24" s="126" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="30">
+        <v>1.994</v>
+      </c>
+      <c r="G24" s="30">
+        <v>1.994</v>
+      </c>
+      <c r="H24" s="30">
+        <v>3.3679999999999999</v>
+      </c>
+      <c r="I24" s="31">
+        <v>4.4299999999999999E-2</v>
+      </c>
+      <c r="J24" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="K24" s="66"/>
+    </row>
+    <row r="25" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C25" s="124"/>
+      <c r="D25" s="116" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="126" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="30">
+        <v>3.077</v>
+      </c>
+      <c r="G25" s="30">
+        <v>3.077</v>
+      </c>
+      <c r="H25" s="30">
+        <v>2.98</v>
+      </c>
+      <c r="I25" s="31">
+        <v>2.63E-2</v>
+      </c>
+      <c r="J25" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="K25" s="66"/>
+    </row>
+    <row r="26" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C26" s="104"/>
+      <c r="D26" s="123"/>
+      <c r="E26" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" s="30">
+        <v>2.097</v>
+      </c>
+      <c r="G26" s="30">
+        <v>2.097</v>
+      </c>
+      <c r="H26" s="30">
+        <v>16.018999999999998</v>
+      </c>
+      <c r="I26" s="130">
+        <v>6.0500000000000003E-7</v>
+      </c>
+      <c r="J26" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="K26" s="66"/>
+    </row>
+    <row r="27" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C27" s="104"/>
+      <c r="D27" s="123"/>
+      <c r="E27" s="125" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" s="127">
+        <v>1</v>
+      </c>
+      <c r="G27" s="127">
+        <v>1</v>
+      </c>
+      <c r="H27" s="127">
+        <v>5.4089999999999998</v>
+      </c>
+      <c r="I27" s="128">
+        <v>2.1299999999999999E-2</v>
+      </c>
+      <c r="J27" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="K27" s="66"/>
+    </row>
+    <row r="28" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C28" s="104"/>
+      <c r="D28" s="115"/>
+      <c r="E28" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28" s="27">
+        <v>1.9139999999999999</v>
+      </c>
+      <c r="G28" s="27">
+        <v>1.9139999999999999</v>
+      </c>
+      <c r="H28" s="27">
+        <v>3.6850000000000001</v>
+      </c>
+      <c r="I28" s="28">
+        <v>6.0499999999999998E-2</v>
+      </c>
+      <c r="J28" s="85" t="s">
+        <v>30</v>
+      </c>
+      <c r="K28" s="66"/>
+    </row>
+    <row r="29" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C29" s="104"/>
+      <c r="D29" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="40"/>
+      <c r="F29" s="41"/>
+      <c r="G29" s="41"/>
+      <c r="H29" s="41"/>
+      <c r="I29" s="42"/>
+      <c r="J29" s="42"/>
+      <c r="K29" s="66"/>
+    </row>
+    <row r="30" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C30" s="105"/>
+      <c r="D30" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" s="89" t="s">
+        <v>27</v>
+      </c>
+      <c r="F30" s="90"/>
+      <c r="G30" s="90"/>
+      <c r="H30" s="90"/>
+      <c r="I30" s="91"/>
+      <c r="J30" s="91"/>
+      <c r="K30" s="66"/>
+    </row>
+    <row r="31" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C31" s="66"/>
+      <c r="D31" s="66"/>
+      <c r="E31" s="66"/>
+      <c r="F31" s="66"/>
+      <c r="G31" s="66"/>
+      <c r="H31" s="66"/>
+      <c r="I31" s="66"/>
+      <c r="J31" s="66"/>
+      <c r="K31" s="66"/>
+    </row>
+    <row r="35" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C35" s="66"/>
+      <c r="D35" s="109" t="s">
+        <v>50</v>
+      </c>
+      <c r="E35" s="109"/>
+      <c r="F35" s="109"/>
+      <c r="G35" s="109"/>
+      <c r="H35" s="109"/>
+      <c r="I35" s="109"/>
+      <c r="J35" s="109"/>
+      <c r="K35" s="66"/>
+    </row>
+    <row r="36" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C36" s="66"/>
+      <c r="D36" s="66"/>
+      <c r="E36" s="66"/>
+      <c r="F36" s="66"/>
+      <c r="G36" s="66"/>
+      <c r="H36" s="66"/>
+      <c r="I36" s="66"/>
+      <c r="J36" s="66"/>
+      <c r="K36" s="66"/>
+    </row>
+    <row r="37" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C37" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J37" s="2"/>
+      <c r="K37" s="66"/>
+    </row>
+    <row r="38" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C38" s="114" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38" s="112" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" s="132" t="s">
+        <v>17</v>
+      </c>
+      <c r="F38" s="127">
+        <v>1</v>
+      </c>
+      <c r="G38" s="127">
+        <v>1</v>
+      </c>
+      <c r="H38" s="127">
+        <v>4.6680000000000001</v>
+      </c>
+      <c r="I38" s="128">
+        <v>3.2199999999999999E-2</v>
+      </c>
+      <c r="J38" s="129" t="s">
+        <v>29</v>
+      </c>
+      <c r="K38" s="66"/>
+    </row>
+    <row r="39" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C39" s="123"/>
+      <c r="D39" s="111"/>
+      <c r="E39" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="F39" s="27">
+        <v>4.3049999999999997</v>
+      </c>
+      <c r="G39" s="27">
+        <v>4.3049999999999997</v>
+      </c>
+      <c r="H39" s="27">
+        <v>1.7689999999999999</v>
+      </c>
+      <c r="I39" s="28">
+        <v>9.9299999999999999E-2</v>
+      </c>
+      <c r="J39" s="85" t="s">
+        <v>30</v>
+      </c>
+      <c r="K39" s="66"/>
+    </row>
+    <row r="40" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C40" s="123"/>
+      <c r="D40" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="F40" s="35">
+        <v>1</v>
+      </c>
+      <c r="G40" s="35">
+        <v>1</v>
+      </c>
+      <c r="H40" s="35">
+        <v>8.7590000000000003</v>
+      </c>
+      <c r="I40" s="36">
+        <v>3.5899999999999999E-3</v>
+      </c>
+      <c r="J40" s="84" t="s">
+        <v>29</v>
+      </c>
+      <c r="K40" s="66"/>
+    </row>
+    <row r="41" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C41" s="131"/>
+      <c r="D41" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E41" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="F41" s="45"/>
+      <c r="G41" s="45"/>
+      <c r="H41" s="45"/>
+      <c r="I41" s="46"/>
+      <c r="J41" s="88"/>
+      <c r="K41" s="66"/>
+    </row>
+    <row r="42" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C42" s="114" t="s">
+        <v>1</v>
+      </c>
+      <c r="D42" s="116" t="s">
+        <v>5</v>
+      </c>
+      <c r="E42" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F42" s="30">
+        <v>1</v>
+      </c>
+      <c r="G42" s="30">
+        <v>1</v>
+      </c>
+      <c r="H42" s="30">
+        <v>5.9649999999999999</v>
+      </c>
+      <c r="I42" s="24">
+        <v>1.5706000000000001E-2</v>
+      </c>
+      <c r="J42" s="63" t="s">
+        <v>29</v>
+      </c>
+      <c r="K42" s="66"/>
+    </row>
+    <row r="43" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C43" s="123"/>
+      <c r="D43" s="115"/>
+      <c r="E43" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="F43" s="27">
+        <v>3.6829999999999998</v>
+      </c>
+      <c r="G43" s="27">
+        <v>3.6829999999999998</v>
+      </c>
+      <c r="H43" s="27">
+        <v>6.6989999999999998</v>
+      </c>
+      <c r="I43" s="28">
+        <v>5.5900000000000004E-4</v>
+      </c>
+      <c r="J43" s="85" t="s">
+        <v>29</v>
+      </c>
+      <c r="K43" s="66"/>
+    </row>
+    <row r="44" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C44" s="123"/>
+      <c r="D44" s="112" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="F44" s="27">
+        <v>2.0539999999999998</v>
+      </c>
+      <c r="G44" s="27">
+        <v>2.0550000000000002</v>
+      </c>
+      <c r="H44" s="27">
+        <v>5.3840000000000003</v>
+      </c>
+      <c r="I44" s="28">
+        <v>5.3699999999999998E-3</v>
+      </c>
+      <c r="J44" s="85" t="s">
+        <v>29</v>
+      </c>
+      <c r="K44" s="66"/>
+    </row>
+    <row r="45" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C45" s="123"/>
+      <c r="D45" s="124"/>
+      <c r="E45" s="125" t="s">
+        <v>18</v>
+      </c>
+      <c r="F45" s="35">
+        <v>1</v>
+      </c>
+      <c r="G45" s="35">
+        <v>1</v>
+      </c>
+      <c r="H45" s="35">
+        <v>3.15</v>
+      </c>
+      <c r="I45" s="36">
+        <v>7.7990000000000004E-2</v>
+      </c>
+      <c r="J45" s="84" t="s">
+        <v>30</v>
+      </c>
+      <c r="K45" s="66"/>
+    </row>
+    <row r="46" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C46" s="131"/>
+      <c r="D46" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E46" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="F46" s="45"/>
+      <c r="G46" s="45"/>
+      <c r="H46" s="45"/>
+      <c r="I46" s="46"/>
+      <c r="J46" s="88"/>
+      <c r="K46" s="66"/>
+    </row>
+    <row r="47" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C47" s="114" t="s">
+        <v>2</v>
+      </c>
+      <c r="D47" s="116" t="s">
+        <v>5</v>
+      </c>
+      <c r="E47" s="126" t="s">
+        <v>16</v>
+      </c>
+      <c r="F47" s="30">
+        <v>3.077</v>
+      </c>
+      <c r="G47" s="30">
+        <v>3.077</v>
+      </c>
+      <c r="H47" s="30">
+        <v>2.98</v>
+      </c>
+      <c r="I47" s="31">
+        <v>2.63E-2</v>
+      </c>
+      <c r="J47" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="K47" s="66"/>
+    </row>
+    <row r="48" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C48" s="123"/>
+      <c r="D48" s="123"/>
+      <c r="E48" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F48" s="30">
+        <v>2.097</v>
+      </c>
+      <c r="G48" s="30">
+        <v>2.097</v>
+      </c>
+      <c r="H48" s="30">
+        <v>16.018999999999998</v>
+      </c>
+      <c r="I48" s="130">
+        <v>6.0500000000000003E-7</v>
+      </c>
+      <c r="J48" s="133" t="s">
+        <v>29</v>
+      </c>
+      <c r="K48" s="66"/>
+    </row>
+    <row r="49" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C49" s="123"/>
+      <c r="D49" s="123"/>
+      <c r="E49" s="125" t="s">
+        <v>18</v>
+      </c>
+      <c r="F49" s="127">
+        <v>1</v>
+      </c>
+      <c r="G49" s="127">
+        <v>1</v>
+      </c>
+      <c r="H49" s="127">
+        <v>5.4089999999999998</v>
+      </c>
+      <c r="I49" s="128">
+        <v>2.1299999999999999E-2</v>
+      </c>
+      <c r="J49" s="129" t="s">
+        <v>29</v>
+      </c>
+      <c r="K49" s="66"/>
+    </row>
+    <row r="50" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C50" s="123"/>
+      <c r="D50" s="115"/>
+      <c r="E50" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="F50" s="27">
+        <v>1.9139999999999999</v>
+      </c>
+      <c r="G50" s="27">
+        <v>1.9139999999999999</v>
+      </c>
+      <c r="H50" s="27">
+        <v>3.6850000000000001</v>
+      </c>
+      <c r="I50" s="28">
+        <v>6.0499999999999998E-2</v>
+      </c>
+      <c r="J50" s="85" t="s">
+        <v>30</v>
+      </c>
+      <c r="K50" s="66"/>
+    </row>
+    <row r="51" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C51" s="123"/>
+      <c r="D51" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E51" s="40"/>
+      <c r="F51" s="41"/>
+      <c r="G51" s="41"/>
+      <c r="H51" s="41"/>
+      <c r="I51" s="42"/>
+      <c r="J51" s="42"/>
+      <c r="K51" s="66"/>
+    </row>
+    <row r="52" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C52" s="131"/>
+      <c r="D52" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E52" s="89" t="s">
+        <v>27</v>
+      </c>
+      <c r="F52" s="90"/>
+      <c r="G52" s="90"/>
+      <c r="H52" s="90"/>
+      <c r="I52" s="91"/>
+      <c r="J52" s="91"/>
+      <c r="K52" s="66"/>
+    </row>
+    <row r="53" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C53" s="66"/>
+      <c r="D53" s="66"/>
+      <c r="E53" s="66"/>
+      <c r="F53" s="66"/>
+      <c r="G53" s="66"/>
+      <c r="H53" s="66"/>
+      <c r="I53" s="66"/>
+      <c r="J53" s="66"/>
+      <c r="K53" s="66"/>
+    </row>
+  </sheetData>
+  <mergeCells count="19">
+    <mergeCell ref="C38:C41"/>
+    <mergeCell ref="C42:C46"/>
+    <mergeCell ref="C47:C52"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="D47:D50"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="D25:D28"/>
+    <mergeCell ref="D35:J35"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="D6:J6"/>
+    <mergeCell ref="C9:C14"/>
+    <mergeCell ref="C15:C21"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="C22:C30"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D19:D20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8F6DB0D-2B41-A146-8989-239E41193B1F}">
   <dimension ref="B1:M53"/>
   <sheetViews>
@@ -3445,7 +4852,7 @@
     <row r="4" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C4" s="66"/>
       <c r="D4" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>3</v>
@@ -3472,7 +4879,7 @@
     <row r="5" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C5" s="66"/>
       <c r="D5" s="104" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>4</v>
@@ -3540,7 +4947,7 @@
     <row r="9" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C9" s="66"/>
       <c r="D9" s="104" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>4</v>
@@ -3602,7 +5009,7 @@
     <row r="13" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C13" s="66"/>
       <c r="D13" s="104" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>4</v>
@@ -3664,7 +5071,7 @@
     <row r="17" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C17" s="66"/>
       <c r="D17" s="104" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>4</v>
@@ -3739,7 +5146,7 @@
     <row r="22" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C22" s="66"/>
       <c r="D22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K22" s="66"/>
       <c r="L22" s="66"/>
@@ -3761,7 +5168,7 @@
     <row r="24" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C24" s="66"/>
       <c r="D24" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E24" s="94" t="s">
         <v>7</v>
@@ -3776,10 +5183,10 @@
         <v>9</v>
       </c>
       <c r="I24" s="94" t="s">
+        <v>42</v>
+      </c>
+      <c r="J24" s="94" t="s">
         <v>43</v>
-      </c>
-      <c r="J24" s="94" t="s">
-        <v>44</v>
       </c>
       <c r="K24" s="66"/>
       <c r="L24" s="66"/>
@@ -3788,7 +5195,7 @@
     <row r="25" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C25" s="66"/>
       <c r="D25" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E25" s="10">
         <v>2.7719999999999998</v>
@@ -3815,7 +5222,7 @@
     <row r="26" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C26" s="66"/>
       <c r="D26" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E26" s="10">
         <v>1</v>
@@ -3842,7 +5249,7 @@
     <row r="27" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C27" s="66"/>
       <c r="D27" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E27" s="10">
         <v>1</v>
@@ -3867,7 +5274,7 @@
     <row r="28" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C28" s="66"/>
       <c r="D28" s="37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E28" s="11">
         <v>5.5380000000000003</v>
@@ -3926,7 +5333,7 @@
     <row r="32" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C32" s="66"/>
       <c r="D32" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E32" s="94" t="s">
         <v>7</v>
@@ -3941,17 +5348,17 @@
         <v>9</v>
       </c>
       <c r="I32" s="94" t="s">
+        <v>42</v>
+      </c>
+      <c r="J32" s="98" t="s">
         <v>43</v>
-      </c>
-      <c r="J32" s="98" t="s">
-        <v>44</v>
       </c>
       <c r="K32" s="92"/>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C33" s="66"/>
       <c r="D33" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E33" s="10">
         <v>3.81</v>
@@ -3976,7 +5383,7 @@
     <row r="34" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C34" s="66"/>
       <c r="D34" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E34" s="10">
         <v>1</v>
@@ -4001,7 +5408,7 @@
     <row r="35" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C35" s="66"/>
       <c r="D35" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E35" s="10">
         <v>1</v>
@@ -4026,7 +5433,7 @@
     <row r="36" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C36" s="66"/>
       <c r="D36" s="37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E36" s="11">
         <v>3.101</v>
@@ -4064,7 +5471,7 @@
       <c r="D38" s="17"/>
       <c r="E38" s="10"/>
       <c r="F38" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G38" s="10"/>
       <c r="H38" s="12"/>
@@ -4087,7 +5494,7 @@
     <row r="40" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C40" s="66"/>
       <c r="D40" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E40" s="94" t="s">
         <v>7</v>
@@ -4102,17 +5509,17 @@
         <v>9</v>
       </c>
       <c r="I40" s="94" t="s">
+        <v>42</v>
+      </c>
+      <c r="J40" s="98" t="s">
         <v>43</v>
-      </c>
-      <c r="J40" s="98" t="s">
-        <v>44</v>
       </c>
       <c r="K40" s="92"/>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C41" s="66"/>
       <c r="D41" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E41" s="10">
         <v>3.8519999999999999</v>
@@ -4137,7 +5544,7 @@
     <row r="42" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C42" s="66"/>
       <c r="D42" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E42" s="10">
         <v>1.704</v>
@@ -4162,7 +5569,7 @@
     <row r="43" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C43" s="66"/>
       <c r="D43" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E43" s="10">
         <v>1.258</v>
@@ -4187,7 +5594,7 @@
     <row r="44" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C44" s="66"/>
       <c r="D44" s="37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E44" s="11">
         <v>1.8839999999999999</v>
@@ -4225,7 +5632,7 @@
       <c r="D46" s="17"/>
       <c r="E46" s="10"/>
       <c r="F46" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G46" s="10"/>
       <c r="H46" s="12"/>
@@ -4247,7 +5654,7 @@
     <row r="48" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C48" s="66"/>
       <c r="D48" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E48" s="94" t="s">
         <v>7</v>
@@ -4262,17 +5669,17 @@
         <v>9</v>
       </c>
       <c r="I48" s="94" t="s">
+        <v>42</v>
+      </c>
+      <c r="J48" s="98" t="s">
         <v>43</v>
-      </c>
-      <c r="J48" s="98" t="s">
-        <v>44</v>
       </c>
       <c r="K48" s="92"/>
     </row>
     <row r="49" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C49" s="66"/>
       <c r="D49" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E49" s="10">
         <v>1</v>
@@ -4297,7 +5704,7 @@
     <row r="50" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C50" s="66"/>
       <c r="D50" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E50" s="10">
         <v>1</v>
@@ -4322,7 +5729,7 @@
     <row r="51" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C51" s="66"/>
       <c r="D51" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E51" s="10">
         <v>1.76</v>
@@ -4347,7 +5754,7 @@
     <row r="52" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C52" s="66"/>
       <c r="D52" s="37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E52" s="11">
         <v>1.8240000000000001</v>

</xml_diff>

<commit_message>
Updating the heat maps plots and gams results
</commit_message>
<xml_diff>
--- a/K4S_key_scripts/K4S_DA_Aims/K4S_DA_A2/K4S_DA_A2/K4S_DA_A2_GAM_Temporal_Results.xlsx
+++ b/K4S_key_scripts/K4S_DA_Aims/K4S_DA_A2/K4S_DA_A2/K4S_DA_A2_GAM_Temporal_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoestarkey/Desktop/Honours/Data_Analysis/K_axis_midoc/K4S_key_scripts/K4S_DA_Aims/K4S_DA_A2/K4S_DA_A2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9037F72-2DE6-6849-8957-AD33B46C82E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D0CBF2-1D20-B041-AEBA-5C259C60B76F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5600" yWindow="880" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{33E5A15D-DBA6-5B40-873E-91FBDBF28531}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="38400" windowHeight="19400" activeTab="2" xr2:uid="{33E5A15D-DBA6-5B40-873E-91FBDBF28531}"/>
   </bookViews>
   <sheets>
     <sheet name="GAM_Temporal_Sum" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="58">
   <si>
     <t>Season</t>
   </si>
@@ -159,9 +159,6 @@
     <t xml:space="preserve">Time since melt </t>
   </si>
   <si>
-    <t>Chlorophyll</t>
-  </si>
-  <si>
     <t>Curent speed</t>
   </si>
   <si>
@@ -206,6 +203,30 @@
   <si>
     <t>After  Refit GAMM + RE SUMMARY</t>
   </si>
+  <si>
+    <t xml:space="preserve">ALL DEPTHS SATELLITE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upper 200  SATELLITE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALL DEPTHS  IN SITU </t>
+  </si>
+  <si>
+    <t>In situ Factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temp min </t>
+  </si>
+  <si>
+    <t>Oxygen min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seasonal mixed layer </t>
+  </si>
+  <si>
+    <t>Salinity Max</t>
+  </si>
 </sst>
 </file>
 
@@ -215,7 +236,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -251,6 +272,12 @@
     <font>
       <i/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
@@ -404,7 +431,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -677,92 +704,89 @@
     <xf numFmtId="165" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1190,7 +1214,7 @@
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="104" t="s">
+      <c r="B5" s="107" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -1214,7 +1238,7 @@
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="104"/>
+      <c r="B6" s="107"/>
       <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
@@ -1236,7 +1260,7 @@
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="104"/>
+      <c r="B7" s="107"/>
       <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1258,7 +1282,7 @@
       </c>
     </row>
     <row r="8" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="105"/>
+      <c r="B8" s="108"/>
       <c r="C8" s="5" t="s">
         <v>12</v>
       </c>
@@ -1280,7 +1304,7 @@
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="104" t="s">
+      <c r="B9" s="107" t="s">
         <v>1</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -1304,7 +1328,7 @@
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="104"/>
+      <c r="B10" s="107"/>
       <c r="C10" s="3" t="s">
         <v>5</v>
       </c>
@@ -1326,7 +1350,7 @@
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="104"/>
+      <c r="B11" s="107"/>
       <c r="C11" s="3" t="s">
         <v>6</v>
       </c>
@@ -1348,7 +1372,7 @@
       </c>
     </row>
     <row r="12" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="105"/>
+      <c r="B12" s="108"/>
       <c r="C12" s="5" t="s">
         <v>12</v>
       </c>
@@ -1370,7 +1394,7 @@
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B13" s="104" t="s">
+      <c r="B13" s="107" t="s">
         <v>2</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1394,7 +1418,7 @@
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B14" s="104"/>
+      <c r="B14" s="107"/>
       <c r="C14" s="3" t="s">
         <v>5</v>
       </c>
@@ -1416,7 +1440,7 @@
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B15" s="104"/>
+      <c r="B15" s="107"/>
       <c r="C15" s="3" t="s">
         <v>6</v>
       </c>
@@ -1438,7 +1462,7 @@
       </c>
     </row>
     <row r="16" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="105"/>
+      <c r="B16" s="108"/>
       <c r="C16" s="5" t="s">
         <v>12</v>
       </c>
@@ -1527,10 +1551,10 @@
       </c>
     </row>
     <row r="6" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C6" s="104" t="s">
+      <c r="C6" s="107" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="107" t="s">
+      <c r="D6" s="115" t="s">
         <v>15</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -1543,8 +1567,8 @@
       <c r="J6" s="8"/>
     </row>
     <row r="7" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="104"/>
-      <c r="D7" s="108"/>
+      <c r="C7" s="107"/>
+      <c r="D7" s="116"/>
       <c r="E7" s="3" t="s">
         <v>17</v>
       </c>
@@ -1555,8 +1579,8 @@
       <c r="J7" s="8"/>
     </row>
     <row r="8" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C8" s="104"/>
-      <c r="D8" s="108"/>
+      <c r="C8" s="107"/>
+      <c r="D8" s="116"/>
       <c r="E8" s="3" t="s">
         <v>18</v>
       </c>
@@ -1567,8 +1591,8 @@
       <c r="J8" s="8"/>
     </row>
     <row r="9" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="104"/>
-      <c r="D9" s="108"/>
+      <c r="C9" s="107"/>
+      <c r="D9" s="116"/>
       <c r="E9" s="3" t="s">
         <v>19</v>
       </c>
@@ -1579,8 +1603,8 @@
       <c r="J9" s="8"/>
     </row>
     <row r="10" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="104"/>
-      <c r="D10" s="108"/>
+      <c r="C10" s="107"/>
+      <c r="D10" s="116"/>
       <c r="E10" s="3" t="s">
         <v>20</v>
       </c>
@@ -1591,7 +1615,7 @@
       <c r="J10" s="8"/>
     </row>
     <row r="11" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C11" s="104"/>
+      <c r="C11" s="107"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="10"/>
@@ -1601,7 +1625,7 @@
       <c r="J11" s="8"/>
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C12" s="104"/>
+      <c r="C12" s="107"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="10"/>
@@ -1611,7 +1635,7 @@
       <c r="J12" s="8"/>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C13" s="104"/>
+      <c r="C13" s="107"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="10"/>
@@ -1621,7 +1645,7 @@
       <c r="J13" s="8"/>
     </row>
     <row r="14" spans="3:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="105"/>
+      <c r="C14" s="108"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="11"/>
@@ -1631,7 +1655,7 @@
       <c r="J14" s="14"/>
     </row>
     <row r="15" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C15" s="104" t="s">
+      <c r="C15" s="107" t="s">
         <v>1</v>
       </c>
       <c r="D15" s="3"/>
@@ -1643,7 +1667,7 @@
       <c r="J15" s="15"/>
     </row>
     <row r="16" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C16" s="104"/>
+      <c r="C16" s="107"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="10"/>
@@ -1653,7 +1677,7 @@
       <c r="J16" s="8"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C17" s="104"/>
+      <c r="C17" s="107"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="10"/>
@@ -1663,7 +1687,7 @@
       <c r="J17" s="8"/>
     </row>
     <row r="18" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="105"/>
+      <c r="C18" s="108"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="11"/>
@@ -1673,7 +1697,7 @@
       <c r="J18" s="13"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C19" s="104" t="s">
+      <c r="C19" s="107" t="s">
         <v>2</v>
       </c>
       <c r="D19" s="3"/>
@@ -1685,7 +1709,7 @@
       <c r="J19" s="8"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C20" s="104"/>
+      <c r="C20" s="107"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="10"/>
@@ -1695,7 +1719,7 @@
       <c r="J20" s="8"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C21" s="104"/>
+      <c r="C21" s="107"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="10"/>
@@ -1705,7 +1729,7 @@
       <c r="J21" s="8"/>
     </row>
     <row r="22" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="105"/>
+      <c r="C22" s="108"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="11"/>
@@ -1718,7 +1742,7 @@
       <c r="B26" s="66"/>
       <c r="C26" s="66"/>
       <c r="D26" s="109" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E26" s="109"/>
       <c r="F26" s="109"/>
@@ -1730,13 +1754,13 @@
     </row>
     <row r="27" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" s="66"/>
-      <c r="C27" s="106"/>
-      <c r="D27" s="106"/>
-      <c r="E27" s="106"/>
-      <c r="F27" s="106"/>
-      <c r="G27" s="106"/>
-      <c r="H27" s="106"/>
-      <c r="I27" s="106"/>
+      <c r="C27" s="125"/>
+      <c r="D27" s="125"/>
+      <c r="E27" s="125"/>
+      <c r="F27" s="125"/>
+      <c r="G27" s="125"/>
+      <c r="H27" s="125"/>
+      <c r="I27" s="125"/>
       <c r="J27" s="66"/>
       <c r="K27" s="66"/>
     </row>
@@ -1768,7 +1792,7 @@
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B29" s="66"/>
-      <c r="C29" s="114" t="s">
+      <c r="C29" s="110" t="s">
         <v>0</v>
       </c>
       <c r="D29" s="33" t="s">
@@ -1797,7 +1821,7 @@
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B30" s="66"/>
-      <c r="C30" s="113"/>
+      <c r="C30" s="111"/>
       <c r="D30" s="33" t="s">
         <v>22</v>
       </c>
@@ -1824,7 +1848,7 @@
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B31" s="66"/>
-      <c r="C31" s="113"/>
+      <c r="C31" s="111"/>
       <c r="D31" s="33" t="s">
         <v>6</v>
       </c>
@@ -1851,8 +1875,8 @@
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B32" s="66"/>
-      <c r="C32" s="113"/>
-      <c r="D32" s="113" t="s">
+      <c r="C32" s="111"/>
+      <c r="D32" s="111" t="s">
         <v>24</v>
       </c>
       <c r="E32" s="3" t="s">
@@ -1878,8 +1902,8 @@
     </row>
     <row r="33" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B33" s="66"/>
-      <c r="C33" s="113"/>
-      <c r="D33" s="113"/>
+      <c r="C33" s="111"/>
+      <c r="D33" s="111"/>
       <c r="E33" s="3" t="s">
         <v>20</v>
       </c>
@@ -1906,10 +1930,10 @@
     </row>
     <row r="34" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B34" s="66"/>
-      <c r="C34" s="110" t="s">
-        <v>1</v>
-      </c>
-      <c r="D34" s="110" t="s">
+      <c r="C34" s="112" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" s="112" t="s">
         <v>15</v>
       </c>
       <c r="E34" s="22" t="s">
@@ -1935,8 +1959,8 @@
     </row>
     <row r="35" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B35" s="66"/>
-      <c r="C35" s="104"/>
-      <c r="D35" s="111"/>
+      <c r="C35" s="107"/>
+      <c r="D35" s="120"/>
       <c r="E35" s="26" t="s">
         <v>20</v>
       </c>
@@ -1960,8 +1984,8 @@
     </row>
     <row r="36" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B36" s="66"/>
-      <c r="C36" s="104"/>
-      <c r="D36" s="112" t="s">
+      <c r="C36" s="107"/>
+      <c r="D36" s="121" t="s">
         <v>22</v>
       </c>
       <c r="E36" s="29" t="s">
@@ -1987,8 +2011,8 @@
     </row>
     <row r="37" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B37" s="66"/>
-      <c r="C37" s="104"/>
-      <c r="D37" s="111"/>
+      <c r="C37" s="107"/>
+      <c r="D37" s="120"/>
       <c r="E37" s="32" t="s">
         <v>20</v>
       </c>
@@ -2012,7 +2036,7 @@
     </row>
     <row r="38" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B38" s="66"/>
-      <c r="C38" s="104"/>
+      <c r="C38" s="107"/>
       <c r="D38" s="33" t="s">
         <v>6</v>
       </c>
@@ -2039,7 +2063,7 @@
     </row>
     <row r="39" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B39" s="66"/>
-      <c r="C39" s="105"/>
+      <c r="C39" s="108"/>
       <c r="D39" s="5" t="s">
         <v>24</v>
       </c>
@@ -2066,7 +2090,7 @@
     </row>
     <row r="40" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B40" s="66"/>
-      <c r="C40" s="110" t="s">
+      <c r="C40" s="112" t="s">
         <v>2</v>
       </c>
       <c r="D40" s="33" t="s">
@@ -2095,7 +2119,7 @@
     </row>
     <row r="41" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B41" s="66"/>
-      <c r="C41" s="104"/>
+      <c r="C41" s="107"/>
       <c r="D41" s="33" t="s">
         <v>22</v>
       </c>
@@ -2122,7 +2146,7 @@
     </row>
     <row r="42" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B42" s="66"/>
-      <c r="C42" s="104"/>
+      <c r="C42" s="107"/>
       <c r="D42" s="33" t="s">
         <v>6</v>
       </c>
@@ -2136,7 +2160,7 @@
     </row>
     <row r="43" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B43" s="66"/>
-      <c r="C43" s="105"/>
+      <c r="C43" s="108"/>
       <c r="D43" s="5" t="s">
         <v>24</v>
       </c>
@@ -2191,7 +2215,7 @@
     <row r="47" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C47" s="66"/>
       <c r="D47" s="109" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E47" s="109"/>
       <c r="F47" s="109"/>
@@ -2202,7 +2226,7 @@
       <c r="K47" s="66"/>
       <c r="P47" s="66"/>
       <c r="Q47" s="109" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="R47" s="109"/>
       <c r="S47" s="109"/>
@@ -2286,7 +2310,7 @@
     </row>
     <row r="50" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B50" s="66"/>
-      <c r="C50" s="114" t="s">
+      <c r="C50" s="110" t="s">
         <v>0</v>
       </c>
       <c r="D50" s="33" t="s">
@@ -2313,7 +2337,7 @@
       </c>
       <c r="K50" s="66"/>
       <c r="O50" s="66"/>
-      <c r="P50" s="114" t="s">
+      <c r="P50" s="110" t="s">
         <v>0</v>
       </c>
       <c r="Q50" s="33" t="s">
@@ -2342,7 +2366,7 @@
     </row>
     <row r="51" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B51" s="66"/>
-      <c r="C51" s="113"/>
+      <c r="C51" s="111"/>
       <c r="D51" s="33" t="s">
         <v>5</v>
       </c>
@@ -2367,7 +2391,7 @@
       </c>
       <c r="K51" s="66"/>
       <c r="O51" s="66"/>
-      <c r="P51" s="113"/>
+      <c r="P51" s="111"/>
       <c r="Q51" s="33" t="s">
         <v>5</v>
       </c>
@@ -2387,14 +2411,14 @@
         <v>7.6300000000000007E-2</v>
       </c>
       <c r="W51" s="84" t="str">
-        <f t="shared" ref="W51:W62" si="2">IF(V51&lt;0.05, "&lt;0.05", IF(V51&lt;0.1, "&lt;0.1", ""))</f>
+        <f t="shared" ref="W51:W52" si="2">IF(V51&lt;0.05, "&lt;0.05", IF(V51&lt;0.1, "&lt;0.1", ""))</f>
         <v>&lt;0.1</v>
       </c>
       <c r="X51" s="66"/>
     </row>
     <row r="52" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B52" s="66"/>
-      <c r="C52" s="113"/>
+      <c r="C52" s="111"/>
       <c r="D52" s="33" t="s">
         <v>6</v>
       </c>
@@ -2419,7 +2443,7 @@
       </c>
       <c r="K52" s="66"/>
       <c r="O52" s="66"/>
-      <c r="P52" s="113"/>
+      <c r="P52" s="111"/>
       <c r="Q52" s="33" t="s">
         <v>6</v>
       </c>
@@ -2446,7 +2470,7 @@
     </row>
     <row r="53" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B53" s="66"/>
-      <c r="C53" s="113"/>
+      <c r="C53" s="111"/>
       <c r="D53" s="17" t="s">
         <v>24</v>
       </c>
@@ -2460,7 +2484,7 @@
       <c r="J53" s="88"/>
       <c r="K53" s="66"/>
       <c r="O53" s="66"/>
-      <c r="P53" s="113"/>
+      <c r="P53" s="111"/>
       <c r="Q53" s="17" t="s">
         <v>24</v>
       </c>
@@ -2476,10 +2500,10 @@
     </row>
     <row r="54" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B54" s="66"/>
-      <c r="C54" s="110" t="s">
-        <v>1</v>
-      </c>
-      <c r="D54" s="114" t="s">
+      <c r="C54" s="112" t="s">
+        <v>1</v>
+      </c>
+      <c r="D54" s="110" t="s">
         <v>25</v>
       </c>
       <c r="E54" s="22" t="s">
@@ -2503,10 +2527,10 @@
       </c>
       <c r="K54" s="66"/>
       <c r="O54" s="66"/>
-      <c r="P54" s="110" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q54" s="114" t="s">
+      <c r="P54" s="112" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q54" s="110" t="s">
         <v>25</v>
       </c>
       <c r="R54" s="22" t="s">
@@ -2525,15 +2549,15 @@
         <v>3.7449999999999997E-2</v>
       </c>
       <c r="W54" s="63" t="str">
-        <f t="shared" ref="W54:W65" si="3">IF(V54&lt;0.05, "&lt;0.05", IF(V54&lt;0.1, "&lt;0.1", ""))</f>
+        <f t="shared" ref="W54:W58" si="3">IF(V54&lt;0.05, "&lt;0.05", IF(V54&lt;0.1, "&lt;0.1", ""))</f>
         <v>&lt;0.05</v>
       </c>
       <c r="X54" s="66"/>
     </row>
     <row r="55" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B55" s="66"/>
-      <c r="C55" s="104"/>
-      <c r="D55" s="115"/>
+      <c r="C55" s="107"/>
+      <c r="D55" s="113"/>
       <c r="E55" s="26" t="s">
         <v>26</v>
       </c>
@@ -2555,8 +2579,8 @@
       </c>
       <c r="K55" s="66"/>
       <c r="O55" s="66"/>
-      <c r="P55" s="104"/>
-      <c r="Q55" s="115"/>
+      <c r="P55" s="107"/>
+      <c r="Q55" s="113"/>
       <c r="R55" s="26" t="s">
         <v>26</v>
       </c>
@@ -2580,8 +2604,8 @@
     </row>
     <row r="56" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B56" s="66"/>
-      <c r="C56" s="104"/>
-      <c r="D56" s="116" t="s">
+      <c r="C56" s="107"/>
+      <c r="D56" s="114" t="s">
         <v>5</v>
       </c>
       <c r="E56" s="29" t="s">
@@ -2605,8 +2629,8 @@
       </c>
       <c r="K56" s="66"/>
       <c r="O56" s="66"/>
-      <c r="P56" s="104"/>
-      <c r="Q56" s="116" t="s">
+      <c r="P56" s="107"/>
+      <c r="Q56" s="114" t="s">
         <v>5</v>
       </c>
       <c r="R56" s="29" t="s">
@@ -2632,8 +2656,8 @@
     </row>
     <row r="57" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B57" s="66"/>
-      <c r="C57" s="104"/>
-      <c r="D57" s="115"/>
+      <c r="C57" s="107"/>
+      <c r="D57" s="113"/>
       <c r="E57" s="32" t="s">
         <v>20</v>
       </c>
@@ -2655,8 +2679,8 @@
       </c>
       <c r="K57" s="66"/>
       <c r="O57" s="66"/>
-      <c r="P57" s="104"/>
-      <c r="Q57" s="115"/>
+      <c r="P57" s="107"/>
+      <c r="Q57" s="113"/>
       <c r="R57" s="32" t="s">
         <v>20</v>
       </c>
@@ -2680,7 +2704,7 @@
     </row>
     <row r="58" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B58" s="66"/>
-      <c r="C58" s="104"/>
+      <c r="C58" s="107"/>
       <c r="D58" s="33" t="s">
         <v>6</v>
       </c>
@@ -2705,7 +2729,7 @@
       </c>
       <c r="K58" s="66"/>
       <c r="O58" s="66"/>
-      <c r="P58" s="104"/>
+      <c r="P58" s="107"/>
       <c r="Q58" s="33" t="s">
         <v>6</v>
       </c>
@@ -2732,7 +2756,7 @@
     </row>
     <row r="59" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B59" s="66"/>
-      <c r="C59" s="105"/>
+      <c r="C59" s="108"/>
       <c r="D59" s="5" t="s">
         <v>24</v>
       </c>
@@ -2746,7 +2770,7 @@
       <c r="J59" s="88"/>
       <c r="K59" s="66"/>
       <c r="O59" s="66"/>
-      <c r="P59" s="105"/>
+      <c r="P59" s="108"/>
       <c r="Q59" s="5" t="s">
         <v>24</v>
       </c>
@@ -2762,7 +2786,7 @@
     </row>
     <row r="60" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B60" s="66"/>
-      <c r="C60" s="107" t="s">
+      <c r="C60" s="115" t="s">
         <v>2</v>
       </c>
       <c r="D60" s="33" t="s">
@@ -2789,7 +2813,7 @@
       </c>
       <c r="K60" s="66"/>
       <c r="O60" s="66"/>
-      <c r="P60" s="107" t="s">
+      <c r="P60" s="115" t="s">
         <v>2</v>
       </c>
       <c r="Q60" s="33" t="s">
@@ -2811,15 +2835,15 @@
         <v>9.0399999999999994E-3</v>
       </c>
       <c r="W60" s="84" t="str">
-        <f t="shared" ref="W60:W65" si="4">IF(V60&lt;0.05, "&lt;0.05", IF(V60&lt;0.1, "&lt;0.1", ""))</f>
+        <f t="shared" ref="W60:W62" si="4">IF(V60&lt;0.05, "&lt;0.05", IF(V60&lt;0.1, "&lt;0.1", ""))</f>
         <v>&lt;0.05</v>
       </c>
       <c r="X60" s="66"/>
     </row>
     <row r="61" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B61" s="66"/>
-      <c r="C61" s="108"/>
-      <c r="D61" s="116" t="s">
+      <c r="C61" s="116"/>
+      <c r="D61" s="114" t="s">
         <v>5</v>
       </c>
       <c r="E61" s="29" t="s">
@@ -2843,8 +2867,8 @@
       </c>
       <c r="K61" s="66"/>
       <c r="O61" s="66"/>
-      <c r="P61" s="108"/>
-      <c r="Q61" s="116" t="s">
+      <c r="P61" s="116"/>
+      <c r="Q61" s="114" t="s">
         <v>5</v>
       </c>
       <c r="R61" s="29" t="s">
@@ -2870,8 +2894,8 @@
     </row>
     <row r="62" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B62" s="66"/>
-      <c r="C62" s="108"/>
-      <c r="D62" s="115"/>
+      <c r="C62" s="116"/>
+      <c r="D62" s="113"/>
       <c r="E62" s="32" t="s">
         <v>18</v>
       </c>
@@ -2893,8 +2917,8 @@
       </c>
       <c r="K62" s="66"/>
       <c r="O62" s="66"/>
-      <c r="P62" s="108"/>
-      <c r="Q62" s="115"/>
+      <c r="P62" s="116"/>
+      <c r="Q62" s="113"/>
       <c r="R62" s="32" t="s">
         <v>18</v>
       </c>
@@ -2918,7 +2942,7 @@
     </row>
     <row r="63" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B63" s="66"/>
-      <c r="C63" s="108"/>
+      <c r="C63" s="116"/>
       <c r="D63" s="17" t="s">
         <v>6</v>
       </c>
@@ -2930,7 +2954,7 @@
       <c r="J63" s="42"/>
       <c r="K63" s="66"/>
       <c r="O63" s="66"/>
-      <c r="P63" s="108"/>
+      <c r="P63" s="116"/>
       <c r="Q63" s="17" t="s">
         <v>6</v>
       </c>
@@ -3050,7 +3074,7 @@
     </row>
     <row r="71" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B71" s="66"/>
-      <c r="C71" s="114" t="s">
+      <c r="C71" s="110" t="s">
         <v>0</v>
       </c>
       <c r="D71" t="s">
@@ -3070,7 +3094,7 @@
     </row>
     <row r="72" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B72" s="66"/>
-      <c r="C72" s="113"/>
+      <c r="C72" s="111"/>
       <c r="D72" s="20" t="s">
         <v>28</v>
       </c>
@@ -3088,10 +3112,10 @@
     </row>
     <row r="73" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B73" s="66"/>
-      <c r="C73" s="110" t="s">
-        <v>1</v>
-      </c>
-      <c r="D73" s="110" t="s">
+      <c r="C73" s="112" t="s">
+        <v>1</v>
+      </c>
+      <c r="D73" s="112" t="s">
         <v>21</v>
       </c>
       <c r="E73" s="52" t="s">
@@ -3108,8 +3132,8 @@
     </row>
     <row r="74" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B74" s="66"/>
-      <c r="C74" s="104"/>
-      <c r="D74" s="111"/>
+      <c r="C74" s="107"/>
+      <c r="D74" s="120"/>
       <c r="E74" s="56" t="s">
         <v>20</v>
       </c>
@@ -3124,8 +3148,8 @@
     </row>
     <row r="75" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B75" s="66"/>
-      <c r="C75" s="104"/>
-      <c r="D75" s="112" t="s">
+      <c r="C75" s="107"/>
+      <c r="D75" s="121" t="s">
         <v>28</v>
       </c>
       <c r="E75" s="57" t="s">
@@ -3142,8 +3166,8 @@
     </row>
     <row r="76" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B76" s="66"/>
-      <c r="C76" s="104"/>
-      <c r="D76" s="105"/>
+      <c r="C76" s="107"/>
+      <c r="D76" s="108"/>
       <c r="E76" s="59" t="s">
         <v>20</v>
       </c>
@@ -3158,7 +3182,7 @@
     </row>
     <row r="77" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B77" s="66"/>
-      <c r="C77" s="119" t="s">
+      <c r="C77" s="123" t="s">
         <v>2</v>
       </c>
       <c r="D77" s="63" t="s">
@@ -3178,7 +3202,7 @@
     </row>
     <row r="78" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B78" s="66"/>
-      <c r="C78" s="120"/>
+      <c r="C78" s="124"/>
       <c r="D78" s="65" t="s">
         <v>28</v>
       </c>
@@ -3197,13 +3221,13 @@
     <row r="79" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B79" s="66"/>
       <c r="C79" s="61"/>
-      <c r="D79" s="118"/>
-      <c r="E79" s="118"/>
-      <c r="F79" s="118"/>
-      <c r="G79" s="118"/>
-      <c r="H79" s="118"/>
-      <c r="I79" s="118"/>
-      <c r="J79" s="118"/>
+      <c r="D79" s="122"/>
+      <c r="E79" s="122"/>
+      <c r="F79" s="122"/>
+      <c r="G79" s="122"/>
+      <c r="H79" s="122"/>
+      <c r="I79" s="122"/>
+      <c r="J79" s="122"/>
       <c r="K79" s="66"/>
     </row>
     <row r="80" spans="2:24" x14ac:dyDescent="0.2">
@@ -3272,7 +3296,7 @@
     </row>
     <row r="88" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B88" s="66"/>
-      <c r="C88" s="114" t="s">
+      <c r="C88" s="110" t="s">
         <v>0</v>
       </c>
       <c r="D88" t="s">
@@ -3292,7 +3316,7 @@
     </row>
     <row r="89" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B89" s="66"/>
-      <c r="C89" s="113"/>
+      <c r="C89" s="111"/>
       <c r="D89" s="20" t="s">
         <v>28</v>
       </c>
@@ -3310,10 +3334,10 @@
     </row>
     <row r="90" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B90" s="66"/>
-      <c r="C90" s="110" t="s">
-        <v>1</v>
-      </c>
-      <c r="D90" s="110" t="s">
+      <c r="C90" s="112" t="s">
+        <v>1</v>
+      </c>
+      <c r="D90" s="112" t="s">
         <v>21</v>
       </c>
       <c r="E90" s="29" t="s">
@@ -3330,8 +3354,8 @@
     </row>
     <row r="91" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B91" s="66"/>
-      <c r="C91" s="104"/>
-      <c r="D91" s="111"/>
+      <c r="C91" s="107"/>
+      <c r="D91" s="120"/>
       <c r="E91" s="32" t="s">
         <v>20</v>
       </c>
@@ -3346,8 +3370,8 @@
     </row>
     <row r="92" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B92" s="66"/>
-      <c r="C92" s="104"/>
-      <c r="D92" s="112" t="s">
+      <c r="C92" s="107"/>
+      <c r="D92" s="121" t="s">
         <v>28</v>
       </c>
       <c r="E92" s="29" t="s">
@@ -3364,8 +3388,8 @@
     </row>
     <row r="93" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B93" s="66"/>
-      <c r="C93" s="105"/>
-      <c r="D93" s="105"/>
+      <c r="C93" s="108"/>
+      <c r="D93" s="108"/>
       <c r="E93" s="20" t="s">
         <v>20</v>
       </c>
@@ -3380,7 +3404,7 @@
     </row>
     <row r="94" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B94" s="66"/>
-      <c r="C94" s="110" t="s">
+      <c r="C94" s="112" t="s">
         <v>2</v>
       </c>
       <c r="D94" s="63" t="s">
@@ -3400,7 +3424,7 @@
     </row>
     <row r="95" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B95" s="66"/>
-      <c r="C95" s="104"/>
+      <c r="C95" s="107"/>
       <c r="D95" s="52" t="s">
         <v>28</v>
       </c>
@@ -3418,7 +3442,7 @@
     </row>
     <row r="96" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B96" s="66"/>
-      <c r="C96" s="105"/>
+      <c r="C96" s="108"/>
       <c r="D96" s="67"/>
       <c r="E96" s="20" t="s">
         <v>18</v>
@@ -3475,7 +3499,7 @@
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B102" s="66"/>
-      <c r="C102" s="114" t="s">
+      <c r="C102" s="110" t="s">
         <v>0</v>
       </c>
       <c r="D102" t="s">
@@ -3495,7 +3519,7 @@
     </row>
     <row r="103" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B103" s="66"/>
-      <c r="C103" s="113"/>
+      <c r="C103" s="111"/>
       <c r="D103" s="20" t="s">
         <v>28</v>
       </c>
@@ -3513,7 +3537,7 @@
     </row>
     <row r="104" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B104" s="66"/>
-      <c r="C104" s="110" t="s">
+      <c r="C104" s="112" t="s">
         <v>1</v>
       </c>
       <c r="D104" s="16" t="s">
@@ -3533,7 +3557,7 @@
     </row>
     <row r="105" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B105" s="66"/>
-      <c r="C105" s="104"/>
+      <c r="C105" s="107"/>
       <c r="D105" s="43" t="s">
         <v>28</v>
       </c>
@@ -3551,7 +3575,7 @@
     </row>
     <row r="106" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B106" s="66"/>
-      <c r="C106" s="110" t="s">
+      <c r="C106" s="112" t="s">
         <v>2</v>
       </c>
       <c r="D106" s="63" t="s">
@@ -3569,7 +3593,7 @@
     </row>
     <row r="107" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B107" s="66"/>
-      <c r="C107" s="105"/>
+      <c r="C107" s="108"/>
       <c r="D107" s="65" t="s">
         <v>28</v>
       </c>
@@ -3654,7 +3678,7 @@
       <c r="C115" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D115" s="121" t="s">
+      <c r="D115" s="118" t="s">
         <v>21</v>
       </c>
       <c r="E115" s="76" t="s">
@@ -3671,7 +3695,7 @@
     <row r="116" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B116" s="66"/>
       <c r="C116" s="37"/>
-      <c r="D116" s="122"/>
+      <c r="D116" s="119"/>
       <c r="E116" s="80" t="s">
         <v>20</v>
       </c>
@@ -3764,11 +3788,26 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="Q47:W47"/>
-    <mergeCell ref="P50:P53"/>
-    <mergeCell ref="P54:P59"/>
-    <mergeCell ref="Q54:Q55"/>
-    <mergeCell ref="Q56:Q57"/>
+    <mergeCell ref="C27:I27"/>
+    <mergeCell ref="C6:C14"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="C19:C22"/>
+    <mergeCell ref="D6:D10"/>
+    <mergeCell ref="D26:J26"/>
+    <mergeCell ref="C40:C43"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="C29:C33"/>
+    <mergeCell ref="C34:C39"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="D73:D74"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="D47:J47"/>
+    <mergeCell ref="C50:C53"/>
+    <mergeCell ref="C54:C59"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="D56:D57"/>
     <mergeCell ref="P60:P64"/>
     <mergeCell ref="Q61:Q62"/>
     <mergeCell ref="D115:D116"/>
@@ -3785,26 +3824,11 @@
     <mergeCell ref="D79:J79"/>
     <mergeCell ref="C71:C72"/>
     <mergeCell ref="C73:C76"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="D73:D74"/>
-    <mergeCell ref="C77:C78"/>
-    <mergeCell ref="D47:J47"/>
-    <mergeCell ref="C50:C53"/>
-    <mergeCell ref="C54:C59"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="C40:C43"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="C29:C33"/>
-    <mergeCell ref="C34:C39"/>
-    <mergeCell ref="C27:I27"/>
-    <mergeCell ref="C6:C14"/>
-    <mergeCell ref="C15:C18"/>
-    <mergeCell ref="C19:C22"/>
-    <mergeCell ref="D6:D10"/>
-    <mergeCell ref="D26:J26"/>
+    <mergeCell ref="Q47:W47"/>
+    <mergeCell ref="P50:P53"/>
+    <mergeCell ref="P54:P59"/>
+    <mergeCell ref="Q54:Q55"/>
+    <mergeCell ref="Q56:Q57"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="J6:J22">
@@ -3821,8 +3845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11EC7562-B833-6E47-893A-48CC2F5000AD}">
   <dimension ref="C6:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="88" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="88" workbookViewId="0">
+      <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3834,7 +3858,7 @@
     <row r="6" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C6" s="66"/>
       <c r="D6" s="109" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E6" s="109"/>
       <c r="F6" s="109"/>
@@ -3881,10 +3905,10 @@
       <c r="K8" s="66"/>
     </row>
     <row r="9" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C9" s="114" t="s">
+      <c r="C9" s="110" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="110" t="s">
+      <c r="D9" s="112" t="s">
         <v>25</v>
       </c>
       <c r="E9" s="34" t="s">
@@ -3908,8 +3932,8 @@
       <c r="K9" s="66"/>
     </row>
     <row r="10" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C10" s="123"/>
-      <c r="D10" s="111"/>
+      <c r="C10" s="111"/>
+      <c r="D10" s="120"/>
       <c r="E10" s="34" t="s">
         <v>20</v>
       </c>
@@ -3931,8 +3955,8 @@
       <c r="K10" s="66"/>
     </row>
     <row r="11" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C11" s="123"/>
-      <c r="D11" s="112" t="s">
+      <c r="C11" s="111"/>
+      <c r="D11" s="121" t="s">
         <v>5</v>
       </c>
       <c r="E11" s="34" t="s">
@@ -3956,8 +3980,8 @@
       <c r="K11" s="66"/>
     </row>
     <row r="12" spans="3:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C12" s="113"/>
-      <c r="D12" s="111"/>
+      <c r="C12" s="111"/>
+      <c r="D12" s="120"/>
       <c r="E12" s="34" t="s">
         <v>20</v>
       </c>
@@ -3979,7 +4003,7 @@
       <c r="K12" s="66"/>
     </row>
     <row r="13" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C13" s="113"/>
+      <c r="C13" s="111"/>
       <c r="D13" s="33" t="s">
         <v>6</v>
       </c>
@@ -4004,7 +4028,7 @@
       <c r="K13" s="66"/>
     </row>
     <row r="14" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="113"/>
+      <c r="C14" s="111"/>
       <c r="D14" s="17" t="s">
         <v>24</v>
       </c>
@@ -4019,10 +4043,10 @@
       <c r="K14" s="66"/>
     </row>
     <row r="15" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C15" s="110" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" s="114" t="s">
+      <c r="C15" s="112" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="110" t="s">
         <v>25</v>
       </c>
       <c r="E15" s="22" t="s">
@@ -4046,8 +4070,8 @@
       <c r="K15" s="66"/>
     </row>
     <row r="16" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="104"/>
-      <c r="D16" s="115"/>
+      <c r="C16" s="107"/>
+      <c r="D16" s="113"/>
       <c r="E16" s="26" t="s">
         <v>26</v>
       </c>
@@ -4069,8 +4093,8 @@
       <c r="K16" s="66"/>
     </row>
     <row r="17" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C17" s="104"/>
-      <c r="D17" s="116" t="s">
+      <c r="C17" s="107"/>
+      <c r="D17" s="114" t="s">
         <v>5</v>
       </c>
       <c r="E17" s="29" t="s">
@@ -4094,8 +4118,8 @@
       <c r="K17" s="66"/>
     </row>
     <row r="18" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C18" s="104"/>
-      <c r="D18" s="115"/>
+      <c r="C18" s="107"/>
+      <c r="D18" s="113"/>
       <c r="E18" s="32" t="s">
         <v>20</v>
       </c>
@@ -4117,8 +4141,8 @@
       <c r="K18" s="66"/>
     </row>
     <row r="19" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C19" s="104"/>
-      <c r="D19" s="112" t="s">
+      <c r="C19" s="107"/>
+      <c r="D19" s="121" t="s">
         <v>6</v>
       </c>
       <c r="E19" s="34" t="s">
@@ -4142,9 +4166,9 @@
       <c r="K19" s="66"/>
     </row>
     <row r="20" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C20" s="104"/>
-      <c r="D20" s="124"/>
-      <c r="E20" s="125" t="s">
+      <c r="C20" s="107"/>
+      <c r="D20" s="107"/>
+      <c r="E20" s="3" t="s">
         <v>18</v>
       </c>
       <c r="F20" s="35">
@@ -4165,7 +4189,7 @@
       <c r="K20" s="66"/>
     </row>
     <row r="21" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="105"/>
+      <c r="C21" s="108"/>
       <c r="D21" s="5" t="s">
         <v>24</v>
       </c>
@@ -4180,10 +4204,10 @@
       <c r="K21" s="66"/>
     </row>
     <row r="22" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C22" s="110" t="s">
+      <c r="C22" s="112" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="110" t="s">
+      <c r="D22" s="112" t="s">
         <v>25</v>
       </c>
       <c r="E22" t="s">
@@ -4207,8 +4231,8 @@
       <c r="K22" s="66"/>
     </row>
     <row r="23" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C23" s="124"/>
-      <c r="D23" s="124"/>
+      <c r="C23" s="107"/>
+      <c r="D23" s="107"/>
       <c r="E23" s="34" t="s">
         <v>17</v>
       </c>
@@ -4230,9 +4254,9 @@
       <c r="K23" s="66"/>
     </row>
     <row r="24" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C24" s="124"/>
-      <c r="D24" s="111"/>
-      <c r="E24" s="126" t="s">
+      <c r="C24" s="107"/>
+      <c r="D24" s="120"/>
+      <c r="E24" s="104" t="s">
         <v>20</v>
       </c>
       <c r="F24" s="30">
@@ -4253,11 +4277,11 @@
       <c r="K24" s="66"/>
     </row>
     <row r="25" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C25" s="124"/>
-      <c r="D25" s="116" t="s">
+      <c r="C25" s="107"/>
+      <c r="D25" s="114" t="s">
         <v>5</v>
       </c>
-      <c r="E25" s="126" t="s">
+      <c r="E25" s="104" t="s">
         <v>16</v>
       </c>
       <c r="F25" s="30">
@@ -4278,8 +4302,8 @@
       <c r="K25" s="66"/>
     </row>
     <row r="26" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C26" s="104"/>
-      <c r="D26" s="123"/>
+      <c r="C26" s="107"/>
+      <c r="D26" s="111"/>
       <c r="E26" s="29" t="s">
         <v>17</v>
       </c>
@@ -4292,7 +4316,7 @@
       <c r="H26" s="30">
         <v>16.018999999999998</v>
       </c>
-      <c r="I26" s="130">
+      <c r="I26" s="105">
         <v>6.0500000000000003E-7</v>
       </c>
       <c r="J26" s="57" t="s">
@@ -4301,21 +4325,21 @@
       <c r="K26" s="66"/>
     </row>
     <row r="27" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C27" s="104"/>
-      <c r="D27" s="123"/>
-      <c r="E27" s="125" t="s">
+      <c r="C27" s="107"/>
+      <c r="D27" s="111"/>
+      <c r="E27" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F27" s="127">
-        <v>1</v>
-      </c>
-      <c r="G27" s="127">
-        <v>1</v>
-      </c>
-      <c r="H27" s="127">
+      <c r="F27" s="10">
+        <v>1</v>
+      </c>
+      <c r="G27" s="10">
+        <v>1</v>
+      </c>
+      <c r="H27" s="10">
         <v>5.4089999999999998</v>
       </c>
-      <c r="I27" s="128">
+      <c r="I27" s="18">
         <v>2.1299999999999999E-2</v>
       </c>
       <c r="J27" s="57" t="s">
@@ -4324,8 +4348,8 @@
       <c r="K27" s="66"/>
     </row>
     <row r="28" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C28" s="104"/>
-      <c r="D28" s="115"/>
+      <c r="C28" s="107"/>
+      <c r="D28" s="113"/>
       <c r="E28" s="32" t="s">
         <v>26</v>
       </c>
@@ -4347,7 +4371,7 @@
       <c r="K28" s="66"/>
     </row>
     <row r="29" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C29" s="104"/>
+      <c r="C29" s="107"/>
       <c r="D29" s="17" t="s">
         <v>6</v>
       </c>
@@ -4360,7 +4384,7 @@
       <c r="K29" s="66"/>
     </row>
     <row r="30" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C30" s="105"/>
+      <c r="C30" s="108"/>
       <c r="D30" s="5" t="s">
         <v>24</v>
       </c>
@@ -4388,7 +4412,7 @@
     <row r="35" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C35" s="66"/>
       <c r="D35" s="109" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E35" s="109"/>
       <c r="F35" s="109"/>
@@ -4435,35 +4459,35 @@
       <c r="K37" s="66"/>
     </row>
     <row r="38" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C38" s="114" t="s">
+      <c r="C38" s="110" t="s">
         <v>0</v>
       </c>
-      <c r="D38" s="112" t="s">
+      <c r="D38" s="121" t="s">
         <v>5</v>
       </c>
-      <c r="E38" s="132" t="s">
+      <c r="E38" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="F38" s="127">
-        <v>1</v>
-      </c>
-      <c r="G38" s="127">
-        <v>1</v>
-      </c>
-      <c r="H38" s="127">
+      <c r="F38" s="10">
+        <v>1</v>
+      </c>
+      <c r="G38" s="10">
+        <v>1</v>
+      </c>
+      <c r="H38" s="10">
         <v>4.6680000000000001</v>
       </c>
-      <c r="I38" s="128">
+      <c r="I38" s="18">
         <v>3.2199999999999999E-2</v>
       </c>
-      <c r="J38" s="129" t="s">
+      <c r="J38" s="52" t="s">
         <v>29</v>
       </c>
       <c r="K38" s="66"/>
     </row>
     <row r="39" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C39" s="123"/>
-      <c r="D39" s="111"/>
+      <c r="C39" s="111"/>
+      <c r="D39" s="120"/>
       <c r="E39" s="32" t="s">
         <v>20</v>
       </c>
@@ -4485,7 +4509,7 @@
       <c r="K39" s="66"/>
     </row>
     <row r="40" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C40" s="123"/>
+      <c r="C40" s="111"/>
       <c r="D40" s="33" t="s">
         <v>6</v>
       </c>
@@ -4510,7 +4534,7 @@
       <c r="K40" s="66"/>
     </row>
     <row r="41" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C41" s="131"/>
+      <c r="C41" s="126"/>
       <c r="D41" s="17" t="s">
         <v>24</v>
       </c>
@@ -4525,10 +4549,10 @@
       <c r="K41" s="66"/>
     </row>
     <row r="42" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C42" s="114" t="s">
-        <v>1</v>
-      </c>
-      <c r="D42" s="116" t="s">
+      <c r="C42" s="110" t="s">
+        <v>1</v>
+      </c>
+      <c r="D42" s="114" t="s">
         <v>5</v>
       </c>
       <c r="E42" s="29" t="s">
@@ -4552,8 +4576,8 @@
       <c r="K42" s="66"/>
     </row>
     <row r="43" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C43" s="123"/>
-      <c r="D43" s="115"/>
+      <c r="C43" s="111"/>
+      <c r="D43" s="113"/>
       <c r="E43" s="32" t="s">
         <v>20</v>
       </c>
@@ -4575,8 +4599,8 @@
       <c r="K43" s="66"/>
     </row>
     <row r="44" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C44" s="123"/>
-      <c r="D44" s="112" t="s">
+      <c r="C44" s="111"/>
+      <c r="D44" s="121" t="s">
         <v>6</v>
       </c>
       <c r="E44" s="34" t="s">
@@ -4600,9 +4624,9 @@
       <c r="K44" s="66"/>
     </row>
     <row r="45" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C45" s="123"/>
-      <c r="D45" s="124"/>
-      <c r="E45" s="125" t="s">
+      <c r="C45" s="111"/>
+      <c r="D45" s="107"/>
+      <c r="E45" s="3" t="s">
         <v>18</v>
       </c>
       <c r="F45" s="35">
@@ -4623,7 +4647,7 @@
       <c r="K45" s="66"/>
     </row>
     <row r="46" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C46" s="131"/>
+      <c r="C46" s="126"/>
       <c r="D46" s="5" t="s">
         <v>24</v>
       </c>
@@ -4638,13 +4662,13 @@
       <c r="K46" s="66"/>
     </row>
     <row r="47" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C47" s="114" t="s">
+      <c r="C47" s="110" t="s">
         <v>2</v>
       </c>
-      <c r="D47" s="116" t="s">
+      <c r="D47" s="114" t="s">
         <v>5</v>
       </c>
-      <c r="E47" s="126" t="s">
+      <c r="E47" s="29" t="s">
         <v>16</v>
       </c>
       <c r="F47" s="30">
@@ -4656,63 +4680,63 @@
       <c r="H47" s="30">
         <v>2.98</v>
       </c>
-      <c r="I47" s="31">
+      <c r="I47" s="24">
         <v>2.63E-2</v>
       </c>
-      <c r="J47" s="57" t="s">
+      <c r="J47" s="63" t="s">
         <v>29</v>
       </c>
       <c r="K47" s="66"/>
     </row>
     <row r="48" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C48" s="123"/>
-      <c r="D48" s="123"/>
-      <c r="E48" s="29" t="s">
+      <c r="C48" s="111"/>
+      <c r="D48" s="111"/>
+      <c r="E48" s="129" t="s">
         <v>17</v>
       </c>
-      <c r="F48" s="30">
+      <c r="F48" s="130">
         <v>2.097</v>
       </c>
-      <c r="G48" s="30">
+      <c r="G48" s="130">
         <v>2.097</v>
       </c>
-      <c r="H48" s="30">
+      <c r="H48" s="130">
         <v>16.018999999999998</v>
       </c>
-      <c r="I48" s="130">
+      <c r="I48" s="131">
         <v>6.0500000000000003E-7</v>
       </c>
-      <c r="J48" s="133" t="s">
+      <c r="J48" s="132" t="s">
         <v>29</v>
       </c>
       <c r="K48" s="66"/>
     </row>
     <row r="49" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C49" s="123"/>
-      <c r="D49" s="123"/>
-      <c r="E49" s="125" t="s">
+      <c r="C49" s="111"/>
+      <c r="D49" s="111"/>
+      <c r="E49" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F49" s="127">
-        <v>1</v>
-      </c>
-      <c r="G49" s="127">
-        <v>1</v>
-      </c>
-      <c r="H49" s="127">
+      <c r="F49" s="10">
+        <v>1</v>
+      </c>
+      <c r="G49" s="10">
+        <v>1</v>
+      </c>
+      <c r="H49" s="10">
         <v>5.4089999999999998</v>
       </c>
-      <c r="I49" s="128">
+      <c r="I49" s="18">
         <v>2.1299999999999999E-2</v>
       </c>
-      <c r="J49" s="129" t="s">
+      <c r="J49" s="52" t="s">
         <v>29</v>
       </c>
       <c r="K49" s="66"/>
     </row>
     <row r="50" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C50" s="123"/>
-      <c r="D50" s="115"/>
+      <c r="C50" s="111"/>
+      <c r="D50" s="113"/>
       <c r="E50" s="32" t="s">
         <v>26</v>
       </c>
@@ -4734,7 +4758,7 @@
       <c r="K50" s="66"/>
     </row>
     <row r="51" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C51" s="123"/>
+      <c r="C51" s="111"/>
       <c r="D51" s="17" t="s">
         <v>6</v>
       </c>
@@ -4747,7 +4771,7 @@
       <c r="K51" s="66"/>
     </row>
     <row r="52" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C52" s="131"/>
+      <c r="C52" s="126"/>
       <c r="D52" s="5" t="s">
         <v>24</v>
       </c>
@@ -4774,17 +4798,9 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="D6:J6"/>
     <mergeCell ref="C38:C41"/>
     <mergeCell ref="C42:C46"/>
-    <mergeCell ref="C47:C52"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="D47:D50"/>
-    <mergeCell ref="D22:D24"/>
-    <mergeCell ref="D25:D28"/>
-    <mergeCell ref="D35:J35"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="D6:J6"/>
     <mergeCell ref="C9:C14"/>
     <mergeCell ref="C15:C21"/>
     <mergeCell ref="D15:D16"/>
@@ -4793,6 +4809,14 @@
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="D25:D28"/>
+    <mergeCell ref="C47:C52"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="D47:D50"/>
+    <mergeCell ref="D35:J35"/>
+    <mergeCell ref="D38:D39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4800,19 +4824,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8F6DB0D-2B41-A146-8989-239E41193B1F}">
-  <dimension ref="B1:M53"/>
+  <dimension ref="B1:AD53"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="K48" sqref="K48"/>
+    <sheetView topLeftCell="P18" workbookViewId="0">
+      <selection activeCell="AB54" sqref="AB54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="25.5" customWidth="1"/>
     <col min="5" max="10" width="9.6640625" customWidth="1"/>
+    <col min="13" max="13" width="19.33203125" customWidth="1"/>
+    <col min="23" max="23" width="32.33203125" customWidth="1"/>
+    <col min="27" max="27" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C1" s="66"/>
       <c r="D1" s="66"/>
       <c r="E1" s="66"/>
@@ -4824,7 +4851,7 @@
       <c r="K1" s="66"/>
       <c r="L1" s="66"/>
     </row>
-    <row r="2" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C2" s="66"/>
       <c r="D2" s="66"/>
       <c r="E2" s="66"/>
@@ -4836,7 +4863,7 @@
       <c r="K2" s="66"/>
       <c r="L2" s="66"/>
     </row>
-    <row r="3" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C3" s="66"/>
       <c r="D3" s="66"/>
       <c r="E3" s="66"/>
@@ -4849,62 +4876,36 @@
       <c r="L3" s="66"/>
       <c r="M3" s="66"/>
     </row>
-    <row r="4" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C4" s="66"/>
-      <c r="D4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
       <c r="K4" s="66"/>
       <c r="L4" s="66"/>
       <c r="M4" s="66"/>
     </row>
-    <row r="5" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C5" s="66"/>
-      <c r="D5" s="104" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="10">
-        <v>2.7719999999999998</v>
-      </c>
-      <c r="G5" s="10">
-        <v>3.45</v>
-      </c>
-      <c r="H5" s="10">
-        <v>0.88200000000000001</v>
-      </c>
+      <c r="D5" s="107"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
       <c r="I5" s="12"/>
       <c r="J5" s="8"/>
       <c r="K5" s="92"/>
       <c r="L5" s="66"/>
       <c r="M5" s="66"/>
     </row>
-    <row r="6" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C6" s="66"/>
-      <c r="D6" s="104"/>
-      <c r="E6" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="D6" s="107"/>
+      <c r="E6" s="3"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
@@ -4914,12 +4915,10 @@
       <c r="L6" s="66"/>
       <c r="M6" s="66"/>
     </row>
-    <row r="7" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C7" s="66"/>
-      <c r="D7" s="104"/>
-      <c r="E7" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="D7" s="107"/>
+      <c r="E7" s="3"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
@@ -4929,12 +4928,10 @@
       <c r="L7" s="66"/>
       <c r="M7" s="66"/>
     </row>
-    <row r="8" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C8" s="66"/>
-      <c r="D8" s="105"/>
-      <c r="E8" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="D8" s="108"/>
+      <c r="E8" s="5"/>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
@@ -4944,14 +4941,10 @@
       <c r="L8" s="66"/>
       <c r="M8" s="66"/>
     </row>
-    <row r="9" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C9" s="66"/>
-      <c r="D9" s="104" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="D9" s="107"/>
+      <c r="E9" s="3"/>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
@@ -4961,12 +4954,10 @@
       <c r="L9" s="66"/>
       <c r="M9" s="66"/>
     </row>
-    <row r="10" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C10" s="66"/>
-      <c r="D10" s="104"/>
-      <c r="E10" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="D10" s="107"/>
+      <c r="E10" s="3"/>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
@@ -4976,12 +4967,10 @@
       <c r="L10" s="10"/>
       <c r="M10" s="66"/>
     </row>
-    <row r="11" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C11" s="66"/>
-      <c r="D11" s="104"/>
-      <c r="E11" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="D11" s="107"/>
+      <c r="E11" s="3"/>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
@@ -4991,12 +4980,10 @@
       <c r="L11" s="66"/>
       <c r="M11" s="66"/>
     </row>
-    <row r="12" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C12" s="66"/>
-      <c r="D12" s="105"/>
-      <c r="E12" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="D12" s="108"/>
+      <c r="E12" s="5"/>
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
@@ -5006,59 +4993,81 @@
       <c r="L12" s="66"/>
       <c r="M12" s="66"/>
     </row>
-    <row r="13" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="3:29" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C13" s="66"/>
-      <c r="D13" s="104" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="8"/>
+      <c r="D13" s="127" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="127"/>
+      <c r="F13" s="127"/>
+      <c r="G13" s="127"/>
+      <c r="H13" s="127"/>
+      <c r="I13" s="127"/>
+      <c r="J13" s="127"/>
       <c r="K13" s="52"/>
       <c r="L13" s="66"/>
       <c r="M13" s="66"/>
     </row>
-    <row r="14" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="3:29" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C14" s="66"/>
-      <c r="D14" s="104"/>
-      <c r="E14" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="8"/>
+      <c r="D14" s="128"/>
+      <c r="E14" s="128"/>
+      <c r="F14" s="128"/>
+      <c r="G14" s="128"/>
+      <c r="H14" s="128"/>
+      <c r="I14" s="128"/>
+      <c r="J14" s="128"/>
       <c r="K14" s="52"/>
       <c r="L14" s="66"/>
-      <c r="M14" s="66"/>
-    </row>
-    <row r="15" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="M14" s="127" t="s">
+        <v>51</v>
+      </c>
+      <c r="N14" s="127"/>
+      <c r="O14" s="127"/>
+      <c r="P14" s="127"/>
+      <c r="Q14" s="127"/>
+      <c r="R14" s="127"/>
+      <c r="S14" s="127"/>
+      <c r="W14" s="127" t="s">
+        <v>52</v>
+      </c>
+      <c r="X14" s="127"/>
+      <c r="Y14" s="127"/>
+      <c r="Z14" s="127"/>
+      <c r="AA14" s="127"/>
+      <c r="AB14" s="127"/>
+      <c r="AC14" s="127"/>
+    </row>
+    <row r="15" spans="3:29" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C15" s="66"/>
-      <c r="D15" s="104"/>
-      <c r="E15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="8"/>
+      <c r="D15" s="128"/>
+      <c r="E15" s="128"/>
+      <c r="F15" s="128"/>
+      <c r="G15" s="128"/>
+      <c r="H15" s="128"/>
+      <c r="I15" s="128"/>
+      <c r="J15" s="128"/>
       <c r="K15" s="52"/>
       <c r="L15" s="66"/>
-      <c r="M15" s="66"/>
-    </row>
-    <row r="16" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="M15" s="128"/>
+      <c r="N15" s="128"/>
+      <c r="O15" s="128"/>
+      <c r="P15" s="128"/>
+      <c r="Q15" s="128"/>
+      <c r="R15" s="128"/>
+      <c r="S15" s="128"/>
+      <c r="W15" s="128"/>
+      <c r="X15" s="128"/>
+      <c r="Y15" s="128"/>
+      <c r="Z15" s="128"/>
+      <c r="AA15" s="128"/>
+      <c r="AB15" s="128"/>
+      <c r="AC15" s="128"/>
+    </row>
+    <row r="16" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C16" s="66"/>
-      <c r="D16" s="104"/>
-      <c r="E16" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="D16" s="17"/>
+      <c r="E16" s="3"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
@@ -5066,16 +5075,25 @@
       <c r="J16" s="12"/>
       <c r="K16" s="52"/>
       <c r="L16" s="66"/>
-      <c r="M16" s="66"/>
-    </row>
-    <row r="17" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="M16" s="128"/>
+      <c r="N16" s="128"/>
+      <c r="O16" s="128"/>
+      <c r="P16" s="128"/>
+      <c r="Q16" s="128"/>
+      <c r="R16" s="128"/>
+      <c r="S16" s="128"/>
+      <c r="W16" s="128"/>
+      <c r="X16" s="128"/>
+      <c r="Y16" s="128"/>
+      <c r="Z16" s="128"/>
+      <c r="AA16" s="128"/>
+      <c r="AB16" s="128"/>
+      <c r="AC16" s="128"/>
+    </row>
+    <row r="17" spans="3:30" x14ac:dyDescent="0.2">
       <c r="C17" s="66"/>
-      <c r="D17" s="104" t="s">
-        <v>41</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="D17" s="107"/>
+      <c r="E17" s="3"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
@@ -5085,12 +5103,10 @@
       <c r="L17" s="66"/>
       <c r="M17" s="66"/>
     </row>
-    <row r="18" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:30" x14ac:dyDescent="0.2">
       <c r="C18" s="66"/>
-      <c r="D18" s="104"/>
-      <c r="E18" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="D18" s="107"/>
+      <c r="E18" s="3"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
@@ -5100,12 +5116,10 @@
       <c r="L18" s="66"/>
       <c r="M18" s="66"/>
     </row>
-    <row r="19" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:30" x14ac:dyDescent="0.2">
       <c r="C19" s="66"/>
-      <c r="D19" s="104"/>
-      <c r="E19" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="D19" s="107"/>
+      <c r="E19" s="3"/>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
@@ -5115,12 +5129,10 @@
       <c r="L19" s="66"/>
       <c r="M19" s="66"/>
     </row>
-    <row r="20" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:30" x14ac:dyDescent="0.2">
       <c r="C20" s="66"/>
-      <c r="D20" s="104"/>
-      <c r="E20" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="D20" s="107"/>
+      <c r="E20" s="3"/>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
@@ -5130,7 +5142,7 @@
       <c r="L20" s="66"/>
       <c r="M20" s="66"/>
     </row>
-    <row r="21" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:30" x14ac:dyDescent="0.2">
       <c r="C21" s="66"/>
       <c r="D21" s="3"/>
       <c r="E21" s="66"/>
@@ -5143,16 +5155,19 @@
       <c r="L21" s="66"/>
       <c r="M21" s="66"/>
     </row>
-    <row r="22" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C22" s="66"/>
       <c r="D22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K22" s="66"/>
       <c r="L22" s="66"/>
-      <c r="M22" s="66"/>
-    </row>
-    <row r="23" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M22" t="s">
+        <v>44</v>
+      </c>
+      <c r="T22" s="66"/>
+    </row>
+    <row r="23" spans="3:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C23" s="66"/>
       <c r="D23" s="3"/>
       <c r="E23" s="66"/>
@@ -5163,9 +5178,38 @@
       <c r="J23" s="66"/>
       <c r="K23" s="66"/>
       <c r="L23" s="66"/>
-      <c r="M23" s="66"/>
-    </row>
-    <row r="24" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M23" s="3"/>
+      <c r="N23" s="66"/>
+      <c r="O23" s="66"/>
+      <c r="P23" s="66"/>
+      <c r="Q23" s="66"/>
+      <c r="R23" s="66"/>
+      <c r="S23" s="66"/>
+      <c r="T23" s="66"/>
+      <c r="W23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="X23" s="94" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y23" s="94" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z23" s="94" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA23" s="94" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB23" s="94" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC23" s="94" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD23" s="66"/>
+    </row>
+    <row r="24" spans="3:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C24" s="66"/>
       <c r="D24" s="2" t="s">
         <v>37</v>
@@ -5183,16 +5227,59 @@
         <v>9</v>
       </c>
       <c r="I24" s="94" t="s">
+        <v>41</v>
+      </c>
+      <c r="J24" s="94" t="s">
         <v>42</v>
-      </c>
-      <c r="J24" s="94" t="s">
-        <v>43</v>
       </c>
       <c r="K24" s="66"/>
       <c r="L24" s="66"/>
-      <c r="M24" s="66"/>
-    </row>
-    <row r="25" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="M24" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N24" s="94" t="s">
+        <v>7</v>
+      </c>
+      <c r="O24" s="94" t="s">
+        <v>11</v>
+      </c>
+      <c r="P24" s="94" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q24" s="94" t="s">
+        <v>9</v>
+      </c>
+      <c r="R24" s="94" t="s">
+        <v>41</v>
+      </c>
+      <c r="S24" s="94" t="s">
+        <v>42</v>
+      </c>
+      <c r="T24" s="66"/>
+      <c r="W24" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="X24" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y24" s="10">
+        <v>1</v>
+      </c>
+      <c r="Z24" s="10">
+        <v>1.9E-2</v>
+      </c>
+      <c r="AA24" s="12">
+        <v>0.89</v>
+      </c>
+      <c r="AB24" s="12">
+        <v>-3.0599999999999999E-2</v>
+      </c>
+      <c r="AC24" s="95">
+        <v>34</v>
+      </c>
+      <c r="AD24" s="92"/>
+    </row>
+    <row r="25" spans="3:30" x14ac:dyDescent="0.2">
       <c r="C25" s="66"/>
       <c r="D25" s="16" t="s">
         <v>38</v>
@@ -5217,12 +5304,43 @@
       </c>
       <c r="K25" s="92"/>
       <c r="L25" s="66"/>
-      <c r="M25" s="66"/>
-    </row>
-    <row r="26" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="M25" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="12"/>
+      <c r="R25" s="12"/>
+      <c r="S25" s="95"/>
+      <c r="T25" s="92"/>
+      <c r="W25" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="X25" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y25" s="10">
+        <v>1</v>
+      </c>
+      <c r="Z25" s="10">
+        <v>0.88100000000000001</v>
+      </c>
+      <c r="AA25" s="12">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="AB25" s="12">
+        <v>-3.63E-3</v>
+      </c>
+      <c r="AC25" s="95">
+        <v>34</v>
+      </c>
+      <c r="AD25" s="52"/>
+    </row>
+    <row r="26" spans="3:30" x14ac:dyDescent="0.2">
       <c r="C26" s="66"/>
       <c r="D26" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E26" s="10">
         <v>1</v>
@@ -5244,12 +5362,43 @@
       </c>
       <c r="K26" s="52"/>
       <c r="L26" s="66"/>
-      <c r="M26" s="66"/>
-    </row>
-    <row r="27" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="M26" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="12"/>
+      <c r="R26" s="12"/>
+      <c r="S26" s="95"/>
+      <c r="T26" s="52"/>
+      <c r="W26" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="X26" s="10">
+        <v>2.0920000000000001</v>
+      </c>
+      <c r="Y26" s="10">
+        <v>2.6349999999999998</v>
+      </c>
+      <c r="Z26" s="10">
+        <v>1.4119999999999999</v>
+      </c>
+      <c r="AA26" s="12">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="AB26" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="AC26" s="95">
+        <v>34</v>
+      </c>
+      <c r="AD26" s="6"/>
+    </row>
+    <row r="27" spans="3:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C27" s="66"/>
       <c r="D27" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E27" s="10">
         <v>1</v>
@@ -5270,11 +5419,43 @@
         <v>30</v>
       </c>
       <c r="K27" s="6"/>
-    </row>
-    <row r="28" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M27" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="12"/>
+      <c r="R27" s="8"/>
+      <c r="S27" s="95"/>
+      <c r="T27" s="6"/>
+      <c r="W27" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="X27" s="11">
+        <v>4.2809999999999997</v>
+      </c>
+      <c r="Y27" s="11">
+        <v>5.173</v>
+      </c>
+      <c r="Z27" s="11">
+        <v>2.3039999999999998</v>
+      </c>
+      <c r="AA27" s="102">
+        <v>6.8599999999999994E-2</v>
+      </c>
+      <c r="AB27" s="9">
+        <v>0.23899999999999999</v>
+      </c>
+      <c r="AC27" s="96">
+        <v>34</v>
+      </c>
+      <c r="AD27" s="52"/>
+    </row>
+    <row r="28" spans="3:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C28" s="66"/>
       <c r="D28" s="37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E28" s="11">
         <v>5.5380000000000003</v>
@@ -5295,8 +5476,37 @@
         <v>34</v>
       </c>
       <c r="K28" s="52"/>
-    </row>
-    <row r="29" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="M28" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="N28" s="11">
+        <v>6.3170000000000002</v>
+      </c>
+      <c r="O28" s="11">
+        <v>7.25</v>
+      </c>
+      <c r="P28" s="11">
+        <v>3.2770000000000001</v>
+      </c>
+      <c r="Q28" s="100">
+        <v>1.21E-2</v>
+      </c>
+      <c r="R28" s="9">
+        <v>0.38300000000000001</v>
+      </c>
+      <c r="S28" s="96">
+        <v>33</v>
+      </c>
+      <c r="T28" s="52"/>
+      <c r="X28" s="10"/>
+      <c r="Y28" s="10"/>
+      <c r="Z28" s="10"/>
+      <c r="AA28" s="99"/>
+      <c r="AB28" s="8"/>
+      <c r="AC28" s="95"/>
+      <c r="AD28" s="52"/>
+    </row>
+    <row r="29" spans="3:30" x14ac:dyDescent="0.2">
       <c r="C29" s="66"/>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
@@ -5305,8 +5515,25 @@
       <c r="I29" s="8"/>
       <c r="J29" s="95"/>
       <c r="K29" s="52"/>
-    </row>
-    <row r="30" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="N29" s="10"/>
+      <c r="O29" s="10"/>
+      <c r="P29" s="10"/>
+      <c r="Q29" s="99"/>
+      <c r="R29" s="8"/>
+      <c r="S29" s="95"/>
+      <c r="T29" s="52"/>
+      <c r="W29" s="17"/>
+      <c r="X29" s="10"/>
+      <c r="Y29" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z29" s="10"/>
+      <c r="AA29" s="99"/>
+      <c r="AB29" s="8"/>
+      <c r="AC29" s="95"/>
+      <c r="AD29" s="52"/>
+    </row>
+    <row r="30" spans="3:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C30" s="66"/>
       <c r="D30" s="17"/>
       <c r="E30" s="10"/>
@@ -5318,8 +5545,26 @@
       <c r="I30" s="8"/>
       <c r="J30" s="95"/>
       <c r="K30" s="52"/>
-    </row>
-    <row r="31" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M30" s="17"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="P30" s="10"/>
+      <c r="Q30" s="99"/>
+      <c r="R30" s="8"/>
+      <c r="S30" s="95"/>
+      <c r="T30" s="52"/>
+      <c r="W30" s="66"/>
+      <c r="X30" s="10"/>
+      <c r="Y30" s="10"/>
+      <c r="Z30" s="10"/>
+      <c r="AA30" s="12"/>
+      <c r="AB30" s="8"/>
+      <c r="AC30" s="97"/>
+      <c r="AD30" s="52"/>
+    </row>
+    <row r="31" spans="3:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C31" s="66"/>
       <c r="D31" s="66"/>
       <c r="E31" s="10"/>
@@ -5329,8 +5574,38 @@
       <c r="I31" s="8"/>
       <c r="J31" s="97"/>
       <c r="K31" s="52"/>
-    </row>
-    <row r="32" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M31" s="66"/>
+      <c r="N31" s="10"/>
+      <c r="O31" s="10"/>
+      <c r="P31" s="10"/>
+      <c r="Q31" s="12"/>
+      <c r="R31" s="8"/>
+      <c r="S31" s="97"/>
+      <c r="T31" s="52"/>
+      <c r="W31" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="X31" s="94" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y31" s="94" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z31" s="94" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA31" s="94" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB31" s="94" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC31" s="98" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD31" s="92"/>
+    </row>
+    <row r="32" spans="3:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C32" s="66"/>
       <c r="D32" s="2" t="s">
         <v>37</v>
@@ -5348,14 +5623,58 @@
         <v>9</v>
       </c>
       <c r="I32" s="94" t="s">
+        <v>41</v>
+      </c>
+      <c r="J32" s="98" t="s">
         <v>42</v>
       </c>
-      <c r="J32" s="98" t="s">
-        <v>43</v>
-      </c>
       <c r="K32" s="92"/>
-    </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="M32" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N32" s="94" t="s">
+        <v>7</v>
+      </c>
+      <c r="O32" s="94" t="s">
+        <v>11</v>
+      </c>
+      <c r="P32" s="94" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q32" s="94" t="s">
+        <v>9</v>
+      </c>
+      <c r="R32" s="94" t="s">
+        <v>41</v>
+      </c>
+      <c r="S32" s="98" t="s">
+        <v>42</v>
+      </c>
+      <c r="T32" s="92"/>
+      <c r="W32" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="X32" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y32" s="10">
+        <v>1</v>
+      </c>
+      <c r="Z32" s="10">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="AA32" s="12">
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="AB32" s="12">
+        <v>-3.1E-2</v>
+      </c>
+      <c r="AC32" s="95">
+        <v>34</v>
+      </c>
+      <c r="AD32" s="52"/>
+    </row>
+    <row r="33" spans="2:30" x14ac:dyDescent="0.2">
       <c r="C33" s="66"/>
       <c r="D33" s="16" t="s">
         <v>38</v>
@@ -5379,11 +5698,43 @@
         <v>32</v>
       </c>
       <c r="K33" s="52"/>
-    </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="M33" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="N33" s="10"/>
+      <c r="O33" s="10"/>
+      <c r="P33" s="10"/>
+      <c r="Q33" s="12"/>
+      <c r="R33" s="12"/>
+      <c r="S33" s="95"/>
+      <c r="T33" s="52"/>
+      <c r="W33" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="X33" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y33" s="10">
+        <v>1</v>
+      </c>
+      <c r="Z33" s="10">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="AA33" s="12">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="AB33" s="12">
+        <v>-2.46E-2</v>
+      </c>
+      <c r="AC33" s="95">
+        <v>34</v>
+      </c>
+      <c r="AD33" s="6"/>
+    </row>
+    <row r="34" spans="2:30" x14ac:dyDescent="0.2">
       <c r="C34" s="66"/>
       <c r="D34" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E34" s="10">
         <v>1</v>
@@ -5404,11 +5755,43 @@
         <v>34</v>
       </c>
       <c r="K34" s="6"/>
-    </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="M34" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="N34" s="10"/>
+      <c r="O34" s="10"/>
+      <c r="P34" s="10"/>
+      <c r="Q34" s="12"/>
+      <c r="R34" s="12"/>
+      <c r="S34" s="95"/>
+      <c r="T34" s="6"/>
+      <c r="W34" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="X34" s="10">
+        <v>2.5230000000000001</v>
+      </c>
+      <c r="Y34" s="10">
+        <v>3.1579999999999999</v>
+      </c>
+      <c r="Z34" s="10">
+        <v>0.90200000000000002</v>
+      </c>
+      <c r="AA34" s="8">
+        <v>0.504</v>
+      </c>
+      <c r="AB34" s="8">
+        <v>4.2599999999999999E-2</v>
+      </c>
+      <c r="AC34" s="95">
+        <v>34</v>
+      </c>
+      <c r="AD34" s="92"/>
+    </row>
+    <row r="35" spans="2:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C35" s="66"/>
       <c r="D35" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E35" s="10">
         <v>1</v>
@@ -5429,11 +5812,55 @@
         <v>30</v>
       </c>
       <c r="K35" s="92"/>
-    </row>
-    <row r="36" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M35" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="N35" s="10">
+        <v>6.7750000000000004</v>
+      </c>
+      <c r="O35" s="10">
+        <v>7.8250000000000002</v>
+      </c>
+      <c r="P35" s="10">
+        <v>2.415</v>
+      </c>
+      <c r="Q35" s="103">
+        <v>4.99E-2</v>
+      </c>
+      <c r="R35" s="8">
+        <v>0.36599999999999999</v>
+      </c>
+      <c r="S35" s="95">
+        <v>29</v>
+      </c>
+      <c r="T35" s="92"/>
+      <c r="W35" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="X35" s="11">
+        <v>4.4619999999999997</v>
+      </c>
+      <c r="Y35" s="11">
+        <v>5.375</v>
+      </c>
+      <c r="Z35" s="11">
+        <v>2.52</v>
+      </c>
+      <c r="AA35" s="101">
+        <v>4.8500000000000001E-2</v>
+      </c>
+      <c r="AB35" s="9">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="AC35" s="96">
+        <v>34</v>
+      </c>
+      <c r="AD35" s="52"/>
+    </row>
+    <row r="36" spans="2:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C36" s="66"/>
       <c r="D36" s="37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E36" s="11">
         <v>3.101</v>
@@ -5454,8 +5881,38 @@
         <v>34</v>
       </c>
       <c r="K36" s="52"/>
-    </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="M36" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="N36" s="11">
+        <v>2.9249999999999998</v>
+      </c>
+      <c r="O36" s="11">
+        <v>3.6440000000000001</v>
+      </c>
+      <c r="P36" s="11">
+        <v>3.0569999999999999</v>
+      </c>
+      <c r="Q36" s="101">
+        <v>3.5299999999999998E-2</v>
+      </c>
+      <c r="R36" s="9">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="S36" s="96">
+        <v>33</v>
+      </c>
+      <c r="T36" s="52"/>
+      <c r="W36" s="17"/>
+      <c r="X36" s="10"/>
+      <c r="Y36" s="10"/>
+      <c r="Z36" s="10"/>
+      <c r="AA36" s="12"/>
+      <c r="AB36" s="8"/>
+      <c r="AC36" s="92"/>
+      <c r="AD36" s="6"/>
+    </row>
+    <row r="37" spans="2:30" x14ac:dyDescent="0.2">
       <c r="C37" s="66"/>
       <c r="D37" s="17"/>
       <c r="E37" s="10"/>
@@ -5465,21 +5922,57 @@
       <c r="I37" s="8"/>
       <c r="J37" s="92"/>
       <c r="K37" s="6"/>
-    </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="M37" s="17"/>
+      <c r="N37" s="10"/>
+      <c r="O37" s="10"/>
+      <c r="P37" s="10"/>
+      <c r="Q37" s="12"/>
+      <c r="R37" s="8"/>
+      <c r="S37" s="92"/>
+      <c r="T37" s="6"/>
+      <c r="W37" s="17"/>
+      <c r="X37" s="10"/>
+      <c r="Y37" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z37" s="10"/>
+      <c r="AA37" s="12"/>
+      <c r="AB37" s="8"/>
+      <c r="AC37" s="92"/>
+      <c r="AD37" s="6"/>
+    </row>
+    <row r="38" spans="2:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C38" s="66"/>
       <c r="D38" s="17"/>
       <c r="E38" s="10"/>
       <c r="F38" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G38" s="10"/>
       <c r="H38" s="12"/>
       <c r="I38" s="8"/>
       <c r="J38" s="92"/>
       <c r="K38" s="6"/>
-    </row>
-    <row r="39" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M38" s="17"/>
+      <c r="N38" s="10"/>
+      <c r="O38" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="P38" s="10"/>
+      <c r="Q38" s="12"/>
+      <c r="R38" s="8"/>
+      <c r="S38" s="92"/>
+      <c r="T38" s="6"/>
+      <c r="W38" s="66"/>
+      <c r="X38" s="10"/>
+      <c r="Y38" s="10"/>
+      <c r="Z38" s="10"/>
+      <c r="AA38" s="12"/>
+      <c r="AB38" s="8"/>
+      <c r="AC38" s="97"/>
+      <c r="AD38" s="52"/>
+    </row>
+    <row r="39" spans="2:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B39" s="17"/>
       <c r="C39" s="66"/>
       <c r="D39" s="66"/>
@@ -5490,8 +5983,38 @@
       <c r="I39" s="8"/>
       <c r="J39" s="97"/>
       <c r="K39" s="52"/>
-    </row>
-    <row r="40" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M39" s="66"/>
+      <c r="N39" s="10"/>
+      <c r="O39" s="10"/>
+      <c r="P39" s="10"/>
+      <c r="Q39" s="12"/>
+      <c r="R39" s="8"/>
+      <c r="S39" s="97"/>
+      <c r="T39" s="52"/>
+      <c r="W39" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="X39" s="94" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y39" s="94" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z39" s="94" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA39" s="94" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB39" s="94" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC39" s="98" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD39" s="92"/>
+    </row>
+    <row r="40" spans="2:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C40" s="66"/>
       <c r="D40" s="2" t="s">
         <v>37</v>
@@ -5509,14 +6032,58 @@
         <v>9</v>
       </c>
       <c r="I40" s="94" t="s">
+        <v>41</v>
+      </c>
+      <c r="J40" s="98" t="s">
         <v>42</v>
       </c>
-      <c r="J40" s="98" t="s">
-        <v>43</v>
-      </c>
       <c r="K40" s="92"/>
-    </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="M40" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N40" s="94" t="s">
+        <v>7</v>
+      </c>
+      <c r="O40" s="94" t="s">
+        <v>11</v>
+      </c>
+      <c r="P40" s="94" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q40" s="94" t="s">
+        <v>9</v>
+      </c>
+      <c r="R40" s="94" t="s">
+        <v>41</v>
+      </c>
+      <c r="S40" s="98" t="s">
+        <v>42</v>
+      </c>
+      <c r="T40" s="92"/>
+      <c r="W40" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="X40" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y40" s="10">
+        <v>1</v>
+      </c>
+      <c r="Z40" s="10">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="AA40" s="12">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="AB40" s="12">
+        <v>-3.1E-2</v>
+      </c>
+      <c r="AC40" s="95">
+        <v>34</v>
+      </c>
+      <c r="AD40" s="52"/>
+    </row>
+    <row r="41" spans="2:30" x14ac:dyDescent="0.2">
       <c r="C41" s="66"/>
       <c r="D41" s="16" t="s">
         <v>38</v>
@@ -5540,11 +6107,43 @@
         <v>32</v>
       </c>
       <c r="K41" s="52"/>
-    </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="M41" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="N41" s="10"/>
+      <c r="O41" s="10"/>
+      <c r="P41" s="10"/>
+      <c r="Q41" s="12"/>
+      <c r="R41" s="12"/>
+      <c r="S41" s="95"/>
+      <c r="T41" s="52"/>
+      <c r="W41" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="X41" s="10">
+        <v>5.9409999999999998</v>
+      </c>
+      <c r="Y41" s="10">
+        <v>7.0739999999999998</v>
+      </c>
+      <c r="Z41" s="10">
+        <v>2.0369999999999999</v>
+      </c>
+      <c r="AA41" s="12">
+        <v>9.0300000000000005E-2</v>
+      </c>
+      <c r="AB41" s="12">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="AC41" s="95">
+        <v>34</v>
+      </c>
+      <c r="AD41" s="6"/>
+    </row>
+    <row r="42" spans="2:30" x14ac:dyDescent="0.2">
       <c r="C42" s="66"/>
       <c r="D42" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E42" s="10">
         <v>1.704</v>
@@ -5565,11 +6164,43 @@
         <v>34</v>
       </c>
       <c r="K42" s="6"/>
-    </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="M42" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="N42" s="10"/>
+      <c r="O42" s="10"/>
+      <c r="P42" s="10"/>
+      <c r="Q42" s="12"/>
+      <c r="R42" s="12"/>
+      <c r="S42" s="95"/>
+      <c r="T42" s="6"/>
+      <c r="W42" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="X42" s="10">
+        <v>6.2729999999999997</v>
+      </c>
+      <c r="Y42" s="10">
+        <v>7.3159999999999998</v>
+      </c>
+      <c r="Z42" s="10">
+        <v>1.5660000000000001</v>
+      </c>
+      <c r="AA42" s="12">
+        <v>0.186</v>
+      </c>
+      <c r="AB42" s="8">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="AC42" s="95">
+        <v>34</v>
+      </c>
+      <c r="AD42" s="92"/>
+    </row>
+    <row r="43" spans="2:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C43" s="66"/>
       <c r="D43" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E43" s="10">
         <v>1.258</v>
@@ -5590,11 +6221,43 @@
         <v>30</v>
       </c>
       <c r="K43" s="92"/>
-    </row>
-    <row r="44" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M43" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="N43" s="10"/>
+      <c r="O43" s="10"/>
+      <c r="P43" s="10"/>
+      <c r="Q43" s="12"/>
+      <c r="R43" s="8"/>
+      <c r="S43" s="95"/>
+      <c r="T43" s="92"/>
+      <c r="W43" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="X43" s="11">
+        <v>3.1709999999999998</v>
+      </c>
+      <c r="Y43" s="11">
+        <v>3.8809999999999998</v>
+      </c>
+      <c r="Z43" s="11">
+        <v>1.383</v>
+      </c>
+      <c r="AA43" s="9">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="AB43" s="9">
+        <v>9.6299999999999997E-2</v>
+      </c>
+      <c r="AC43" s="96">
+        <v>34</v>
+      </c>
+      <c r="AD43" s="52"/>
+    </row>
+    <row r="44" spans="2:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C44" s="66"/>
       <c r="D44" s="37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E44" s="11">
         <v>1.8839999999999999</v>
@@ -5615,8 +6278,26 @@
         <v>34</v>
       </c>
       <c r="K44" s="52"/>
-    </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="M44" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="N44" s="11"/>
+      <c r="O44" s="11"/>
+      <c r="P44" s="11"/>
+      <c r="Q44" s="106"/>
+      <c r="R44" s="9"/>
+      <c r="S44" s="96"/>
+      <c r="T44" s="52"/>
+      <c r="W44" s="17"/>
+      <c r="X44" s="10"/>
+      <c r="Y44" s="10"/>
+      <c r="Z44" s="10"/>
+      <c r="AA44" s="12"/>
+      <c r="AB44" s="8"/>
+      <c r="AC44" s="92"/>
+      <c r="AD44" s="6"/>
+    </row>
+    <row r="45" spans="2:30" x14ac:dyDescent="0.2">
       <c r="C45" s="66"/>
       <c r="D45" s="17"/>
       <c r="E45" s="10"/>
@@ -5626,21 +6307,57 @@
       <c r="I45" s="8"/>
       <c r="J45" s="92"/>
       <c r="K45" s="6"/>
-    </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="M45" s="17"/>
+      <c r="N45" s="10"/>
+      <c r="O45" s="10"/>
+      <c r="P45" s="10"/>
+      <c r="Q45" s="12"/>
+      <c r="R45" s="8"/>
+      <c r="S45" s="92"/>
+      <c r="T45" s="6"/>
+      <c r="W45" s="17"/>
+      <c r="X45" s="10"/>
+      <c r="Y45" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z45" s="10"/>
+      <c r="AA45" s="12"/>
+      <c r="AB45" s="8"/>
+      <c r="AC45" s="92"/>
+      <c r="AD45" s="6"/>
+    </row>
+    <row r="46" spans="2:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C46" s="66"/>
       <c r="D46" s="17"/>
       <c r="E46" s="10"/>
       <c r="F46" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G46" s="10"/>
       <c r="H46" s="12"/>
       <c r="I46" s="8"/>
       <c r="J46" s="92"/>
       <c r="K46" s="6"/>
-    </row>
-    <row r="47" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M46" s="17"/>
+      <c r="N46" s="10"/>
+      <c r="O46" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="P46" s="10"/>
+      <c r="Q46" s="12"/>
+      <c r="R46" s="8"/>
+      <c r="S46" s="92"/>
+      <c r="T46" s="6"/>
+      <c r="W46" s="66"/>
+      <c r="X46" s="10"/>
+      <c r="Y46" s="10"/>
+      <c r="Z46" s="10"/>
+      <c r="AA46" s="12"/>
+      <c r="AB46" s="8"/>
+      <c r="AC46" s="97"/>
+      <c r="AD46" s="52"/>
+    </row>
+    <row r="47" spans="2:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C47" s="66"/>
       <c r="D47" s="66"/>
       <c r="E47" s="10"/>
@@ -5650,8 +6367,38 @@
       <c r="I47" s="8"/>
       <c r="J47" s="97"/>
       <c r="K47" s="52"/>
-    </row>
-    <row r="48" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M47" s="66"/>
+      <c r="N47" s="10"/>
+      <c r="O47" s="10"/>
+      <c r="P47" s="10"/>
+      <c r="Q47" s="12"/>
+      <c r="R47" s="8"/>
+      <c r="S47" s="97"/>
+      <c r="T47" s="52"/>
+      <c r="W47" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="X47" s="94" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y47" s="94" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z47" s="94" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA47" s="94" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB47" s="94" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC47" s="98" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD47" s="92"/>
+    </row>
+    <row r="48" spans="2:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C48" s="66"/>
       <c r="D48" s="2" t="s">
         <v>37</v>
@@ -5669,14 +6416,58 @@
         <v>9</v>
       </c>
       <c r="I48" s="94" t="s">
+        <v>41</v>
+      </c>
+      <c r="J48" s="98" t="s">
         <v>42</v>
       </c>
-      <c r="J48" s="98" t="s">
-        <v>43</v>
-      </c>
       <c r="K48" s="92"/>
-    </row>
-    <row r="49" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="M48" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N48" s="94" t="s">
+        <v>7</v>
+      </c>
+      <c r="O48" s="94" t="s">
+        <v>11</v>
+      </c>
+      <c r="P48" s="94" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q48" s="94" t="s">
+        <v>9</v>
+      </c>
+      <c r="R48" s="94" t="s">
+        <v>41</v>
+      </c>
+      <c r="S48" s="98" t="s">
+        <v>42</v>
+      </c>
+      <c r="T48" s="92"/>
+      <c r="W48" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="X48" s="10">
+        <v>1.4610000000000001</v>
+      </c>
+      <c r="Y48" s="10">
+        <v>1.7909999999999999</v>
+      </c>
+      <c r="Z48" s="10">
+        <v>1.6459999999999999</v>
+      </c>
+      <c r="AA48" s="10">
+        <v>0.159</v>
+      </c>
+      <c r="AB48" s="12">
+        <v>9.3100000000000002E-2</v>
+      </c>
+      <c r="AC48" s="95">
+        <v>29</v>
+      </c>
+      <c r="AD48" s="52"/>
+    </row>
+    <row r="49" spans="3:30" x14ac:dyDescent="0.2">
       <c r="C49" s="66"/>
       <c r="D49" s="16" t="s">
         <v>38</v>
@@ -5700,11 +6491,55 @@
         <v>27</v>
       </c>
       <c r="K49" s="52"/>
-    </row>
-    <row r="50" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="M49" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="N49" s="10">
+        <v>1</v>
+      </c>
+      <c r="O49" s="10">
+        <v>1</v>
+      </c>
+      <c r="P49" s="10">
+        <v>9.7539999999999996</v>
+      </c>
+      <c r="Q49" s="103">
+        <v>4.4799999999999996E-3</v>
+      </c>
+      <c r="R49" s="12">
+        <v>0.252</v>
+      </c>
+      <c r="S49" s="95">
+        <v>27</v>
+      </c>
+      <c r="T49" s="52"/>
+      <c r="W49" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="X49" s="10">
+        <v>2.7370000000000001</v>
+      </c>
+      <c r="Y49" s="10">
+        <v>3.4319999999999999</v>
+      </c>
+      <c r="Z49" s="10">
+        <v>6.13</v>
+      </c>
+      <c r="AA49" s="103">
+        <v>2.1800000000000001E-3</v>
+      </c>
+      <c r="AB49" s="12">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="AC49" s="95">
+        <v>29</v>
+      </c>
+      <c r="AD49" s="6"/>
+    </row>
+    <row r="50" spans="3:30" x14ac:dyDescent="0.2">
       <c r="C50" s="66"/>
       <c r="D50" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E50" s="10">
         <v>1</v>
@@ -5725,11 +6560,43 @@
         <v>29</v>
       </c>
       <c r="K50" s="6"/>
-    </row>
-    <row r="51" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="M50" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="N50" s="10"/>
+      <c r="O50" s="10"/>
+      <c r="P50" s="10"/>
+      <c r="Q50" s="12"/>
+      <c r="R50" s="12"/>
+      <c r="S50" s="95"/>
+      <c r="T50" s="6"/>
+      <c r="W50" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="X50" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y50" s="10">
+        <v>1</v>
+      </c>
+      <c r="Z50" s="10">
+        <v>3.0960000000000001</v>
+      </c>
+      <c r="AA50" s="102">
+        <v>8.9800000000000005E-2</v>
+      </c>
+      <c r="AB50" s="8">
+        <v>6.9699999999999998E-2</v>
+      </c>
+      <c r="AC50" s="95">
+        <v>29</v>
+      </c>
+      <c r="AD50" s="92"/>
+    </row>
+    <row r="51" spans="3:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C51" s="66"/>
       <c r="D51" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E51" s="10">
         <v>1.76</v>
@@ -5750,11 +6617,43 @@
         <v>26</v>
       </c>
       <c r="K51" s="92"/>
-    </row>
-    <row r="52" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M51" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="N51" s="10"/>
+      <c r="O51" s="10"/>
+      <c r="P51" s="10"/>
+      <c r="Q51" s="12"/>
+      <c r="R51" s="8"/>
+      <c r="S51" s="95"/>
+      <c r="T51" s="92"/>
+      <c r="W51" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="X51" s="11">
+        <v>3.3290000000000002</v>
+      </c>
+      <c r="Y51" s="11">
+        <v>4.0529999999999999</v>
+      </c>
+      <c r="Z51" s="11">
+        <v>3.2890000000000001</v>
+      </c>
+      <c r="AA51" s="11">
+        <v>2.5600000000000001E-2</v>
+      </c>
+      <c r="AB51" s="9">
+        <v>0.29599999999999999</v>
+      </c>
+      <c r="AC51" s="96">
+        <v>29</v>
+      </c>
+      <c r="AD51" s="52"/>
+    </row>
+    <row r="52" spans="3:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C52" s="66"/>
       <c r="D52" s="37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E52" s="11">
         <v>1.8240000000000001</v>
@@ -5775,8 +6674,38 @@
         <v>29</v>
       </c>
       <c r="K52" s="52"/>
-    </row>
-    <row r="53" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="M52" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="N52" s="11">
+        <v>1.27</v>
+      </c>
+      <c r="O52" s="11">
+        <v>1.4890000000000001</v>
+      </c>
+      <c r="P52" s="11">
+        <v>13.07</v>
+      </c>
+      <c r="Q52" s="100">
+        <v>8.1800000000000004E-4</v>
+      </c>
+      <c r="R52" s="9">
+        <v>0.377</v>
+      </c>
+      <c r="S52" s="96">
+        <v>29</v>
+      </c>
+      <c r="T52" s="52"/>
+      <c r="W52" s="17"/>
+      <c r="X52" s="10"/>
+      <c r="Y52" s="10"/>
+      <c r="Z52" s="10"/>
+      <c r="AA52" s="12"/>
+      <c r="AB52" s="8"/>
+      <c r="AC52" s="92"/>
+      <c r="AD52" s="6"/>
+    </row>
+    <row r="53" spans="3:30" x14ac:dyDescent="0.2">
       <c r="C53" s="66"/>
       <c r="D53" s="17"/>
       <c r="E53" s="10"/>
@@ -5786,13 +6715,23 @@
       <c r="I53" s="8"/>
       <c r="J53" s="92"/>
       <c r="K53" s="6"/>
+      <c r="M53" s="17"/>
+      <c r="N53" s="10"/>
+      <c r="O53" s="10"/>
+      <c r="P53" s="10"/>
+      <c r="Q53" s="12"/>
+      <c r="R53" s="8"/>
+      <c r="S53" s="92"/>
+      <c r="T53" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="M14:S16"/>
+    <mergeCell ref="W14:AC16"/>
     <mergeCell ref="D17:D20"/>
     <mergeCell ref="D5:D8"/>
     <mergeCell ref="D9:D12"/>
-    <mergeCell ref="D13:D16"/>
+    <mergeCell ref="D13:J15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding in AIC results from GAM sat and insitu
</commit_message>
<xml_diff>
--- a/K4S_key_scripts/K4S_DA_Aims/K4S_DA_A2/K4S_DA_A2/K4S_DA_A2_GAM_Temporal_Results.xlsx
+++ b/K4S_key_scripts/K4S_DA_Aims/K4S_DA_A2/K4S_DA_A2/K4S_DA_A2_GAM_Temporal_Results.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoestarkey/Desktop/Honours/Data_Analysis/K_axis_midoc/K4S_key_scripts/K4S_DA_Aims/K4S_DA_A2/K4S_DA_A2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D0CBF2-1D20-B041-AEBA-5C259C60B76F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB794F6-C50E-5E42-AAFB-BC0EE85659A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="38400" windowHeight="19400" activeTab="2" xr2:uid="{33E5A15D-DBA6-5B40-873E-91FBDBF28531}"/>
+    <workbookView xWindow="3940" yWindow="780" windowWidth="34200" windowHeight="19400" activeTab="4" xr2:uid="{33E5A15D-DBA6-5B40-873E-91FBDBF28531}"/>
   </bookViews>
   <sheets>
     <sheet name="GAM_Temporal_Sum" sheetId="1" r:id="rId1"/>
     <sheet name="GAM_Temporal_Depth_Before_Refit" sheetId="2" r:id="rId2"/>
     <sheet name="GAM_Temporal_Depth_After_Refit" sheetId="4" r:id="rId3"/>
     <sheet name="GAM_Sat+Insitu_Sum" sheetId="3" r:id="rId4"/>
+    <sheet name="GAM_Sat+Insitu_Additive_models" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="68">
   <si>
     <t>Season</t>
   </si>
@@ -227,6 +228,36 @@
   <si>
     <t>Salinity Max</t>
   </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>TAXA</t>
+  </si>
+  <si>
+    <t>SST</t>
+  </si>
+  <si>
+    <t>TSM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model </t>
+  </si>
+  <si>
+    <t>AIC</t>
+  </si>
+  <si>
+    <t>All Taxa</t>
+  </si>
+  <si>
+    <t>Tmin + O2_min</t>
+  </si>
+  <si>
+    <t>With SST outliers removed</t>
+  </si>
+  <si>
+    <t>With SST outliers kept in</t>
+  </si>
 </sst>
 </file>
 
@@ -283,7 +314,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -338,8 +369,14 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -427,11 +464,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -713,23 +786,47 @@
     <xf numFmtId="11" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="11" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -737,12 +834,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -752,24 +843,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -779,15 +855,43 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1214,7 +1318,7 @@
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="107" t="s">
+      <c r="B5" s="108" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -1238,7 +1342,7 @@
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="107"/>
+      <c r="B6" s="108"/>
       <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
@@ -1260,7 +1364,7 @@
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="107"/>
+      <c r="B7" s="108"/>
       <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1282,7 +1386,7 @@
       </c>
     </row>
     <row r="8" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="108"/>
+      <c r="B8" s="109"/>
       <c r="C8" s="5" t="s">
         <v>12</v>
       </c>
@@ -1304,7 +1408,7 @@
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="107" t="s">
+      <c r="B9" s="108" t="s">
         <v>1</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -1328,7 +1432,7 @@
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="107"/>
+      <c r="B10" s="108"/>
       <c r="C10" s="3" t="s">
         <v>5</v>
       </c>
@@ -1350,7 +1454,7 @@
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="107"/>
+      <c r="B11" s="108"/>
       <c r="C11" s="3" t="s">
         <v>6</v>
       </c>
@@ -1372,7 +1476,7 @@
       </c>
     </row>
     <row r="12" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="108"/>
+      <c r="B12" s="109"/>
       <c r="C12" s="5" t="s">
         <v>12</v>
       </c>
@@ -1394,7 +1498,7 @@
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B13" s="107" t="s">
+      <c r="B13" s="108" t="s">
         <v>2</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1418,7 +1522,7 @@
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B14" s="107"/>
+      <c r="B14" s="108"/>
       <c r="C14" s="3" t="s">
         <v>5</v>
       </c>
@@ -1440,7 +1544,7 @@
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B15" s="107"/>
+      <c r="B15" s="108"/>
       <c r="C15" s="3" t="s">
         <v>6</v>
       </c>
@@ -1462,7 +1566,7 @@
       </c>
     </row>
     <row r="16" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="108"/>
+      <c r="B16" s="109"/>
       <c r="C16" s="5" t="s">
         <v>12</v>
       </c>
@@ -1551,10 +1655,10 @@
       </c>
     </row>
     <row r="6" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C6" s="107" t="s">
+      <c r="C6" s="108" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="115" t="s">
+      <c r="D6" s="111" t="s">
         <v>15</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -1567,8 +1671,8 @@
       <c r="J6" s="8"/>
     </row>
     <row r="7" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="107"/>
-      <c r="D7" s="116"/>
+      <c r="C7" s="108"/>
+      <c r="D7" s="112"/>
       <c r="E7" s="3" t="s">
         <v>17</v>
       </c>
@@ -1579,8 +1683,8 @@
       <c r="J7" s="8"/>
     </row>
     <row r="8" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C8" s="107"/>
-      <c r="D8" s="116"/>
+      <c r="C8" s="108"/>
+      <c r="D8" s="112"/>
       <c r="E8" s="3" t="s">
         <v>18</v>
       </c>
@@ -1591,8 +1695,8 @@
       <c r="J8" s="8"/>
     </row>
     <row r="9" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="107"/>
-      <c r="D9" s="116"/>
+      <c r="C9" s="108"/>
+      <c r="D9" s="112"/>
       <c r="E9" s="3" t="s">
         <v>19</v>
       </c>
@@ -1603,8 +1707,8 @@
       <c r="J9" s="8"/>
     </row>
     <row r="10" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="107"/>
-      <c r="D10" s="116"/>
+      <c r="C10" s="108"/>
+      <c r="D10" s="112"/>
       <c r="E10" s="3" t="s">
         <v>20</v>
       </c>
@@ -1615,7 +1719,7 @@
       <c r="J10" s="8"/>
     </row>
     <row r="11" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C11" s="107"/>
+      <c r="C11" s="108"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="10"/>
@@ -1625,7 +1729,7 @@
       <c r="J11" s="8"/>
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C12" s="107"/>
+      <c r="C12" s="108"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="10"/>
@@ -1635,7 +1739,7 @@
       <c r="J12" s="8"/>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C13" s="107"/>
+      <c r="C13" s="108"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="10"/>
@@ -1645,7 +1749,7 @@
       <c r="J13" s="8"/>
     </row>
     <row r="14" spans="3:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="108"/>
+      <c r="C14" s="109"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="11"/>
@@ -1655,7 +1759,7 @@
       <c r="J14" s="14"/>
     </row>
     <row r="15" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C15" s="107" t="s">
+      <c r="C15" s="108" t="s">
         <v>1</v>
       </c>
       <c r="D15" s="3"/>
@@ -1667,7 +1771,7 @@
       <c r="J15" s="15"/>
     </row>
     <row r="16" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C16" s="107"/>
+      <c r="C16" s="108"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="10"/>
@@ -1677,7 +1781,7 @@
       <c r="J16" s="8"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C17" s="107"/>
+      <c r="C17" s="108"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="10"/>
@@ -1687,7 +1791,7 @@
       <c r="J17" s="8"/>
     </row>
     <row r="18" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="108"/>
+      <c r="C18" s="109"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="11"/>
@@ -1697,7 +1801,7 @@
       <c r="J18" s="13"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C19" s="107" t="s">
+      <c r="C19" s="108" t="s">
         <v>2</v>
       </c>
       <c r="D19" s="3"/>
@@ -1709,7 +1813,7 @@
       <c r="J19" s="8"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C20" s="107"/>
+      <c r="C20" s="108"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="10"/>
@@ -1719,7 +1823,7 @@
       <c r="J20" s="8"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C21" s="107"/>
+      <c r="C21" s="108"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="10"/>
@@ -1729,7 +1833,7 @@
       <c r="J21" s="8"/>
     </row>
     <row r="22" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="108"/>
+      <c r="C22" s="109"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="11"/>
@@ -1741,26 +1845,26 @@
     <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B26" s="66"/>
       <c r="C26" s="66"/>
-      <c r="D26" s="109" t="s">
+      <c r="D26" s="113" t="s">
         <v>48</v>
       </c>
-      <c r="E26" s="109"/>
-      <c r="F26" s="109"/>
-      <c r="G26" s="109"/>
-      <c r="H26" s="109"/>
-      <c r="I26" s="109"/>
-      <c r="J26" s="109"/>
+      <c r="E26" s="113"/>
+      <c r="F26" s="113"/>
+      <c r="G26" s="113"/>
+      <c r="H26" s="113"/>
+      <c r="I26" s="113"/>
+      <c r="J26" s="113"/>
       <c r="K26" s="66"/>
     </row>
     <row r="27" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" s="66"/>
-      <c r="C27" s="125"/>
-      <c r="D27" s="125"/>
-      <c r="E27" s="125"/>
-      <c r="F27" s="125"/>
-      <c r="G27" s="125"/>
-      <c r="H27" s="125"/>
-      <c r="I27" s="125"/>
+      <c r="C27" s="110"/>
+      <c r="D27" s="110"/>
+      <c r="E27" s="110"/>
+      <c r="F27" s="110"/>
+      <c r="G27" s="110"/>
+      <c r="H27" s="110"/>
+      <c r="I27" s="110"/>
       <c r="J27" s="66"/>
       <c r="K27" s="66"/>
     </row>
@@ -1792,7 +1896,7 @@
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B29" s="66"/>
-      <c r="C29" s="110" t="s">
+      <c r="C29" s="118" t="s">
         <v>0</v>
       </c>
       <c r="D29" s="33" t="s">
@@ -1821,7 +1925,7 @@
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B30" s="66"/>
-      <c r="C30" s="111"/>
+      <c r="C30" s="117"/>
       <c r="D30" s="33" t="s">
         <v>22</v>
       </c>
@@ -1848,7 +1952,7 @@
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B31" s="66"/>
-      <c r="C31" s="111"/>
+      <c r="C31" s="117"/>
       <c r="D31" s="33" t="s">
         <v>6</v>
       </c>
@@ -1875,8 +1979,8 @@
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B32" s="66"/>
-      <c r="C32" s="111"/>
-      <c r="D32" s="111" t="s">
+      <c r="C32" s="117"/>
+      <c r="D32" s="117" t="s">
         <v>24</v>
       </c>
       <c r="E32" s="3" t="s">
@@ -1902,8 +2006,8 @@
     </row>
     <row r="33" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B33" s="66"/>
-      <c r="C33" s="111"/>
-      <c r="D33" s="111"/>
+      <c r="C33" s="117"/>
+      <c r="D33" s="117"/>
       <c r="E33" s="3" t="s">
         <v>20</v>
       </c>
@@ -1930,10 +2034,10 @@
     </row>
     <row r="34" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B34" s="66"/>
-      <c r="C34" s="112" t="s">
-        <v>1</v>
-      </c>
-      <c r="D34" s="112" t="s">
+      <c r="C34" s="114" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" s="114" t="s">
         <v>15</v>
       </c>
       <c r="E34" s="22" t="s">
@@ -1959,8 +2063,8 @@
     </row>
     <row r="35" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B35" s="66"/>
-      <c r="C35" s="107"/>
-      <c r="D35" s="120"/>
+      <c r="C35" s="108"/>
+      <c r="D35" s="115"/>
       <c r="E35" s="26" t="s">
         <v>20</v>
       </c>
@@ -1984,8 +2088,8 @@
     </row>
     <row r="36" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B36" s="66"/>
-      <c r="C36" s="107"/>
-      <c r="D36" s="121" t="s">
+      <c r="C36" s="108"/>
+      <c r="D36" s="116" t="s">
         <v>22</v>
       </c>
       <c r="E36" s="29" t="s">
@@ -2011,8 +2115,8 @@
     </row>
     <row r="37" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B37" s="66"/>
-      <c r="C37" s="107"/>
-      <c r="D37" s="120"/>
+      <c r="C37" s="108"/>
+      <c r="D37" s="115"/>
       <c r="E37" s="32" t="s">
         <v>20</v>
       </c>
@@ -2036,7 +2140,7 @@
     </row>
     <row r="38" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B38" s="66"/>
-      <c r="C38" s="107"/>
+      <c r="C38" s="108"/>
       <c r="D38" s="33" t="s">
         <v>6</v>
       </c>
@@ -2063,7 +2167,7 @@
     </row>
     <row r="39" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B39" s="66"/>
-      <c r="C39" s="108"/>
+      <c r="C39" s="109"/>
       <c r="D39" s="5" t="s">
         <v>24</v>
       </c>
@@ -2090,7 +2194,7 @@
     </row>
     <row r="40" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B40" s="66"/>
-      <c r="C40" s="112" t="s">
+      <c r="C40" s="114" t="s">
         <v>2</v>
       </c>
       <c r="D40" s="33" t="s">
@@ -2119,7 +2223,7 @@
     </row>
     <row r="41" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B41" s="66"/>
-      <c r="C41" s="107"/>
+      <c r="C41" s="108"/>
       <c r="D41" s="33" t="s">
         <v>22</v>
       </c>
@@ -2146,7 +2250,7 @@
     </row>
     <row r="42" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B42" s="66"/>
-      <c r="C42" s="107"/>
+      <c r="C42" s="108"/>
       <c r="D42" s="33" t="s">
         <v>6</v>
       </c>
@@ -2160,7 +2264,7 @@
     </row>
     <row r="43" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B43" s="66"/>
-      <c r="C43" s="108"/>
+      <c r="C43" s="109"/>
       <c r="D43" s="5" t="s">
         <v>24</v>
       </c>
@@ -2214,26 +2318,26 @@
     </row>
     <row r="47" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C47" s="66"/>
-      <c r="D47" s="109" t="s">
+      <c r="D47" s="113" t="s">
         <v>47</v>
       </c>
-      <c r="E47" s="109"/>
-      <c r="F47" s="109"/>
-      <c r="G47" s="109"/>
-      <c r="H47" s="109"/>
-      <c r="I47" s="109"/>
-      <c r="J47" s="109"/>
+      <c r="E47" s="113"/>
+      <c r="F47" s="113"/>
+      <c r="G47" s="113"/>
+      <c r="H47" s="113"/>
+      <c r="I47" s="113"/>
+      <c r="J47" s="113"/>
       <c r="K47" s="66"/>
       <c r="P47" s="66"/>
-      <c r="Q47" s="109" t="s">
+      <c r="Q47" s="113" t="s">
         <v>49</v>
       </c>
-      <c r="R47" s="109"/>
-      <c r="S47" s="109"/>
-      <c r="T47" s="109"/>
-      <c r="U47" s="109"/>
-      <c r="V47" s="109"/>
-      <c r="W47" s="109"/>
+      <c r="R47" s="113"/>
+      <c r="S47" s="113"/>
+      <c r="T47" s="113"/>
+      <c r="U47" s="113"/>
+      <c r="V47" s="113"/>
+      <c r="W47" s="113"/>
       <c r="X47" s="66"/>
     </row>
     <row r="48" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2310,7 +2414,7 @@
     </row>
     <row r="50" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B50" s="66"/>
-      <c r="C50" s="110" t="s">
+      <c r="C50" s="118" t="s">
         <v>0</v>
       </c>
       <c r="D50" s="33" t="s">
@@ -2337,7 +2441,7 @@
       </c>
       <c r="K50" s="66"/>
       <c r="O50" s="66"/>
-      <c r="P50" s="110" t="s">
+      <c r="P50" s="118" t="s">
         <v>0</v>
       </c>
       <c r="Q50" s="33" t="s">
@@ -2366,7 +2470,7 @@
     </row>
     <row r="51" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B51" s="66"/>
-      <c r="C51" s="111"/>
+      <c r="C51" s="117"/>
       <c r="D51" s="33" t="s">
         <v>5</v>
       </c>
@@ -2391,7 +2495,7 @@
       </c>
       <c r="K51" s="66"/>
       <c r="O51" s="66"/>
-      <c r="P51" s="111"/>
+      <c r="P51" s="117"/>
       <c r="Q51" s="33" t="s">
         <v>5</v>
       </c>
@@ -2418,7 +2522,7 @@
     </row>
     <row r="52" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B52" s="66"/>
-      <c r="C52" s="111"/>
+      <c r="C52" s="117"/>
       <c r="D52" s="33" t="s">
         <v>6</v>
       </c>
@@ -2443,7 +2547,7 @@
       </c>
       <c r="K52" s="66"/>
       <c r="O52" s="66"/>
-      <c r="P52" s="111"/>
+      <c r="P52" s="117"/>
       <c r="Q52" s="33" t="s">
         <v>6</v>
       </c>
@@ -2470,7 +2574,7 @@
     </row>
     <row r="53" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B53" s="66"/>
-      <c r="C53" s="111"/>
+      <c r="C53" s="117"/>
       <c r="D53" s="17" t="s">
         <v>24</v>
       </c>
@@ -2484,7 +2588,7 @@
       <c r="J53" s="88"/>
       <c r="K53" s="66"/>
       <c r="O53" s="66"/>
-      <c r="P53" s="111"/>
+      <c r="P53" s="117"/>
       <c r="Q53" s="17" t="s">
         <v>24</v>
       </c>
@@ -2500,10 +2604,10 @@
     </row>
     <row r="54" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B54" s="66"/>
-      <c r="C54" s="112" t="s">
-        <v>1</v>
-      </c>
-      <c r="D54" s="110" t="s">
+      <c r="C54" s="114" t="s">
+        <v>1</v>
+      </c>
+      <c r="D54" s="118" t="s">
         <v>25</v>
       </c>
       <c r="E54" s="22" t="s">
@@ -2527,10 +2631,10 @@
       </c>
       <c r="K54" s="66"/>
       <c r="O54" s="66"/>
-      <c r="P54" s="112" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q54" s="110" t="s">
+      <c r="P54" s="114" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q54" s="118" t="s">
         <v>25</v>
       </c>
       <c r="R54" s="22" t="s">
@@ -2556,8 +2660,8 @@
     </row>
     <row r="55" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B55" s="66"/>
-      <c r="C55" s="107"/>
-      <c r="D55" s="113"/>
+      <c r="C55" s="108"/>
+      <c r="D55" s="121"/>
       <c r="E55" s="26" t="s">
         <v>26</v>
       </c>
@@ -2579,8 +2683,8 @@
       </c>
       <c r="K55" s="66"/>
       <c r="O55" s="66"/>
-      <c r="P55" s="107"/>
-      <c r="Q55" s="113"/>
+      <c r="P55" s="108"/>
+      <c r="Q55" s="121"/>
       <c r="R55" s="26" t="s">
         <v>26</v>
       </c>
@@ -2604,8 +2708,8 @@
     </row>
     <row r="56" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B56" s="66"/>
-      <c r="C56" s="107"/>
-      <c r="D56" s="114" t="s">
+      <c r="C56" s="108"/>
+      <c r="D56" s="122" t="s">
         <v>5</v>
       </c>
       <c r="E56" s="29" t="s">
@@ -2629,8 +2733,8 @@
       </c>
       <c r="K56" s="66"/>
       <c r="O56" s="66"/>
-      <c r="P56" s="107"/>
-      <c r="Q56" s="114" t="s">
+      <c r="P56" s="108"/>
+      <c r="Q56" s="122" t="s">
         <v>5</v>
       </c>
       <c r="R56" s="29" t="s">
@@ -2656,8 +2760,8 @@
     </row>
     <row r="57" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B57" s="66"/>
-      <c r="C57" s="107"/>
-      <c r="D57" s="113"/>
+      <c r="C57" s="108"/>
+      <c r="D57" s="121"/>
       <c r="E57" s="32" t="s">
         <v>20</v>
       </c>
@@ -2679,8 +2783,8 @@
       </c>
       <c r="K57" s="66"/>
       <c r="O57" s="66"/>
-      <c r="P57" s="107"/>
-      <c r="Q57" s="113"/>
+      <c r="P57" s="108"/>
+      <c r="Q57" s="121"/>
       <c r="R57" s="32" t="s">
         <v>20</v>
       </c>
@@ -2704,7 +2808,7 @@
     </row>
     <row r="58" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B58" s="66"/>
-      <c r="C58" s="107"/>
+      <c r="C58" s="108"/>
       <c r="D58" s="33" t="s">
         <v>6</v>
       </c>
@@ -2729,7 +2833,7 @@
       </c>
       <c r="K58" s="66"/>
       <c r="O58" s="66"/>
-      <c r="P58" s="107"/>
+      <c r="P58" s="108"/>
       <c r="Q58" s="33" t="s">
         <v>6</v>
       </c>
@@ -2756,7 +2860,7 @@
     </row>
     <row r="59" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B59" s="66"/>
-      <c r="C59" s="108"/>
+      <c r="C59" s="109"/>
       <c r="D59" s="5" t="s">
         <v>24</v>
       </c>
@@ -2770,7 +2874,7 @@
       <c r="J59" s="88"/>
       <c r="K59" s="66"/>
       <c r="O59" s="66"/>
-      <c r="P59" s="108"/>
+      <c r="P59" s="109"/>
       <c r="Q59" s="5" t="s">
         <v>24</v>
       </c>
@@ -2786,7 +2890,7 @@
     </row>
     <row r="60" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B60" s="66"/>
-      <c r="C60" s="115" t="s">
+      <c r="C60" s="111" t="s">
         <v>2</v>
       </c>
       <c r="D60" s="33" t="s">
@@ -2813,7 +2917,7 @@
       </c>
       <c r="K60" s="66"/>
       <c r="O60" s="66"/>
-      <c r="P60" s="115" t="s">
+      <c r="P60" s="111" t="s">
         <v>2</v>
       </c>
       <c r="Q60" s="33" t="s">
@@ -2842,8 +2946,8 @@
     </row>
     <row r="61" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B61" s="66"/>
-      <c r="C61" s="116"/>
-      <c r="D61" s="114" t="s">
+      <c r="C61" s="112"/>
+      <c r="D61" s="122" t="s">
         <v>5</v>
       </c>
       <c r="E61" s="29" t="s">
@@ -2867,8 +2971,8 @@
       </c>
       <c r="K61" s="66"/>
       <c r="O61" s="66"/>
-      <c r="P61" s="116"/>
-      <c r="Q61" s="114" t="s">
+      <c r="P61" s="112"/>
+      <c r="Q61" s="122" t="s">
         <v>5</v>
       </c>
       <c r="R61" s="29" t="s">
@@ -2894,8 +2998,8 @@
     </row>
     <row r="62" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B62" s="66"/>
-      <c r="C62" s="116"/>
-      <c r="D62" s="113"/>
+      <c r="C62" s="112"/>
+      <c r="D62" s="121"/>
       <c r="E62" s="32" t="s">
         <v>18</v>
       </c>
@@ -2917,8 +3021,8 @@
       </c>
       <c r="K62" s="66"/>
       <c r="O62" s="66"/>
-      <c r="P62" s="116"/>
-      <c r="Q62" s="113"/>
+      <c r="P62" s="112"/>
+      <c r="Q62" s="121"/>
       <c r="R62" s="32" t="s">
         <v>18</v>
       </c>
@@ -2942,7 +3046,7 @@
     </row>
     <row r="63" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B63" s="66"/>
-      <c r="C63" s="116"/>
+      <c r="C63" s="112"/>
       <c r="D63" s="17" t="s">
         <v>6</v>
       </c>
@@ -2954,7 +3058,7 @@
       <c r="J63" s="42"/>
       <c r="K63" s="66"/>
       <c r="O63" s="66"/>
-      <c r="P63" s="116"/>
+      <c r="P63" s="112"/>
       <c r="Q63" s="17" t="s">
         <v>6</v>
       </c>
@@ -2968,7 +3072,7 @@
     </row>
     <row r="64" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B64" s="66"/>
-      <c r="C64" s="117"/>
+      <c r="C64" s="123"/>
       <c r="D64" s="5" t="s">
         <v>24</v>
       </c>
@@ -2982,7 +3086,7 @@
       <c r="J64" s="91"/>
       <c r="K64" s="66"/>
       <c r="O64" s="66"/>
-      <c r="P64" s="117"/>
+      <c r="P64" s="123"/>
       <c r="Q64" s="5" t="s">
         <v>24</v>
       </c>
@@ -3074,7 +3178,7 @@
     </row>
     <row r="71" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B71" s="66"/>
-      <c r="C71" s="110" t="s">
+      <c r="C71" s="118" t="s">
         <v>0</v>
       </c>
       <c r="D71" t="s">
@@ -3094,7 +3198,7 @@
     </row>
     <row r="72" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B72" s="66"/>
-      <c r="C72" s="111"/>
+      <c r="C72" s="117"/>
       <c r="D72" s="20" t="s">
         <v>28</v>
       </c>
@@ -3112,10 +3216,10 @@
     </row>
     <row r="73" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B73" s="66"/>
-      <c r="C73" s="112" t="s">
-        <v>1</v>
-      </c>
-      <c r="D73" s="112" t="s">
+      <c r="C73" s="114" t="s">
+        <v>1</v>
+      </c>
+      <c r="D73" s="114" t="s">
         <v>21</v>
       </c>
       <c r="E73" s="52" t="s">
@@ -3132,8 +3236,8 @@
     </row>
     <row r="74" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B74" s="66"/>
-      <c r="C74" s="107"/>
-      <c r="D74" s="120"/>
+      <c r="C74" s="108"/>
+      <c r="D74" s="115"/>
       <c r="E74" s="56" t="s">
         <v>20</v>
       </c>
@@ -3148,8 +3252,8 @@
     </row>
     <row r="75" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B75" s="66"/>
-      <c r="C75" s="107"/>
-      <c r="D75" s="121" t="s">
+      <c r="C75" s="108"/>
+      <c r="D75" s="116" t="s">
         <v>28</v>
       </c>
       <c r="E75" s="57" t="s">
@@ -3166,8 +3270,8 @@
     </row>
     <row r="76" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B76" s="66"/>
-      <c r="C76" s="107"/>
-      <c r="D76" s="108"/>
+      <c r="C76" s="108"/>
+      <c r="D76" s="109"/>
       <c r="E76" s="59" t="s">
         <v>20</v>
       </c>
@@ -3182,7 +3286,7 @@
     </row>
     <row r="77" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B77" s="66"/>
-      <c r="C77" s="123" t="s">
+      <c r="C77" s="119" t="s">
         <v>2</v>
       </c>
       <c r="D77" s="63" t="s">
@@ -3202,7 +3306,7 @@
     </row>
     <row r="78" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B78" s="66"/>
-      <c r="C78" s="124"/>
+      <c r="C78" s="120"/>
       <c r="D78" s="65" t="s">
         <v>28</v>
       </c>
@@ -3221,13 +3325,13 @@
     <row r="79" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B79" s="66"/>
       <c r="C79" s="61"/>
-      <c r="D79" s="122"/>
-      <c r="E79" s="122"/>
-      <c r="F79" s="122"/>
-      <c r="G79" s="122"/>
-      <c r="H79" s="122"/>
-      <c r="I79" s="122"/>
-      <c r="J79" s="122"/>
+      <c r="D79" s="126"/>
+      <c r="E79" s="126"/>
+      <c r="F79" s="126"/>
+      <c r="G79" s="126"/>
+      <c r="H79" s="126"/>
+      <c r="I79" s="126"/>
+      <c r="J79" s="126"/>
       <c r="K79" s="66"/>
     </row>
     <row r="80" spans="2:24" x14ac:dyDescent="0.2">
@@ -3296,7 +3400,7 @@
     </row>
     <row r="88" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B88" s="66"/>
-      <c r="C88" s="110" t="s">
+      <c r="C88" s="118" t="s">
         <v>0</v>
       </c>
       <c r="D88" t="s">
@@ -3316,7 +3420,7 @@
     </row>
     <row r="89" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B89" s="66"/>
-      <c r="C89" s="111"/>
+      <c r="C89" s="117"/>
       <c r="D89" s="20" t="s">
         <v>28</v>
       </c>
@@ -3334,10 +3438,10 @@
     </row>
     <row r="90" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B90" s="66"/>
-      <c r="C90" s="112" t="s">
-        <v>1</v>
-      </c>
-      <c r="D90" s="112" t="s">
+      <c r="C90" s="114" t="s">
+        <v>1</v>
+      </c>
+      <c r="D90" s="114" t="s">
         <v>21</v>
       </c>
       <c r="E90" s="29" t="s">
@@ -3354,8 +3458,8 @@
     </row>
     <row r="91" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B91" s="66"/>
-      <c r="C91" s="107"/>
-      <c r="D91" s="120"/>
+      <c r="C91" s="108"/>
+      <c r="D91" s="115"/>
       <c r="E91" s="32" t="s">
         <v>20</v>
       </c>
@@ -3370,8 +3474,8 @@
     </row>
     <row r="92" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B92" s="66"/>
-      <c r="C92" s="107"/>
-      <c r="D92" s="121" t="s">
+      <c r="C92" s="108"/>
+      <c r="D92" s="116" t="s">
         <v>28</v>
       </c>
       <c r="E92" s="29" t="s">
@@ -3388,8 +3492,8 @@
     </row>
     <row r="93" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B93" s="66"/>
-      <c r="C93" s="108"/>
-      <c r="D93" s="108"/>
+      <c r="C93" s="109"/>
+      <c r="D93" s="109"/>
       <c r="E93" s="20" t="s">
         <v>20</v>
       </c>
@@ -3404,7 +3508,7 @@
     </row>
     <row r="94" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B94" s="66"/>
-      <c r="C94" s="112" t="s">
+      <c r="C94" s="114" t="s">
         <v>2</v>
       </c>
       <c r="D94" s="63" t="s">
@@ -3424,7 +3528,7 @@
     </row>
     <row r="95" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B95" s="66"/>
-      <c r="C95" s="107"/>
+      <c r="C95" s="108"/>
       <c r="D95" s="52" t="s">
         <v>28</v>
       </c>
@@ -3442,7 +3546,7 @@
     </row>
     <row r="96" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B96" s="66"/>
-      <c r="C96" s="108"/>
+      <c r="C96" s="109"/>
       <c r="D96" s="67"/>
       <c r="E96" s="20" t="s">
         <v>18</v>
@@ -3499,7 +3603,7 @@
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B102" s="66"/>
-      <c r="C102" s="110" t="s">
+      <c r="C102" s="118" t="s">
         <v>0</v>
       </c>
       <c r="D102" t="s">
@@ -3519,7 +3623,7 @@
     </row>
     <row r="103" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B103" s="66"/>
-      <c r="C103" s="111"/>
+      <c r="C103" s="117"/>
       <c r="D103" s="20" t="s">
         <v>28</v>
       </c>
@@ -3537,7 +3641,7 @@
     </row>
     <row r="104" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B104" s="66"/>
-      <c r="C104" s="112" t="s">
+      <c r="C104" s="114" t="s">
         <v>1</v>
       </c>
       <c r="D104" s="16" t="s">
@@ -3557,7 +3661,7 @@
     </row>
     <row r="105" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B105" s="66"/>
-      <c r="C105" s="107"/>
+      <c r="C105" s="108"/>
       <c r="D105" s="43" t="s">
         <v>28</v>
       </c>
@@ -3575,7 +3679,7 @@
     </row>
     <row r="106" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B106" s="66"/>
-      <c r="C106" s="112" t="s">
+      <c r="C106" s="114" t="s">
         <v>2</v>
       </c>
       <c r="D106" s="63" t="s">
@@ -3593,7 +3697,7 @@
     </row>
     <row r="107" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B107" s="66"/>
-      <c r="C107" s="108"/>
+      <c r="C107" s="109"/>
       <c r="D107" s="65" t="s">
         <v>28</v>
       </c>
@@ -3678,7 +3782,7 @@
       <c r="C115" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D115" s="118" t="s">
+      <c r="D115" s="124" t="s">
         <v>21</v>
       </c>
       <c r="E115" s="76" t="s">
@@ -3695,7 +3799,7 @@
     <row r="116" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B116" s="66"/>
       <c r="C116" s="37"/>
-      <c r="D116" s="119"/>
+      <c r="D116" s="125"/>
       <c r="E116" s="80" t="s">
         <v>20</v>
       </c>
@@ -3788,26 +3892,11 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="C27:I27"/>
-    <mergeCell ref="C6:C14"/>
-    <mergeCell ref="C15:C18"/>
-    <mergeCell ref="C19:C22"/>
-    <mergeCell ref="D6:D10"/>
-    <mergeCell ref="D26:J26"/>
-    <mergeCell ref="C40:C43"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="C29:C33"/>
-    <mergeCell ref="C34:C39"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="D73:D74"/>
-    <mergeCell ref="C77:C78"/>
-    <mergeCell ref="D47:J47"/>
-    <mergeCell ref="C50:C53"/>
-    <mergeCell ref="C54:C59"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="Q47:W47"/>
+    <mergeCell ref="P50:P53"/>
+    <mergeCell ref="P54:P59"/>
+    <mergeCell ref="Q54:Q55"/>
+    <mergeCell ref="Q56:Q57"/>
     <mergeCell ref="P60:P64"/>
     <mergeCell ref="Q61:Q62"/>
     <mergeCell ref="D115:D116"/>
@@ -3824,11 +3913,26 @@
     <mergeCell ref="D79:J79"/>
     <mergeCell ref="C71:C72"/>
     <mergeCell ref="C73:C76"/>
-    <mergeCell ref="Q47:W47"/>
-    <mergeCell ref="P50:P53"/>
-    <mergeCell ref="P54:P59"/>
-    <mergeCell ref="Q54:Q55"/>
-    <mergeCell ref="Q56:Q57"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="D73:D74"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="D47:J47"/>
+    <mergeCell ref="C50:C53"/>
+    <mergeCell ref="C54:C59"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="C40:C43"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="C29:C33"/>
+    <mergeCell ref="C34:C39"/>
+    <mergeCell ref="C27:I27"/>
+    <mergeCell ref="C6:C14"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="C19:C22"/>
+    <mergeCell ref="D6:D10"/>
+    <mergeCell ref="D26:J26"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="J6:J22">
@@ -3845,7 +3949,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11EC7562-B833-6E47-893A-48CC2F5000AD}">
   <dimension ref="C6:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="88" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScale="88" workbookViewId="0">
       <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
@@ -3857,15 +3961,15 @@
   <sheetData>
     <row r="6" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C6" s="66"/>
-      <c r="D6" s="109" t="s">
+      <c r="D6" s="113" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="109"/>
-      <c r="F6" s="109"/>
-      <c r="G6" s="109"/>
-      <c r="H6" s="109"/>
-      <c r="I6" s="109"/>
-      <c r="J6" s="109"/>
+      <c r="E6" s="113"/>
+      <c r="F6" s="113"/>
+      <c r="G6" s="113"/>
+      <c r="H6" s="113"/>
+      <c r="I6" s="113"/>
+      <c r="J6" s="113"/>
       <c r="K6" s="66"/>
     </row>
     <row r="7" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3905,10 +4009,10 @@
       <c r="K8" s="66"/>
     </row>
     <row r="9" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C9" s="110" t="s">
+      <c r="C9" s="118" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="112" t="s">
+      <c r="D9" s="114" t="s">
         <v>25</v>
       </c>
       <c r="E9" s="34" t="s">
@@ -3932,8 +4036,8 @@
       <c r="K9" s="66"/>
     </row>
     <row r="10" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C10" s="111"/>
-      <c r="D10" s="120"/>
+      <c r="C10" s="117"/>
+      <c r="D10" s="115"/>
       <c r="E10" s="34" t="s">
         <v>20</v>
       </c>
@@ -3955,8 +4059,8 @@
       <c r="K10" s="66"/>
     </row>
     <row r="11" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C11" s="111"/>
-      <c r="D11" s="121" t="s">
+      <c r="C11" s="117"/>
+      <c r="D11" s="116" t="s">
         <v>5</v>
       </c>
       <c r="E11" s="34" t="s">
@@ -3980,8 +4084,8 @@
       <c r="K11" s="66"/>
     </row>
     <row r="12" spans="3:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C12" s="111"/>
-      <c r="D12" s="120"/>
+      <c r="C12" s="117"/>
+      <c r="D12" s="115"/>
       <c r="E12" s="34" t="s">
         <v>20</v>
       </c>
@@ -4003,7 +4107,7 @@
       <c r="K12" s="66"/>
     </row>
     <row r="13" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C13" s="111"/>
+      <c r="C13" s="117"/>
       <c r="D13" s="33" t="s">
         <v>6</v>
       </c>
@@ -4028,7 +4132,7 @@
       <c r="K13" s="66"/>
     </row>
     <row r="14" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="111"/>
+      <c r="C14" s="117"/>
       <c r="D14" s="17" t="s">
         <v>24</v>
       </c>
@@ -4043,10 +4147,10 @@
       <c r="K14" s="66"/>
     </row>
     <row r="15" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C15" s="112" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" s="110" t="s">
+      <c r="C15" s="114" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="118" t="s">
         <v>25</v>
       </c>
       <c r="E15" s="22" t="s">
@@ -4070,8 +4174,8 @@
       <c r="K15" s="66"/>
     </row>
     <row r="16" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="107"/>
-      <c r="D16" s="113"/>
+      <c r="C16" s="108"/>
+      <c r="D16" s="121"/>
       <c r="E16" s="26" t="s">
         <v>26</v>
       </c>
@@ -4093,8 +4197,8 @@
       <c r="K16" s="66"/>
     </row>
     <row r="17" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C17" s="107"/>
-      <c r="D17" s="114" t="s">
+      <c r="C17" s="108"/>
+      <c r="D17" s="122" t="s">
         <v>5</v>
       </c>
       <c r="E17" s="29" t="s">
@@ -4118,8 +4222,8 @@
       <c r="K17" s="66"/>
     </row>
     <row r="18" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C18" s="107"/>
-      <c r="D18" s="113"/>
+      <c r="C18" s="108"/>
+      <c r="D18" s="121"/>
       <c r="E18" s="32" t="s">
         <v>20</v>
       </c>
@@ -4141,8 +4245,8 @@
       <c r="K18" s="66"/>
     </row>
     <row r="19" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C19" s="107"/>
-      <c r="D19" s="121" t="s">
+      <c r="C19" s="108"/>
+      <c r="D19" s="116" t="s">
         <v>6</v>
       </c>
       <c r="E19" s="34" t="s">
@@ -4166,8 +4270,8 @@
       <c r="K19" s="66"/>
     </row>
     <row r="20" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C20" s="107"/>
-      <c r="D20" s="107"/>
+      <c r="C20" s="108"/>
+      <c r="D20" s="108"/>
       <c r="E20" s="3" t="s">
         <v>18</v>
       </c>
@@ -4189,7 +4293,7 @@
       <c r="K20" s="66"/>
     </row>
     <row r="21" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="108"/>
+      <c r="C21" s="109"/>
       <c r="D21" s="5" t="s">
         <v>24</v>
       </c>
@@ -4204,10 +4308,10 @@
       <c r="K21" s="66"/>
     </row>
     <row r="22" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C22" s="112" t="s">
+      <c r="C22" s="114" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="112" t="s">
+      <c r="D22" s="114" t="s">
         <v>25</v>
       </c>
       <c r="E22" t="s">
@@ -4231,8 +4335,8 @@
       <c r="K22" s="66"/>
     </row>
     <row r="23" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C23" s="107"/>
-      <c r="D23" s="107"/>
+      <c r="C23" s="108"/>
+      <c r="D23" s="108"/>
       <c r="E23" s="34" t="s">
         <v>17</v>
       </c>
@@ -4254,8 +4358,8 @@
       <c r="K23" s="66"/>
     </row>
     <row r="24" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C24" s="107"/>
-      <c r="D24" s="120"/>
+      <c r="C24" s="108"/>
+      <c r="D24" s="115"/>
       <c r="E24" s="104" t="s">
         <v>20</v>
       </c>
@@ -4277,8 +4381,8 @@
       <c r="K24" s="66"/>
     </row>
     <row r="25" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C25" s="107"/>
-      <c r="D25" s="114" t="s">
+      <c r="C25" s="108"/>
+      <c r="D25" s="122" t="s">
         <v>5</v>
       </c>
       <c r="E25" s="104" t="s">
@@ -4302,8 +4406,8 @@
       <c r="K25" s="66"/>
     </row>
     <row r="26" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C26" s="107"/>
-      <c r="D26" s="111"/>
+      <c r="C26" s="108"/>
+      <c r="D26" s="117"/>
       <c r="E26" s="29" t="s">
         <v>17</v>
       </c>
@@ -4325,8 +4429,8 @@
       <c r="K26" s="66"/>
     </row>
     <row r="27" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C27" s="107"/>
-      <c r="D27" s="111"/>
+      <c r="C27" s="108"/>
+      <c r="D27" s="117"/>
       <c r="E27" s="3" t="s">
         <v>18</v>
       </c>
@@ -4348,8 +4452,8 @@
       <c r="K27" s="66"/>
     </row>
     <row r="28" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C28" s="107"/>
-      <c r="D28" s="113"/>
+      <c r="C28" s="108"/>
+      <c r="D28" s="121"/>
       <c r="E28" s="32" t="s">
         <v>26</v>
       </c>
@@ -4371,7 +4475,7 @@
       <c r="K28" s="66"/>
     </row>
     <row r="29" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C29" s="107"/>
+      <c r="C29" s="108"/>
       <c r="D29" s="17" t="s">
         <v>6</v>
       </c>
@@ -4384,7 +4488,7 @@
       <c r="K29" s="66"/>
     </row>
     <row r="30" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C30" s="108"/>
+      <c r="C30" s="109"/>
       <c r="D30" s="5" t="s">
         <v>24</v>
       </c>
@@ -4411,15 +4515,15 @@
     </row>
     <row r="35" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C35" s="66"/>
-      <c r="D35" s="109" t="s">
+      <c r="D35" s="113" t="s">
         <v>49</v>
       </c>
-      <c r="E35" s="109"/>
-      <c r="F35" s="109"/>
-      <c r="G35" s="109"/>
-      <c r="H35" s="109"/>
-      <c r="I35" s="109"/>
-      <c r="J35" s="109"/>
+      <c r="E35" s="113"/>
+      <c r="F35" s="113"/>
+      <c r="G35" s="113"/>
+      <c r="H35" s="113"/>
+      <c r="I35" s="113"/>
+      <c r="J35" s="113"/>
       <c r="K35" s="66"/>
     </row>
     <row r="36" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4459,10 +4563,10 @@
       <c r="K37" s="66"/>
     </row>
     <row r="38" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C38" s="110" t="s">
+      <c r="C38" s="118" t="s">
         <v>0</v>
       </c>
-      <c r="D38" s="121" t="s">
+      <c r="D38" s="116" t="s">
         <v>5</v>
       </c>
       <c r="E38" s="21" t="s">
@@ -4486,8 +4590,8 @@
       <c r="K38" s="66"/>
     </row>
     <row r="39" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C39" s="111"/>
-      <c r="D39" s="120"/>
+      <c r="C39" s="117"/>
+      <c r="D39" s="115"/>
       <c r="E39" s="32" t="s">
         <v>20</v>
       </c>
@@ -4509,7 +4613,7 @@
       <c r="K39" s="66"/>
     </row>
     <row r="40" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C40" s="111"/>
+      <c r="C40" s="117"/>
       <c r="D40" s="33" t="s">
         <v>6</v>
       </c>
@@ -4534,7 +4638,7 @@
       <c r="K40" s="66"/>
     </row>
     <row r="41" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C41" s="126"/>
+      <c r="C41" s="127"/>
       <c r="D41" s="17" t="s">
         <v>24</v>
       </c>
@@ -4549,10 +4653,10 @@
       <c r="K41" s="66"/>
     </row>
     <row r="42" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C42" s="110" t="s">
-        <v>1</v>
-      </c>
-      <c r="D42" s="114" t="s">
+      <c r="C42" s="118" t="s">
+        <v>1</v>
+      </c>
+      <c r="D42" s="122" t="s">
         <v>5</v>
       </c>
       <c r="E42" s="29" t="s">
@@ -4576,8 +4680,8 @@
       <c r="K42" s="66"/>
     </row>
     <row r="43" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C43" s="111"/>
-      <c r="D43" s="113"/>
+      <c r="C43" s="117"/>
+      <c r="D43" s="121"/>
       <c r="E43" s="32" t="s">
         <v>20</v>
       </c>
@@ -4599,8 +4703,8 @@
       <c r="K43" s="66"/>
     </row>
     <row r="44" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C44" s="111"/>
-      <c r="D44" s="121" t="s">
+      <c r="C44" s="117"/>
+      <c r="D44" s="116" t="s">
         <v>6</v>
       </c>
       <c r="E44" s="34" t="s">
@@ -4624,8 +4728,8 @@
       <c r="K44" s="66"/>
     </row>
     <row r="45" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C45" s="111"/>
-      <c r="D45" s="107"/>
+      <c r="C45" s="117"/>
+      <c r="D45" s="108"/>
       <c r="E45" s="3" t="s">
         <v>18</v>
       </c>
@@ -4647,7 +4751,7 @@
       <c r="K45" s="66"/>
     </row>
     <row r="46" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C46" s="126"/>
+      <c r="C46" s="127"/>
       <c r="D46" s="5" t="s">
         <v>24</v>
       </c>
@@ -4662,10 +4766,10 @@
       <c r="K46" s="66"/>
     </row>
     <row r="47" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C47" s="110" t="s">
+      <c r="C47" s="118" t="s">
         <v>2</v>
       </c>
-      <c r="D47" s="114" t="s">
+      <c r="D47" s="122" t="s">
         <v>5</v>
       </c>
       <c r="E47" s="29" t="s">
@@ -4689,31 +4793,31 @@
       <c r="K47" s="66"/>
     </row>
     <row r="48" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C48" s="111"/>
-      <c r="D48" s="111"/>
-      <c r="E48" s="129" t="s">
+      <c r="C48" s="117"/>
+      <c r="D48" s="117"/>
+      <c r="E48" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F48" s="130">
+      <c r="F48" s="10">
         <v>2.097</v>
       </c>
-      <c r="G48" s="130">
+      <c r="G48" s="10">
         <v>2.097</v>
       </c>
-      <c r="H48" s="130">
+      <c r="H48" s="10">
         <v>16.018999999999998</v>
       </c>
-      <c r="I48" s="131">
+      <c r="I48" s="99">
         <v>6.0500000000000003E-7</v>
       </c>
-      <c r="J48" s="132" t="s">
+      <c r="J48" s="107" t="s">
         <v>29</v>
       </c>
       <c r="K48" s="66"/>
     </row>
     <row r="49" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C49" s="111"/>
-      <c r="D49" s="111"/>
+      <c r="C49" s="117"/>
+      <c r="D49" s="117"/>
       <c r="E49" s="3" t="s">
         <v>18</v>
       </c>
@@ -4735,8 +4839,8 @@
       <c r="K49" s="66"/>
     </row>
     <row r="50" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C50" s="111"/>
-      <c r="D50" s="113"/>
+      <c r="C50" s="117"/>
+      <c r="D50" s="121"/>
       <c r="E50" s="32" t="s">
         <v>26</v>
       </c>
@@ -4758,7 +4862,7 @@
       <c r="K50" s="66"/>
     </row>
     <row r="51" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C51" s="111"/>
+      <c r="C51" s="117"/>
       <c r="D51" s="17" t="s">
         <v>6</v>
       </c>
@@ -4771,7 +4875,7 @@
       <c r="K51" s="66"/>
     </row>
     <row r="52" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C52" s="126"/>
+      <c r="C52" s="127"/>
       <c r="D52" s="5" t="s">
         <v>24</v>
       </c>
@@ -4798,6 +4902,12 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C47:C52"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="D47:D50"/>
+    <mergeCell ref="D35:J35"/>
+    <mergeCell ref="D38:D39"/>
     <mergeCell ref="D6:J6"/>
     <mergeCell ref="C38:C41"/>
     <mergeCell ref="C42:C46"/>
@@ -4811,12 +4921,6 @@
     <mergeCell ref="D19:D20"/>
     <mergeCell ref="D22:D24"/>
     <mergeCell ref="D25:D28"/>
-    <mergeCell ref="C47:C52"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="D47:D50"/>
-    <mergeCell ref="D35:J35"/>
-    <mergeCell ref="D38:D39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4826,7 +4930,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8F6DB0D-2B41-A146-8989-239E41193B1F}">
   <dimension ref="B1:AD53"/>
   <sheetViews>
-    <sheetView topLeftCell="P18" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="AB54" sqref="AB54"/>
     </sheetView>
   </sheetViews>
@@ -4891,7 +4995,7 @@
     </row>
     <row r="5" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C5" s="66"/>
-      <c r="D5" s="107"/>
+      <c r="D5" s="108"/>
       <c r="E5" s="3"/>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
@@ -4904,7 +5008,7 @@
     </row>
     <row r="6" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C6" s="66"/>
-      <c r="D6" s="107"/>
+      <c r="D6" s="108"/>
       <c r="E6" s="3"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
@@ -4917,7 +5021,7 @@
     </row>
     <row r="7" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C7" s="66"/>
-      <c r="D7" s="107"/>
+      <c r="D7" s="108"/>
       <c r="E7" s="3"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
@@ -4930,7 +5034,7 @@
     </row>
     <row r="8" spans="3:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C8" s="66"/>
-      <c r="D8" s="108"/>
+      <c r="D8" s="109"/>
       <c r="E8" s="5"/>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
@@ -4943,7 +5047,7 @@
     </row>
     <row r="9" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C9" s="66"/>
-      <c r="D9" s="107"/>
+      <c r="D9" s="108"/>
       <c r="E9" s="3"/>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
@@ -4956,7 +5060,7 @@
     </row>
     <row r="10" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C10" s="66"/>
-      <c r="D10" s="107"/>
+      <c r="D10" s="108"/>
       <c r="E10" s="3"/>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
@@ -4969,7 +5073,7 @@
     </row>
     <row r="11" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C11" s="66"/>
-      <c r="D11" s="107"/>
+      <c r="D11" s="108"/>
       <c r="E11" s="3"/>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
@@ -4982,7 +5086,7 @@
     </row>
     <row r="12" spans="3:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C12" s="66"/>
-      <c r="D12" s="108"/>
+      <c r="D12" s="109"/>
       <c r="E12" s="5"/>
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
@@ -4995,74 +5099,74 @@
     </row>
     <row r="13" spans="3:29" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C13" s="66"/>
-      <c r="D13" s="127" t="s">
+      <c r="D13" s="128" t="s">
         <v>50</v>
       </c>
-      <c r="E13" s="127"/>
-      <c r="F13" s="127"/>
-      <c r="G13" s="127"/>
-      <c r="H13" s="127"/>
-      <c r="I13" s="127"/>
-      <c r="J13" s="127"/>
+      <c r="E13" s="128"/>
+      <c r="F13" s="128"/>
+      <c r="G13" s="128"/>
+      <c r="H13" s="128"/>
+      <c r="I13" s="128"/>
+      <c r="J13" s="128"/>
       <c r="K13" s="52"/>
       <c r="L13" s="66"/>
       <c r="M13" s="66"/>
     </row>
     <row r="14" spans="3:29" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C14" s="66"/>
-      <c r="D14" s="128"/>
-      <c r="E14" s="128"/>
-      <c r="F14" s="128"/>
-      <c r="G14" s="128"/>
-      <c r="H14" s="128"/>
-      <c r="I14" s="128"/>
-      <c r="J14" s="128"/>
+      <c r="D14" s="129"/>
+      <c r="E14" s="129"/>
+      <c r="F14" s="129"/>
+      <c r="G14" s="129"/>
+      <c r="H14" s="129"/>
+      <c r="I14" s="129"/>
+      <c r="J14" s="129"/>
       <c r="K14" s="52"/>
       <c r="L14" s="66"/>
-      <c r="M14" s="127" t="s">
+      <c r="M14" s="128" t="s">
         <v>51</v>
       </c>
-      <c r="N14" s="127"/>
-      <c r="O14" s="127"/>
-      <c r="P14" s="127"/>
-      <c r="Q14" s="127"/>
-      <c r="R14" s="127"/>
-      <c r="S14" s="127"/>
-      <c r="W14" s="127" t="s">
+      <c r="N14" s="128"/>
+      <c r="O14" s="128"/>
+      <c r="P14" s="128"/>
+      <c r="Q14" s="128"/>
+      <c r="R14" s="128"/>
+      <c r="S14" s="128"/>
+      <c r="W14" s="128" t="s">
         <v>52</v>
       </c>
-      <c r="X14" s="127"/>
-      <c r="Y14" s="127"/>
-      <c r="Z14" s="127"/>
-      <c r="AA14" s="127"/>
-      <c r="AB14" s="127"/>
-      <c r="AC14" s="127"/>
+      <c r="X14" s="128"/>
+      <c r="Y14" s="128"/>
+      <c r="Z14" s="128"/>
+      <c r="AA14" s="128"/>
+      <c r="AB14" s="128"/>
+      <c r="AC14" s="128"/>
     </row>
     <row r="15" spans="3:29" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C15" s="66"/>
-      <c r="D15" s="128"/>
-      <c r="E15" s="128"/>
-      <c r="F15" s="128"/>
-      <c r="G15" s="128"/>
-      <c r="H15" s="128"/>
-      <c r="I15" s="128"/>
-      <c r="J15" s="128"/>
+      <c r="D15" s="129"/>
+      <c r="E15" s="129"/>
+      <c r="F15" s="129"/>
+      <c r="G15" s="129"/>
+      <c r="H15" s="129"/>
+      <c r="I15" s="129"/>
+      <c r="J15" s="129"/>
       <c r="K15" s="52"/>
       <c r="L15" s="66"/>
-      <c r="M15" s="128"/>
-      <c r="N15" s="128"/>
-      <c r="O15" s="128"/>
-      <c r="P15" s="128"/>
-      <c r="Q15" s="128"/>
-      <c r="R15" s="128"/>
-      <c r="S15" s="128"/>
-      <c r="W15" s="128"/>
-      <c r="X15" s="128"/>
-      <c r="Y15" s="128"/>
-      <c r="Z15" s="128"/>
-      <c r="AA15" s="128"/>
-      <c r="AB15" s="128"/>
-      <c r="AC15" s="128"/>
+      <c r="M15" s="129"/>
+      <c r="N15" s="129"/>
+      <c r="O15" s="129"/>
+      <c r="P15" s="129"/>
+      <c r="Q15" s="129"/>
+      <c r="R15" s="129"/>
+      <c r="S15" s="129"/>
+      <c r="W15" s="129"/>
+      <c r="X15" s="129"/>
+      <c r="Y15" s="129"/>
+      <c r="Z15" s="129"/>
+      <c r="AA15" s="129"/>
+      <c r="AB15" s="129"/>
+      <c r="AC15" s="129"/>
     </row>
     <row r="16" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C16" s="66"/>
@@ -5075,24 +5179,24 @@
       <c r="J16" s="12"/>
       <c r="K16" s="52"/>
       <c r="L16" s="66"/>
-      <c r="M16" s="128"/>
-      <c r="N16" s="128"/>
-      <c r="O16" s="128"/>
-      <c r="P16" s="128"/>
-      <c r="Q16" s="128"/>
-      <c r="R16" s="128"/>
-      <c r="S16" s="128"/>
-      <c r="W16" s="128"/>
-      <c r="X16" s="128"/>
-      <c r="Y16" s="128"/>
-      <c r="Z16" s="128"/>
-      <c r="AA16" s="128"/>
-      <c r="AB16" s="128"/>
-      <c r="AC16" s="128"/>
+      <c r="M16" s="129"/>
+      <c r="N16" s="129"/>
+      <c r="O16" s="129"/>
+      <c r="P16" s="129"/>
+      <c r="Q16" s="129"/>
+      <c r="R16" s="129"/>
+      <c r="S16" s="129"/>
+      <c r="W16" s="129"/>
+      <c r="X16" s="129"/>
+      <c r="Y16" s="129"/>
+      <c r="Z16" s="129"/>
+      <c r="AA16" s="129"/>
+      <c r="AB16" s="129"/>
+      <c r="AC16" s="129"/>
     </row>
     <row r="17" spans="3:30" x14ac:dyDescent="0.2">
       <c r="C17" s="66"/>
-      <c r="D17" s="107"/>
+      <c r="D17" s="108"/>
       <c r="E17" s="3"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
@@ -5105,7 +5209,7 @@
     </row>
     <row r="18" spans="3:30" x14ac:dyDescent="0.2">
       <c r="C18" s="66"/>
-      <c r="D18" s="107"/>
+      <c r="D18" s="108"/>
       <c r="E18" s="3"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
@@ -5118,7 +5222,7 @@
     </row>
     <row r="19" spans="3:30" x14ac:dyDescent="0.2">
       <c r="C19" s="66"/>
-      <c r="D19" s="107"/>
+      <c r="D19" s="108"/>
       <c r="E19" s="3"/>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
@@ -5131,7 +5235,7 @@
     </row>
     <row r="20" spans="3:30" x14ac:dyDescent="0.2">
       <c r="C20" s="66"/>
-      <c r="D20" s="107"/>
+      <c r="D20" s="108"/>
       <c r="E20" s="3"/>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
@@ -6735,4 +6839,430 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95BB507F-C9F5-F04E-AC61-C149D982E15D}">
+  <dimension ref="J28:U52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="H25" zoomScale="150" workbookViewId="0">
+      <selection activeCell="Q44" sqref="Q44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="10.83203125" customWidth="1"/>
+    <col min="8" max="8" width="39.5" customWidth="1"/>
+    <col min="11" max="11" width="19.1640625" customWidth="1"/>
+    <col min="12" max="12" width="7.1640625" customWidth="1"/>
+    <col min="13" max="13" width="10.5" customWidth="1"/>
+    <col min="14" max="14" width="11.6640625" customWidth="1"/>
+    <col min="18" max="18" width="12.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="28" spans="10:21" x14ac:dyDescent="0.2">
+      <c r="J28" s="66"/>
+      <c r="K28" s="66"/>
+      <c r="L28" s="66"/>
+      <c r="M28" s="66"/>
+      <c r="N28" s="66"/>
+      <c r="O28" s="66"/>
+      <c r="P28" s="66"/>
+      <c r="Q28" s="66"/>
+      <c r="R28" s="66"/>
+      <c r="S28" s="66"/>
+      <c r="T28" s="66"/>
+      <c r="U28" s="66"/>
+    </row>
+    <row r="29" spans="10:21" x14ac:dyDescent="0.2">
+      <c r="J29" s="66"/>
+      <c r="K29" s="145" t="s">
+        <v>66</v>
+      </c>
+      <c r="L29" s="145"/>
+      <c r="M29" s="145"/>
+      <c r="N29" s="145"/>
+      <c r="O29" s="66"/>
+      <c r="P29" s="66"/>
+      <c r="Q29" s="66"/>
+      <c r="R29" s="66"/>
+      <c r="S29" s="66"/>
+      <c r="T29" s="66"/>
+      <c r="U29" s="66"/>
+    </row>
+    <row r="30" spans="10:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J30" s="66"/>
+      <c r="K30" s="66"/>
+      <c r="L30" s="66"/>
+      <c r="M30" s="66"/>
+      <c r="N30" s="66"/>
+      <c r="O30" s="66"/>
+      <c r="P30" s="66"/>
+      <c r="Q30" s="130" t="s">
+        <v>59</v>
+      </c>
+      <c r="R30" s="130" t="s">
+        <v>62</v>
+      </c>
+      <c r="S30" s="130" t="s">
+        <v>58</v>
+      </c>
+      <c r="T30" s="130" t="s">
+        <v>63</v>
+      </c>
+      <c r="U30" s="66"/>
+    </row>
+    <row r="31" spans="10:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J31" s="66"/>
+      <c r="K31" s="130" t="s">
+        <v>59</v>
+      </c>
+      <c r="L31" s="130" t="s">
+        <v>62</v>
+      </c>
+      <c r="M31" s="130" t="s">
+        <v>58</v>
+      </c>
+      <c r="N31" s="130" t="s">
+        <v>63</v>
+      </c>
+      <c r="O31" s="66"/>
+      <c r="P31" s="66"/>
+      <c r="Q31" s="142" t="s">
+        <v>64</v>
+      </c>
+      <c r="R31" s="139" t="s">
+        <v>65</v>
+      </c>
+      <c r="S31" s="132">
+        <v>4</v>
+      </c>
+      <c r="T31" s="132">
+        <v>54.021970000000003</v>
+      </c>
+      <c r="U31" s="66"/>
+    </row>
+    <row r="32" spans="10:21" x14ac:dyDescent="0.2">
+      <c r="J32" s="66"/>
+      <c r="K32" s="131" t="s">
+        <v>15</v>
+      </c>
+      <c r="L32" s="139" t="s">
+        <v>60</v>
+      </c>
+      <c r="M32" s="132">
+        <v>6.820417</v>
+      </c>
+      <c r="N32" s="137">
+        <v>25.528949999999998</v>
+      </c>
+      <c r="O32" s="66"/>
+      <c r="P32" s="66"/>
+      <c r="Q32" s="143" t="s">
+        <v>5</v>
+      </c>
+      <c r="R32" s="140" t="s">
+        <v>65</v>
+      </c>
+      <c r="S32" s="134">
+        <v>5</v>
+      </c>
+      <c r="T32" s="134">
+        <v>59.862450000000003</v>
+      </c>
+      <c r="U32" s="66"/>
+    </row>
+    <row r="33" spans="10:21" x14ac:dyDescent="0.2">
+      <c r="J33" s="66"/>
+      <c r="K33" s="133"/>
+      <c r="L33" s="140" t="s">
+        <v>61</v>
+      </c>
+      <c r="M33" s="134">
+        <v>7.2917740000000002</v>
+      </c>
+      <c r="N33" s="134">
+        <v>28.326519999999999</v>
+      </c>
+      <c r="O33" s="66"/>
+      <c r="P33" s="66"/>
+      <c r="Q33" s="144" t="s">
+        <v>6</v>
+      </c>
+      <c r="R33" s="141" t="s">
+        <v>65</v>
+      </c>
+      <c r="S33" s="136">
+        <v>9.2653459999999992</v>
+      </c>
+      <c r="T33" s="136">
+        <v>80.715180000000004</v>
+      </c>
+      <c r="U33" s="66"/>
+    </row>
+    <row r="34" spans="10:21" x14ac:dyDescent="0.2">
+      <c r="J34" s="66"/>
+      <c r="K34" s="135" t="s">
+        <v>5</v>
+      </c>
+      <c r="L34" s="141" t="s">
+        <v>60</v>
+      </c>
+      <c r="M34" s="136">
+        <v>5</v>
+      </c>
+      <c r="N34" s="138">
+        <v>36.09104</v>
+      </c>
+      <c r="O34" s="66"/>
+      <c r="P34" s="66"/>
+      <c r="Q34" s="143" t="s">
+        <v>24</v>
+      </c>
+      <c r="R34" s="140" t="s">
+        <v>65</v>
+      </c>
+      <c r="S34" s="134">
+        <v>7.7588999999999997</v>
+      </c>
+      <c r="T34" s="134">
+        <v>92.156210000000002</v>
+      </c>
+      <c r="U34" s="66"/>
+    </row>
+    <row r="35" spans="10:21" x14ac:dyDescent="0.2">
+      <c r="J35" s="66"/>
+      <c r="K35" s="133"/>
+      <c r="L35" s="140" t="s">
+        <v>61</v>
+      </c>
+      <c r="M35" s="134">
+        <v>5.9688330000000001</v>
+      </c>
+      <c r="N35" s="134">
+        <v>50.782449999999997</v>
+      </c>
+      <c r="O35" s="66"/>
+      <c r="P35" s="66"/>
+      <c r="Q35" s="66"/>
+      <c r="R35" s="66"/>
+      <c r="S35" s="66"/>
+      <c r="T35" s="66"/>
+      <c r="U35" s="66"/>
+    </row>
+    <row r="36" spans="10:21" x14ac:dyDescent="0.2">
+      <c r="J36" s="66"/>
+      <c r="K36" s="135" t="s">
+        <v>6</v>
+      </c>
+      <c r="L36" s="141" t="s">
+        <v>60</v>
+      </c>
+      <c r="M36" s="136">
+        <v>6.9876889999999996</v>
+      </c>
+      <c r="N36" s="138">
+        <v>70.550629999999998</v>
+      </c>
+      <c r="O36" s="66"/>
+      <c r="P36" s="66"/>
+      <c r="Q36" s="66"/>
+      <c r="R36" s="66"/>
+      <c r="S36" s="66"/>
+      <c r="T36" s="66"/>
+      <c r="U36" s="66"/>
+    </row>
+    <row r="37" spans="10:21" x14ac:dyDescent="0.2">
+      <c r="J37" s="66"/>
+      <c r="K37" s="133"/>
+      <c r="L37" s="140" t="s">
+        <v>61</v>
+      </c>
+      <c r="M37" s="134">
+        <v>7.9859780000000002</v>
+      </c>
+      <c r="N37" s="134">
+        <v>79.455860000000001</v>
+      </c>
+      <c r="O37" s="66"/>
+    </row>
+    <row r="38" spans="10:21" x14ac:dyDescent="0.2">
+      <c r="J38" s="66"/>
+      <c r="K38" s="135" t="s">
+        <v>12</v>
+      </c>
+      <c r="L38" s="141" t="s">
+        <v>60</v>
+      </c>
+      <c r="M38" s="136">
+        <v>12.85126</v>
+      </c>
+      <c r="N38" s="138">
+        <v>63.976089999999999</v>
+      </c>
+      <c r="O38" s="66"/>
+    </row>
+    <row r="39" spans="10:21" x14ac:dyDescent="0.2">
+      <c r="J39" s="66"/>
+      <c r="K39" s="133"/>
+      <c r="L39" s="140" t="s">
+        <v>61</v>
+      </c>
+      <c r="M39" s="134">
+        <v>12.693714</v>
+      </c>
+      <c r="N39" s="134">
+        <v>83.763069999999999</v>
+      </c>
+      <c r="O39" s="66"/>
+    </row>
+    <row r="40" spans="10:21" x14ac:dyDescent="0.2">
+      <c r="J40" s="66"/>
+      <c r="K40" s="66"/>
+      <c r="L40" s="66"/>
+      <c r="M40" s="66"/>
+      <c r="N40" s="66"/>
+      <c r="O40" s="66"/>
+    </row>
+    <row r="43" spans="10:21" x14ac:dyDescent="0.2">
+      <c r="J43" s="145" t="s">
+        <v>67</v>
+      </c>
+      <c r="K43" s="145"/>
+      <c r="L43" s="145"/>
+      <c r="M43" s="145"/>
+    </row>
+    <row r="44" spans="10:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J44" s="130" t="s">
+        <v>59</v>
+      </c>
+      <c r="K44" s="130" t="s">
+        <v>62</v>
+      </c>
+      <c r="L44" s="130" t="s">
+        <v>58</v>
+      </c>
+      <c r="M44" s="130" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="10:21" x14ac:dyDescent="0.2">
+      <c r="J45" s="131" t="s">
+        <v>15</v>
+      </c>
+      <c r="K45" s="139" t="s">
+        <v>60</v>
+      </c>
+      <c r="L45">
+        <v>7.8456219999999997</v>
+      </c>
+      <c r="M45">
+        <v>29.234929999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="10:21" x14ac:dyDescent="0.2">
+      <c r="J46" s="133"/>
+      <c r="K46" s="140" t="s">
+        <v>61</v>
+      </c>
+      <c r="L46">
+        <v>7.0123470000000001</v>
+      </c>
+      <c r="M46">
+        <v>45.306550000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="10:21" x14ac:dyDescent="0.2">
+      <c r="J47" s="135" t="s">
+        <v>5</v>
+      </c>
+      <c r="K47" s="141" t="s">
+        <v>60</v>
+      </c>
+      <c r="L47">
+        <v>6.5228169999999999</v>
+      </c>
+      <c r="M47">
+        <v>42.06091</v>
+      </c>
+    </row>
+    <row r="48" spans="10:21" x14ac:dyDescent="0.2">
+      <c r="J48" s="133"/>
+      <c r="K48" s="140" t="s">
+        <v>61</v>
+      </c>
+      <c r="L48">
+        <v>5.9688330000000001</v>
+      </c>
+      <c r="M48">
+        <v>50.782449999999997</v>
+      </c>
+    </row>
+    <row r="49" spans="10:13" x14ac:dyDescent="0.2">
+      <c r="J49" s="135" t="s">
+        <v>6</v>
+      </c>
+      <c r="K49" s="141" t="s">
+        <v>60</v>
+      </c>
+      <c r="L49">
+        <v>6.3269760000000002</v>
+      </c>
+      <c r="M49">
+        <v>83.92165</v>
+      </c>
+    </row>
+    <row r="50" spans="10:13" x14ac:dyDescent="0.2">
+      <c r="J50" s="133"/>
+      <c r="K50" s="140" t="s">
+        <v>61</v>
+      </c>
+      <c r="L50">
+        <v>7.9859780000000002</v>
+      </c>
+      <c r="M50">
+        <v>79.455860000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="10:13" x14ac:dyDescent="0.2">
+      <c r="J51" s="135" t="s">
+        <v>12</v>
+      </c>
+      <c r="K51" s="141" t="s">
+        <v>60</v>
+      </c>
+      <c r="L51">
+        <v>11.056463000000001</v>
+      </c>
+      <c r="M51">
+        <v>82.390469999999993</v>
+      </c>
+    </row>
+    <row r="52" spans="10:13" x14ac:dyDescent="0.2">
+      <c r="J52" s="133"/>
+      <c r="K52" s="140" t="s">
+        <v>61</v>
+      </c>
+      <c r="L52">
+        <v>12.693714</v>
+      </c>
+      <c r="M52">
+        <v>83.763069999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="J45:J46"/>
+    <mergeCell ref="J47:J48"/>
+    <mergeCell ref="J49:J50"/>
+    <mergeCell ref="J51:J52"/>
+    <mergeCell ref="K29:N29"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="K32:K33"/>
+    <mergeCell ref="K34:K35"/>
+    <mergeCell ref="K36:K37"/>
+    <mergeCell ref="K38:K39"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updating with AIC info
</commit_message>
<xml_diff>
--- a/K4S_key_scripts/K4S_DA_Aims/K4S_DA_A2/K4S_DA_A2/K4S_DA_A2_GAM_Temporal_Results.xlsx
+++ b/K4S_key_scripts/K4S_DA_Aims/K4S_DA_A2/K4S_DA_A2/K4S_DA_A2_GAM_Temporal_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoestarkey/Desktop/Honours/Data_Analysis/K_axis_midoc/K4S_key_scripts/K4S_DA_Aims/K4S_DA_A2/K4S_DA_A2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB794F6-C50E-5E42-AAFB-BC0EE85659A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63110C5B-817E-FD48-BFBA-CEDB158C0637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3940" yWindow="780" windowWidth="34200" windowHeight="19400" activeTab="4" xr2:uid="{33E5A15D-DBA6-5B40-873E-91FBDBF28531}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="19400" activeTab="4" xr2:uid="{33E5A15D-DBA6-5B40-873E-91FBDBF28531}"/>
   </bookViews>
   <sheets>
     <sheet name="GAM_Temporal_Sum" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="69">
   <si>
     <t>Season</t>
   </si>
@@ -257,6 +257,9 @@
   </si>
   <si>
     <t>With SST outliers kept in</t>
+  </si>
+  <si>
+    <t>All satellite vars</t>
   </si>
 </sst>
 </file>
@@ -504,7 +507,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -789,72 +792,6 @@
     <xf numFmtId="11" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -890,9 +827,105 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1318,7 +1351,7 @@
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="108" t="s">
+      <c r="B5" s="123" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -1342,7 +1375,7 @@
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="108"/>
+      <c r="B6" s="123"/>
       <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
@@ -1364,7 +1397,7 @@
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="108"/>
+      <c r="B7" s="123"/>
       <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1386,7 +1419,7 @@
       </c>
     </row>
     <row r="8" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="109"/>
+      <c r="B8" s="124"/>
       <c r="C8" s="5" t="s">
         <v>12</v>
       </c>
@@ -1408,7 +1441,7 @@
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="108" t="s">
+      <c r="B9" s="123" t="s">
         <v>1</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -1432,7 +1465,7 @@
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="108"/>
+      <c r="B10" s="123"/>
       <c r="C10" s="3" t="s">
         <v>5</v>
       </c>
@@ -1454,7 +1487,7 @@
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="108"/>
+      <c r="B11" s="123"/>
       <c r="C11" s="3" t="s">
         <v>6</v>
       </c>
@@ -1476,7 +1509,7 @@
       </c>
     </row>
     <row r="12" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="109"/>
+      <c r="B12" s="124"/>
       <c r="C12" s="5" t="s">
         <v>12</v>
       </c>
@@ -1498,7 +1531,7 @@
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B13" s="108" t="s">
+      <c r="B13" s="123" t="s">
         <v>2</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1522,7 +1555,7 @@
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B14" s="108"/>
+      <c r="B14" s="123"/>
       <c r="C14" s="3" t="s">
         <v>5</v>
       </c>
@@ -1544,7 +1577,7 @@
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B15" s="108"/>
+      <c r="B15" s="123"/>
       <c r="C15" s="3" t="s">
         <v>6</v>
       </c>
@@ -1566,7 +1599,7 @@
       </c>
     </row>
     <row r="16" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="109"/>
+      <c r="B16" s="124"/>
       <c r="C16" s="5" t="s">
         <v>12</v>
       </c>
@@ -1655,10 +1688,10 @@
       </c>
     </row>
     <row r="6" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C6" s="108" t="s">
+      <c r="C6" s="123" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="111" t="s">
+      <c r="D6" s="131" t="s">
         <v>15</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -1671,8 +1704,8 @@
       <c r="J6" s="8"/>
     </row>
     <row r="7" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="108"/>
-      <c r="D7" s="112"/>
+      <c r="C7" s="123"/>
+      <c r="D7" s="132"/>
       <c r="E7" s="3" t="s">
         <v>17</v>
       </c>
@@ -1683,8 +1716,8 @@
       <c r="J7" s="8"/>
     </row>
     <row r="8" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C8" s="108"/>
-      <c r="D8" s="112"/>
+      <c r="C8" s="123"/>
+      <c r="D8" s="132"/>
       <c r="E8" s="3" t="s">
         <v>18</v>
       </c>
@@ -1695,8 +1728,8 @@
       <c r="J8" s="8"/>
     </row>
     <row r="9" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="108"/>
-      <c r="D9" s="112"/>
+      <c r="C9" s="123"/>
+      <c r="D9" s="132"/>
       <c r="E9" s="3" t="s">
         <v>19</v>
       </c>
@@ -1707,8 +1740,8 @@
       <c r="J9" s="8"/>
     </row>
     <row r="10" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="108"/>
-      <c r="D10" s="112"/>
+      <c r="C10" s="123"/>
+      <c r="D10" s="132"/>
       <c r="E10" s="3" t="s">
         <v>20</v>
       </c>
@@ -1719,7 +1752,7 @@
       <c r="J10" s="8"/>
     </row>
     <row r="11" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C11" s="108"/>
+      <c r="C11" s="123"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="10"/>
@@ -1729,7 +1762,7 @@
       <c r="J11" s="8"/>
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C12" s="108"/>
+      <c r="C12" s="123"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="10"/>
@@ -1739,7 +1772,7 @@
       <c r="J12" s="8"/>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C13" s="108"/>
+      <c r="C13" s="123"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="10"/>
@@ -1749,7 +1782,7 @@
       <c r="J13" s="8"/>
     </row>
     <row r="14" spans="3:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="109"/>
+      <c r="C14" s="124"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="11"/>
@@ -1759,7 +1792,7 @@
       <c r="J14" s="14"/>
     </row>
     <row r="15" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C15" s="108" t="s">
+      <c r="C15" s="123" t="s">
         <v>1</v>
       </c>
       <c r="D15" s="3"/>
@@ -1771,7 +1804,7 @@
       <c r="J15" s="15"/>
     </row>
     <row r="16" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C16" s="108"/>
+      <c r="C16" s="123"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="10"/>
@@ -1781,7 +1814,7 @@
       <c r="J16" s="8"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C17" s="108"/>
+      <c r="C17" s="123"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="10"/>
@@ -1791,7 +1824,7 @@
       <c r="J17" s="8"/>
     </row>
     <row r="18" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="109"/>
+      <c r="C18" s="124"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="11"/>
@@ -1801,7 +1834,7 @@
       <c r="J18" s="13"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C19" s="108" t="s">
+      <c r="C19" s="123" t="s">
         <v>2</v>
       </c>
       <c r="D19" s="3"/>
@@ -1813,7 +1846,7 @@
       <c r="J19" s="8"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C20" s="108"/>
+      <c r="C20" s="123"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="10"/>
@@ -1823,7 +1856,7 @@
       <c r="J20" s="8"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C21" s="108"/>
+      <c r="C21" s="123"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="10"/>
@@ -1833,7 +1866,7 @@
       <c r="J21" s="8"/>
     </row>
     <row r="22" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="109"/>
+      <c r="C22" s="124"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="11"/>
@@ -1845,26 +1878,26 @@
     <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B26" s="66"/>
       <c r="C26" s="66"/>
-      <c r="D26" s="113" t="s">
+      <c r="D26" s="125" t="s">
         <v>48</v>
       </c>
-      <c r="E26" s="113"/>
-      <c r="F26" s="113"/>
-      <c r="G26" s="113"/>
-      <c r="H26" s="113"/>
-      <c r="I26" s="113"/>
-      <c r="J26" s="113"/>
+      <c r="E26" s="125"/>
+      <c r="F26" s="125"/>
+      <c r="G26" s="125"/>
+      <c r="H26" s="125"/>
+      <c r="I26" s="125"/>
+      <c r="J26" s="125"/>
       <c r="K26" s="66"/>
     </row>
     <row r="27" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" s="66"/>
-      <c r="C27" s="110"/>
-      <c r="D27" s="110"/>
-      <c r="E27" s="110"/>
-      <c r="F27" s="110"/>
-      <c r="G27" s="110"/>
-      <c r="H27" s="110"/>
-      <c r="I27" s="110"/>
+      <c r="C27" s="141"/>
+      <c r="D27" s="141"/>
+      <c r="E27" s="141"/>
+      <c r="F27" s="141"/>
+      <c r="G27" s="141"/>
+      <c r="H27" s="141"/>
+      <c r="I27" s="141"/>
       <c r="J27" s="66"/>
       <c r="K27" s="66"/>
     </row>
@@ -1896,7 +1929,7 @@
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B29" s="66"/>
-      <c r="C29" s="118" t="s">
+      <c r="C29" s="126" t="s">
         <v>0</v>
       </c>
       <c r="D29" s="33" t="s">
@@ -1925,7 +1958,7 @@
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B30" s="66"/>
-      <c r="C30" s="117"/>
+      <c r="C30" s="127"/>
       <c r="D30" s="33" t="s">
         <v>22</v>
       </c>
@@ -1952,7 +1985,7 @@
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B31" s="66"/>
-      <c r="C31" s="117"/>
+      <c r="C31" s="127"/>
       <c r="D31" s="33" t="s">
         <v>6</v>
       </c>
@@ -1979,8 +2012,8 @@
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B32" s="66"/>
-      <c r="C32" s="117"/>
-      <c r="D32" s="117" t="s">
+      <c r="C32" s="127"/>
+      <c r="D32" s="127" t="s">
         <v>24</v>
       </c>
       <c r="E32" s="3" t="s">
@@ -2006,8 +2039,8 @@
     </row>
     <row r="33" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B33" s="66"/>
-      <c r="C33" s="117"/>
-      <c r="D33" s="117"/>
+      <c r="C33" s="127"/>
+      <c r="D33" s="127"/>
       <c r="E33" s="3" t="s">
         <v>20</v>
       </c>
@@ -2034,10 +2067,10 @@
     </row>
     <row r="34" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B34" s="66"/>
-      <c r="C34" s="114" t="s">
-        <v>1</v>
-      </c>
-      <c r="D34" s="114" t="s">
+      <c r="C34" s="128" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" s="128" t="s">
         <v>15</v>
       </c>
       <c r="E34" s="22" t="s">
@@ -2063,8 +2096,8 @@
     </row>
     <row r="35" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B35" s="66"/>
-      <c r="C35" s="108"/>
-      <c r="D35" s="115"/>
+      <c r="C35" s="123"/>
+      <c r="D35" s="136"/>
       <c r="E35" s="26" t="s">
         <v>20</v>
       </c>
@@ -2088,8 +2121,8 @@
     </row>
     <row r="36" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B36" s="66"/>
-      <c r="C36" s="108"/>
-      <c r="D36" s="116" t="s">
+      <c r="C36" s="123"/>
+      <c r="D36" s="137" t="s">
         <v>22</v>
       </c>
       <c r="E36" s="29" t="s">
@@ -2115,8 +2148,8 @@
     </row>
     <row r="37" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B37" s="66"/>
-      <c r="C37" s="108"/>
-      <c r="D37" s="115"/>
+      <c r="C37" s="123"/>
+      <c r="D37" s="136"/>
       <c r="E37" s="32" t="s">
         <v>20</v>
       </c>
@@ -2140,7 +2173,7 @@
     </row>
     <row r="38" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B38" s="66"/>
-      <c r="C38" s="108"/>
+      <c r="C38" s="123"/>
       <c r="D38" s="33" t="s">
         <v>6</v>
       </c>
@@ -2167,7 +2200,7 @@
     </row>
     <row r="39" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B39" s="66"/>
-      <c r="C39" s="109"/>
+      <c r="C39" s="124"/>
       <c r="D39" s="5" t="s">
         <v>24</v>
       </c>
@@ -2194,7 +2227,7 @@
     </row>
     <row r="40" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B40" s="66"/>
-      <c r="C40" s="114" t="s">
+      <c r="C40" s="128" t="s">
         <v>2</v>
       </c>
       <c r="D40" s="33" t="s">
@@ -2223,7 +2256,7 @@
     </row>
     <row r="41" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B41" s="66"/>
-      <c r="C41" s="108"/>
+      <c r="C41" s="123"/>
       <c r="D41" s="33" t="s">
         <v>22</v>
       </c>
@@ -2250,7 +2283,7 @@
     </row>
     <row r="42" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B42" s="66"/>
-      <c r="C42" s="108"/>
+      <c r="C42" s="123"/>
       <c r="D42" s="33" t="s">
         <v>6</v>
       </c>
@@ -2264,7 +2297,7 @@
     </row>
     <row r="43" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B43" s="66"/>
-      <c r="C43" s="109"/>
+      <c r="C43" s="124"/>
       <c r="D43" s="5" t="s">
         <v>24</v>
       </c>
@@ -2318,26 +2351,26 @@
     </row>
     <row r="47" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C47" s="66"/>
-      <c r="D47" s="113" t="s">
+      <c r="D47" s="125" t="s">
         <v>47</v>
       </c>
-      <c r="E47" s="113"/>
-      <c r="F47" s="113"/>
-      <c r="G47" s="113"/>
-      <c r="H47" s="113"/>
-      <c r="I47" s="113"/>
-      <c r="J47" s="113"/>
+      <c r="E47" s="125"/>
+      <c r="F47" s="125"/>
+      <c r="G47" s="125"/>
+      <c r="H47" s="125"/>
+      <c r="I47" s="125"/>
+      <c r="J47" s="125"/>
       <c r="K47" s="66"/>
       <c r="P47" s="66"/>
-      <c r="Q47" s="113" t="s">
+      <c r="Q47" s="125" t="s">
         <v>49</v>
       </c>
-      <c r="R47" s="113"/>
-      <c r="S47" s="113"/>
-      <c r="T47" s="113"/>
-      <c r="U47" s="113"/>
-      <c r="V47" s="113"/>
-      <c r="W47" s="113"/>
+      <c r="R47" s="125"/>
+      <c r="S47" s="125"/>
+      <c r="T47" s="125"/>
+      <c r="U47" s="125"/>
+      <c r="V47" s="125"/>
+      <c r="W47" s="125"/>
       <c r="X47" s="66"/>
     </row>
     <row r="48" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2414,7 +2447,7 @@
     </row>
     <row r="50" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B50" s="66"/>
-      <c r="C50" s="118" t="s">
+      <c r="C50" s="126" t="s">
         <v>0</v>
       </c>
       <c r="D50" s="33" t="s">
@@ -2441,7 +2474,7 @@
       </c>
       <c r="K50" s="66"/>
       <c r="O50" s="66"/>
-      <c r="P50" s="118" t="s">
+      <c r="P50" s="126" t="s">
         <v>0</v>
       </c>
       <c r="Q50" s="33" t="s">
@@ -2470,7 +2503,7 @@
     </row>
     <row r="51" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B51" s="66"/>
-      <c r="C51" s="117"/>
+      <c r="C51" s="127"/>
       <c r="D51" s="33" t="s">
         <v>5</v>
       </c>
@@ -2495,7 +2528,7 @@
       </c>
       <c r="K51" s="66"/>
       <c r="O51" s="66"/>
-      <c r="P51" s="117"/>
+      <c r="P51" s="127"/>
       <c r="Q51" s="33" t="s">
         <v>5</v>
       </c>
@@ -2522,7 +2555,7 @@
     </row>
     <row r="52" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B52" s="66"/>
-      <c r="C52" s="117"/>
+      <c r="C52" s="127"/>
       <c r="D52" s="33" t="s">
         <v>6</v>
       </c>
@@ -2547,7 +2580,7 @@
       </c>
       <c r="K52" s="66"/>
       <c r="O52" s="66"/>
-      <c r="P52" s="117"/>
+      <c r="P52" s="127"/>
       <c r="Q52" s="33" t="s">
         <v>6</v>
       </c>
@@ -2574,7 +2607,7 @@
     </row>
     <row r="53" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B53" s="66"/>
-      <c r="C53" s="117"/>
+      <c r="C53" s="127"/>
       <c r="D53" s="17" t="s">
         <v>24</v>
       </c>
@@ -2588,7 +2621,7 @@
       <c r="J53" s="88"/>
       <c r="K53" s="66"/>
       <c r="O53" s="66"/>
-      <c r="P53" s="117"/>
+      <c r="P53" s="127"/>
       <c r="Q53" s="17" t="s">
         <v>24</v>
       </c>
@@ -2604,10 +2637,10 @@
     </row>
     <row r="54" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B54" s="66"/>
-      <c r="C54" s="114" t="s">
-        <v>1</v>
-      </c>
-      <c r="D54" s="118" t="s">
+      <c r="C54" s="128" t="s">
+        <v>1</v>
+      </c>
+      <c r="D54" s="126" t="s">
         <v>25</v>
       </c>
       <c r="E54" s="22" t="s">
@@ -2631,10 +2664,10 @@
       </c>
       <c r="K54" s="66"/>
       <c r="O54" s="66"/>
-      <c r="P54" s="114" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q54" s="118" t="s">
+      <c r="P54" s="128" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q54" s="126" t="s">
         <v>25</v>
       </c>
       <c r="R54" s="22" t="s">
@@ -2660,8 +2693,8 @@
     </row>
     <row r="55" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B55" s="66"/>
-      <c r="C55" s="108"/>
-      <c r="D55" s="121"/>
+      <c r="C55" s="123"/>
+      <c r="D55" s="129"/>
       <c r="E55" s="26" t="s">
         <v>26</v>
       </c>
@@ -2683,8 +2716,8 @@
       </c>
       <c r="K55" s="66"/>
       <c r="O55" s="66"/>
-      <c r="P55" s="108"/>
-      <c r="Q55" s="121"/>
+      <c r="P55" s="123"/>
+      <c r="Q55" s="129"/>
       <c r="R55" s="26" t="s">
         <v>26</v>
       </c>
@@ -2708,8 +2741,8 @@
     </row>
     <row r="56" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B56" s="66"/>
-      <c r="C56" s="108"/>
-      <c r="D56" s="122" t="s">
+      <c r="C56" s="123"/>
+      <c r="D56" s="130" t="s">
         <v>5</v>
       </c>
       <c r="E56" s="29" t="s">
@@ -2733,8 +2766,8 @@
       </c>
       <c r="K56" s="66"/>
       <c r="O56" s="66"/>
-      <c r="P56" s="108"/>
-      <c r="Q56" s="122" t="s">
+      <c r="P56" s="123"/>
+      <c r="Q56" s="130" t="s">
         <v>5</v>
       </c>
       <c r="R56" s="29" t="s">
@@ -2760,8 +2793,8 @@
     </row>
     <row r="57" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B57" s="66"/>
-      <c r="C57" s="108"/>
-      <c r="D57" s="121"/>
+      <c r="C57" s="123"/>
+      <c r="D57" s="129"/>
       <c r="E57" s="32" t="s">
         <v>20</v>
       </c>
@@ -2783,8 +2816,8 @@
       </c>
       <c r="K57" s="66"/>
       <c r="O57" s="66"/>
-      <c r="P57" s="108"/>
-      <c r="Q57" s="121"/>
+      <c r="P57" s="123"/>
+      <c r="Q57" s="129"/>
       <c r="R57" s="32" t="s">
         <v>20</v>
       </c>
@@ -2808,7 +2841,7 @@
     </row>
     <row r="58" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B58" s="66"/>
-      <c r="C58" s="108"/>
+      <c r="C58" s="123"/>
       <c r="D58" s="33" t="s">
         <v>6</v>
       </c>
@@ -2833,7 +2866,7 @@
       </c>
       <c r="K58" s="66"/>
       <c r="O58" s="66"/>
-      <c r="P58" s="108"/>
+      <c r="P58" s="123"/>
       <c r="Q58" s="33" t="s">
         <v>6</v>
       </c>
@@ -2860,7 +2893,7 @@
     </row>
     <row r="59" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B59" s="66"/>
-      <c r="C59" s="109"/>
+      <c r="C59" s="124"/>
       <c r="D59" s="5" t="s">
         <v>24</v>
       </c>
@@ -2874,7 +2907,7 @@
       <c r="J59" s="88"/>
       <c r="K59" s="66"/>
       <c r="O59" s="66"/>
-      <c r="P59" s="109"/>
+      <c r="P59" s="124"/>
       <c r="Q59" s="5" t="s">
         <v>24</v>
       </c>
@@ -2890,7 +2923,7 @@
     </row>
     <row r="60" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B60" s="66"/>
-      <c r="C60" s="111" t="s">
+      <c r="C60" s="131" t="s">
         <v>2</v>
       </c>
       <c r="D60" s="33" t="s">
@@ -2917,7 +2950,7 @@
       </c>
       <c r="K60" s="66"/>
       <c r="O60" s="66"/>
-      <c r="P60" s="111" t="s">
+      <c r="P60" s="131" t="s">
         <v>2</v>
       </c>
       <c r="Q60" s="33" t="s">
@@ -2946,8 +2979,8 @@
     </row>
     <row r="61" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B61" s="66"/>
-      <c r="C61" s="112"/>
-      <c r="D61" s="122" t="s">
+      <c r="C61" s="132"/>
+      <c r="D61" s="130" t="s">
         <v>5</v>
       </c>
       <c r="E61" s="29" t="s">
@@ -2971,8 +3004,8 @@
       </c>
       <c r="K61" s="66"/>
       <c r="O61" s="66"/>
-      <c r="P61" s="112"/>
-      <c r="Q61" s="122" t="s">
+      <c r="P61" s="132"/>
+      <c r="Q61" s="130" t="s">
         <v>5</v>
       </c>
       <c r="R61" s="29" t="s">
@@ -2998,8 +3031,8 @@
     </row>
     <row r="62" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B62" s="66"/>
-      <c r="C62" s="112"/>
-      <c r="D62" s="121"/>
+      <c r="C62" s="132"/>
+      <c r="D62" s="129"/>
       <c r="E62" s="32" t="s">
         <v>18</v>
       </c>
@@ -3021,8 +3054,8 @@
       </c>
       <c r="K62" s="66"/>
       <c r="O62" s="66"/>
-      <c r="P62" s="112"/>
-      <c r="Q62" s="121"/>
+      <c r="P62" s="132"/>
+      <c r="Q62" s="129"/>
       <c r="R62" s="32" t="s">
         <v>18</v>
       </c>
@@ -3046,7 +3079,7 @@
     </row>
     <row r="63" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B63" s="66"/>
-      <c r="C63" s="112"/>
+      <c r="C63" s="132"/>
       <c r="D63" s="17" t="s">
         <v>6</v>
       </c>
@@ -3058,7 +3091,7 @@
       <c r="J63" s="42"/>
       <c r="K63" s="66"/>
       <c r="O63" s="66"/>
-      <c r="P63" s="112"/>
+      <c r="P63" s="132"/>
       <c r="Q63" s="17" t="s">
         <v>6</v>
       </c>
@@ -3072,7 +3105,7 @@
     </row>
     <row r="64" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B64" s="66"/>
-      <c r="C64" s="123"/>
+      <c r="C64" s="133"/>
       <c r="D64" s="5" t="s">
         <v>24</v>
       </c>
@@ -3086,7 +3119,7 @@
       <c r="J64" s="91"/>
       <c r="K64" s="66"/>
       <c r="O64" s="66"/>
-      <c r="P64" s="123"/>
+      <c r="P64" s="133"/>
       <c r="Q64" s="5" t="s">
         <v>24</v>
       </c>
@@ -3178,7 +3211,7 @@
     </row>
     <row r="71" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B71" s="66"/>
-      <c r="C71" s="118" t="s">
+      <c r="C71" s="126" t="s">
         <v>0</v>
       </c>
       <c r="D71" t="s">
@@ -3198,7 +3231,7 @@
     </row>
     <row r="72" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B72" s="66"/>
-      <c r="C72" s="117"/>
+      <c r="C72" s="127"/>
       <c r="D72" s="20" t="s">
         <v>28</v>
       </c>
@@ -3216,10 +3249,10 @@
     </row>
     <row r="73" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B73" s="66"/>
-      <c r="C73" s="114" t="s">
-        <v>1</v>
-      </c>
-      <c r="D73" s="114" t="s">
+      <c r="C73" s="128" t="s">
+        <v>1</v>
+      </c>
+      <c r="D73" s="128" t="s">
         <v>21</v>
       </c>
       <c r="E73" s="52" t="s">
@@ -3236,8 +3269,8 @@
     </row>
     <row r="74" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B74" s="66"/>
-      <c r="C74" s="108"/>
-      <c r="D74" s="115"/>
+      <c r="C74" s="123"/>
+      <c r="D74" s="136"/>
       <c r="E74" s="56" t="s">
         <v>20</v>
       </c>
@@ -3252,8 +3285,8 @@
     </row>
     <row r="75" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B75" s="66"/>
-      <c r="C75" s="108"/>
-      <c r="D75" s="116" t="s">
+      <c r="C75" s="123"/>
+      <c r="D75" s="137" t="s">
         <v>28</v>
       </c>
       <c r="E75" s="57" t="s">
@@ -3270,8 +3303,8 @@
     </row>
     <row r="76" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B76" s="66"/>
-      <c r="C76" s="108"/>
-      <c r="D76" s="109"/>
+      <c r="C76" s="123"/>
+      <c r="D76" s="124"/>
       <c r="E76" s="59" t="s">
         <v>20</v>
       </c>
@@ -3286,7 +3319,7 @@
     </row>
     <row r="77" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B77" s="66"/>
-      <c r="C77" s="119" t="s">
+      <c r="C77" s="139" t="s">
         <v>2</v>
       </c>
       <c r="D77" s="63" t="s">
@@ -3306,7 +3339,7 @@
     </row>
     <row r="78" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B78" s="66"/>
-      <c r="C78" s="120"/>
+      <c r="C78" s="140"/>
       <c r="D78" s="65" t="s">
         <v>28</v>
       </c>
@@ -3325,13 +3358,13 @@
     <row r="79" spans="2:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B79" s="66"/>
       <c r="C79" s="61"/>
-      <c r="D79" s="126"/>
-      <c r="E79" s="126"/>
-      <c r="F79" s="126"/>
-      <c r="G79" s="126"/>
-      <c r="H79" s="126"/>
-      <c r="I79" s="126"/>
-      <c r="J79" s="126"/>
+      <c r="D79" s="138"/>
+      <c r="E79" s="138"/>
+      <c r="F79" s="138"/>
+      <c r="G79" s="138"/>
+      <c r="H79" s="138"/>
+      <c r="I79" s="138"/>
+      <c r="J79" s="138"/>
       <c r="K79" s="66"/>
     </row>
     <row r="80" spans="2:24" x14ac:dyDescent="0.2">
@@ -3400,7 +3433,7 @@
     </row>
     <row r="88" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B88" s="66"/>
-      <c r="C88" s="118" t="s">
+      <c r="C88" s="126" t="s">
         <v>0</v>
       </c>
       <c r="D88" t="s">
@@ -3420,7 +3453,7 @@
     </row>
     <row r="89" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B89" s="66"/>
-      <c r="C89" s="117"/>
+      <c r="C89" s="127"/>
       <c r="D89" s="20" t="s">
         <v>28</v>
       </c>
@@ -3438,10 +3471,10 @@
     </row>
     <row r="90" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B90" s="66"/>
-      <c r="C90" s="114" t="s">
-        <v>1</v>
-      </c>
-      <c r="D90" s="114" t="s">
+      <c r="C90" s="128" t="s">
+        <v>1</v>
+      </c>
+      <c r="D90" s="128" t="s">
         <v>21</v>
       </c>
       <c r="E90" s="29" t="s">
@@ -3458,8 +3491,8 @@
     </row>
     <row r="91" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B91" s="66"/>
-      <c r="C91" s="108"/>
-      <c r="D91" s="115"/>
+      <c r="C91" s="123"/>
+      <c r="D91" s="136"/>
       <c r="E91" s="32" t="s">
         <v>20</v>
       </c>
@@ -3474,8 +3507,8 @@
     </row>
     <row r="92" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B92" s="66"/>
-      <c r="C92" s="108"/>
-      <c r="D92" s="116" t="s">
+      <c r="C92" s="123"/>
+      <c r="D92" s="137" t="s">
         <v>28</v>
       </c>
       <c r="E92" s="29" t="s">
@@ -3492,8 +3525,8 @@
     </row>
     <row r="93" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B93" s="66"/>
-      <c r="C93" s="109"/>
-      <c r="D93" s="109"/>
+      <c r="C93" s="124"/>
+      <c r="D93" s="124"/>
       <c r="E93" s="20" t="s">
         <v>20</v>
       </c>
@@ -3508,7 +3541,7 @@
     </row>
     <row r="94" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B94" s="66"/>
-      <c r="C94" s="114" t="s">
+      <c r="C94" s="128" t="s">
         <v>2</v>
       </c>
       <c r="D94" s="63" t="s">
@@ -3528,7 +3561,7 @@
     </row>
     <row r="95" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B95" s="66"/>
-      <c r="C95" s="108"/>
+      <c r="C95" s="123"/>
       <c r="D95" s="52" t="s">
         <v>28</v>
       </c>
@@ -3546,7 +3579,7 @@
     </row>
     <row r="96" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B96" s="66"/>
-      <c r="C96" s="109"/>
+      <c r="C96" s="124"/>
       <c r="D96" s="67"/>
       <c r="E96" s="20" t="s">
         <v>18</v>
@@ -3603,7 +3636,7 @@
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B102" s="66"/>
-      <c r="C102" s="118" t="s">
+      <c r="C102" s="126" t="s">
         <v>0</v>
       </c>
       <c r="D102" t="s">
@@ -3623,7 +3656,7 @@
     </row>
     <row r="103" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B103" s="66"/>
-      <c r="C103" s="117"/>
+      <c r="C103" s="127"/>
       <c r="D103" s="20" t="s">
         <v>28</v>
       </c>
@@ -3641,7 +3674,7 @@
     </row>
     <row r="104" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B104" s="66"/>
-      <c r="C104" s="114" t="s">
+      <c r="C104" s="128" t="s">
         <v>1</v>
       </c>
       <c r="D104" s="16" t="s">
@@ -3661,7 +3694,7 @@
     </row>
     <row r="105" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B105" s="66"/>
-      <c r="C105" s="108"/>
+      <c r="C105" s="123"/>
       <c r="D105" s="43" t="s">
         <v>28</v>
       </c>
@@ -3679,7 +3712,7 @@
     </row>
     <row r="106" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B106" s="66"/>
-      <c r="C106" s="114" t="s">
+      <c r="C106" s="128" t="s">
         <v>2</v>
       </c>
       <c r="D106" s="63" t="s">
@@ -3697,7 +3730,7 @@
     </row>
     <row r="107" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B107" s="66"/>
-      <c r="C107" s="109"/>
+      <c r="C107" s="124"/>
       <c r="D107" s="65" t="s">
         <v>28</v>
       </c>
@@ -3782,7 +3815,7 @@
       <c r="C115" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D115" s="124" t="s">
+      <c r="D115" s="134" t="s">
         <v>21</v>
       </c>
       <c r="E115" s="76" t="s">
@@ -3799,7 +3832,7 @@
     <row r="116" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B116" s="66"/>
       <c r="C116" s="37"/>
-      <c r="D116" s="125"/>
+      <c r="D116" s="135"/>
       <c r="E116" s="80" t="s">
         <v>20</v>
       </c>
@@ -3892,11 +3925,26 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="Q47:W47"/>
-    <mergeCell ref="P50:P53"/>
-    <mergeCell ref="P54:P59"/>
-    <mergeCell ref="Q54:Q55"/>
-    <mergeCell ref="Q56:Q57"/>
+    <mergeCell ref="C27:I27"/>
+    <mergeCell ref="C6:C14"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="C19:C22"/>
+    <mergeCell ref="D6:D10"/>
+    <mergeCell ref="D26:J26"/>
+    <mergeCell ref="C40:C43"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="C29:C33"/>
+    <mergeCell ref="C34:C39"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="D73:D74"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="D47:J47"/>
+    <mergeCell ref="C50:C53"/>
+    <mergeCell ref="C54:C59"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="D56:D57"/>
     <mergeCell ref="P60:P64"/>
     <mergeCell ref="Q61:Q62"/>
     <mergeCell ref="D115:D116"/>
@@ -3913,26 +3961,11 @@
     <mergeCell ref="D79:J79"/>
     <mergeCell ref="C71:C72"/>
     <mergeCell ref="C73:C76"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="D73:D74"/>
-    <mergeCell ref="C77:C78"/>
-    <mergeCell ref="D47:J47"/>
-    <mergeCell ref="C50:C53"/>
-    <mergeCell ref="C54:C59"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="C40:C43"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="C29:C33"/>
-    <mergeCell ref="C34:C39"/>
-    <mergeCell ref="C27:I27"/>
-    <mergeCell ref="C6:C14"/>
-    <mergeCell ref="C15:C18"/>
-    <mergeCell ref="C19:C22"/>
-    <mergeCell ref="D6:D10"/>
-    <mergeCell ref="D26:J26"/>
+    <mergeCell ref="Q47:W47"/>
+    <mergeCell ref="P50:P53"/>
+    <mergeCell ref="P54:P59"/>
+    <mergeCell ref="Q54:Q55"/>
+    <mergeCell ref="Q56:Q57"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="J6:J22">
@@ -3961,15 +3994,15 @@
   <sheetData>
     <row r="6" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C6" s="66"/>
-      <c r="D6" s="113" t="s">
+      <c r="D6" s="125" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="113"/>
-      <c r="F6" s="113"/>
-      <c r="G6" s="113"/>
-      <c r="H6" s="113"/>
-      <c r="I6" s="113"/>
-      <c r="J6" s="113"/>
+      <c r="E6" s="125"/>
+      <c r="F6" s="125"/>
+      <c r="G6" s="125"/>
+      <c r="H6" s="125"/>
+      <c r="I6" s="125"/>
+      <c r="J6" s="125"/>
       <c r="K6" s="66"/>
     </row>
     <row r="7" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4009,10 +4042,10 @@
       <c r="K8" s="66"/>
     </row>
     <row r="9" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C9" s="118" t="s">
+      <c r="C9" s="126" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="114" t="s">
+      <c r="D9" s="128" t="s">
         <v>25</v>
       </c>
       <c r="E9" s="34" t="s">
@@ -4036,8 +4069,8 @@
       <c r="K9" s="66"/>
     </row>
     <row r="10" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C10" s="117"/>
-      <c r="D10" s="115"/>
+      <c r="C10" s="127"/>
+      <c r="D10" s="136"/>
       <c r="E10" s="34" t="s">
         <v>20</v>
       </c>
@@ -4059,8 +4092,8 @@
       <c r="K10" s="66"/>
     </row>
     <row r="11" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C11" s="117"/>
-      <c r="D11" s="116" t="s">
+      <c r="C11" s="127"/>
+      <c r="D11" s="137" t="s">
         <v>5</v>
       </c>
       <c r="E11" s="34" t="s">
@@ -4084,8 +4117,8 @@
       <c r="K11" s="66"/>
     </row>
     <row r="12" spans="3:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C12" s="117"/>
-      <c r="D12" s="115"/>
+      <c r="C12" s="127"/>
+      <c r="D12" s="136"/>
       <c r="E12" s="34" t="s">
         <v>20</v>
       </c>
@@ -4107,7 +4140,7 @@
       <c r="K12" s="66"/>
     </row>
     <row r="13" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C13" s="117"/>
+      <c r="C13" s="127"/>
       <c r="D13" s="33" t="s">
         <v>6</v>
       </c>
@@ -4132,7 +4165,7 @@
       <c r="K13" s="66"/>
     </row>
     <row r="14" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="117"/>
+      <c r="C14" s="127"/>
       <c r="D14" s="17" t="s">
         <v>24</v>
       </c>
@@ -4147,10 +4180,10 @@
       <c r="K14" s="66"/>
     </row>
     <row r="15" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C15" s="114" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" s="118" t="s">
+      <c r="C15" s="128" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="126" t="s">
         <v>25</v>
       </c>
       <c r="E15" s="22" t="s">
@@ -4174,8 +4207,8 @@
       <c r="K15" s="66"/>
     </row>
     <row r="16" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="108"/>
-      <c r="D16" s="121"/>
+      <c r="C16" s="123"/>
+      <c r="D16" s="129"/>
       <c r="E16" s="26" t="s">
         <v>26</v>
       </c>
@@ -4197,8 +4230,8 @@
       <c r="K16" s="66"/>
     </row>
     <row r="17" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C17" s="108"/>
-      <c r="D17" s="122" t="s">
+      <c r="C17" s="123"/>
+      <c r="D17" s="130" t="s">
         <v>5</v>
       </c>
       <c r="E17" s="29" t="s">
@@ -4222,8 +4255,8 @@
       <c r="K17" s="66"/>
     </row>
     <row r="18" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C18" s="108"/>
-      <c r="D18" s="121"/>
+      <c r="C18" s="123"/>
+      <c r="D18" s="129"/>
       <c r="E18" s="32" t="s">
         <v>20</v>
       </c>
@@ -4245,8 +4278,8 @@
       <c r="K18" s="66"/>
     </row>
     <row r="19" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C19" s="108"/>
-      <c r="D19" s="116" t="s">
+      <c r="C19" s="123"/>
+      <c r="D19" s="137" t="s">
         <v>6</v>
       </c>
       <c r="E19" s="34" t="s">
@@ -4270,8 +4303,8 @@
       <c r="K19" s="66"/>
     </row>
     <row r="20" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C20" s="108"/>
-      <c r="D20" s="108"/>
+      <c r="C20" s="123"/>
+      <c r="D20" s="123"/>
       <c r="E20" s="3" t="s">
         <v>18</v>
       </c>
@@ -4293,7 +4326,7 @@
       <c r="K20" s="66"/>
     </row>
     <row r="21" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="109"/>
+      <c r="C21" s="124"/>
       <c r="D21" s="5" t="s">
         <v>24</v>
       </c>
@@ -4308,10 +4341,10 @@
       <c r="K21" s="66"/>
     </row>
     <row r="22" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C22" s="114" t="s">
+      <c r="C22" s="128" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="114" t="s">
+      <c r="D22" s="128" t="s">
         <v>25</v>
       </c>
       <c r="E22" t="s">
@@ -4335,8 +4368,8 @@
       <c r="K22" s="66"/>
     </row>
     <row r="23" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C23" s="108"/>
-      <c r="D23" s="108"/>
+      <c r="C23" s="123"/>
+      <c r="D23" s="123"/>
       <c r="E23" s="34" t="s">
         <v>17</v>
       </c>
@@ -4358,8 +4391,8 @@
       <c r="K23" s="66"/>
     </row>
     <row r="24" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C24" s="108"/>
-      <c r="D24" s="115"/>
+      <c r="C24" s="123"/>
+      <c r="D24" s="136"/>
       <c r="E24" s="104" t="s">
         <v>20</v>
       </c>
@@ -4381,8 +4414,8 @@
       <c r="K24" s="66"/>
     </row>
     <row r="25" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C25" s="108"/>
-      <c r="D25" s="122" t="s">
+      <c r="C25" s="123"/>
+      <c r="D25" s="130" t="s">
         <v>5</v>
       </c>
       <c r="E25" s="104" t="s">
@@ -4406,8 +4439,8 @@
       <c r="K25" s="66"/>
     </row>
     <row r="26" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C26" s="108"/>
-      <c r="D26" s="117"/>
+      <c r="C26" s="123"/>
+      <c r="D26" s="127"/>
       <c r="E26" s="29" t="s">
         <v>17</v>
       </c>
@@ -4429,8 +4462,8 @@
       <c r="K26" s="66"/>
     </row>
     <row r="27" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C27" s="108"/>
-      <c r="D27" s="117"/>
+      <c r="C27" s="123"/>
+      <c r="D27" s="127"/>
       <c r="E27" s="3" t="s">
         <v>18</v>
       </c>
@@ -4452,8 +4485,8 @@
       <c r="K27" s="66"/>
     </row>
     <row r="28" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C28" s="108"/>
-      <c r="D28" s="121"/>
+      <c r="C28" s="123"/>
+      <c r="D28" s="129"/>
       <c r="E28" s="32" t="s">
         <v>26</v>
       </c>
@@ -4475,7 +4508,7 @@
       <c r="K28" s="66"/>
     </row>
     <row r="29" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C29" s="108"/>
+      <c r="C29" s="123"/>
       <c r="D29" s="17" t="s">
         <v>6</v>
       </c>
@@ -4488,7 +4521,7 @@
       <c r="K29" s="66"/>
     </row>
     <row r="30" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C30" s="109"/>
+      <c r="C30" s="124"/>
       <c r="D30" s="5" t="s">
         <v>24</v>
       </c>
@@ -4515,15 +4548,15 @@
     </row>
     <row r="35" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C35" s="66"/>
-      <c r="D35" s="113" t="s">
+      <c r="D35" s="125" t="s">
         <v>49</v>
       </c>
-      <c r="E35" s="113"/>
-      <c r="F35" s="113"/>
-      <c r="G35" s="113"/>
-      <c r="H35" s="113"/>
-      <c r="I35" s="113"/>
-      <c r="J35" s="113"/>
+      <c r="E35" s="125"/>
+      <c r="F35" s="125"/>
+      <c r="G35" s="125"/>
+      <c r="H35" s="125"/>
+      <c r="I35" s="125"/>
+      <c r="J35" s="125"/>
       <c r="K35" s="66"/>
     </row>
     <row r="36" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4563,10 +4596,10 @@
       <c r="K37" s="66"/>
     </row>
     <row r="38" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C38" s="118" t="s">
+      <c r="C38" s="126" t="s">
         <v>0</v>
       </c>
-      <c r="D38" s="116" t="s">
+      <c r="D38" s="137" t="s">
         <v>5</v>
       </c>
       <c r="E38" s="21" t="s">
@@ -4590,8 +4623,8 @@
       <c r="K38" s="66"/>
     </row>
     <row r="39" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C39" s="117"/>
-      <c r="D39" s="115"/>
+      <c r="C39" s="127"/>
+      <c r="D39" s="136"/>
       <c r="E39" s="32" t="s">
         <v>20</v>
       </c>
@@ -4613,7 +4646,7 @@
       <c r="K39" s="66"/>
     </row>
     <row r="40" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C40" s="117"/>
+      <c r="C40" s="127"/>
       <c r="D40" s="33" t="s">
         <v>6</v>
       </c>
@@ -4638,7 +4671,7 @@
       <c r="K40" s="66"/>
     </row>
     <row r="41" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C41" s="127"/>
+      <c r="C41" s="142"/>
       <c r="D41" s="17" t="s">
         <v>24</v>
       </c>
@@ -4653,10 +4686,10 @@
       <c r="K41" s="66"/>
     </row>
     <row r="42" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C42" s="118" t="s">
-        <v>1</v>
-      </c>
-      <c r="D42" s="122" t="s">
+      <c r="C42" s="126" t="s">
+        <v>1</v>
+      </c>
+      <c r="D42" s="130" t="s">
         <v>5</v>
       </c>
       <c r="E42" s="29" t="s">
@@ -4680,8 +4713,8 @@
       <c r="K42" s="66"/>
     </row>
     <row r="43" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C43" s="117"/>
-      <c r="D43" s="121"/>
+      <c r="C43" s="127"/>
+      <c r="D43" s="129"/>
       <c r="E43" s="32" t="s">
         <v>20</v>
       </c>
@@ -4703,8 +4736,8 @@
       <c r="K43" s="66"/>
     </row>
     <row r="44" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C44" s="117"/>
-      <c r="D44" s="116" t="s">
+      <c r="C44" s="127"/>
+      <c r="D44" s="137" t="s">
         <v>6</v>
       </c>
       <c r="E44" s="34" t="s">
@@ -4728,8 +4761,8 @@
       <c r="K44" s="66"/>
     </row>
     <row r="45" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C45" s="117"/>
-      <c r="D45" s="108"/>
+      <c r="C45" s="127"/>
+      <c r="D45" s="123"/>
       <c r="E45" s="3" t="s">
         <v>18</v>
       </c>
@@ -4751,7 +4784,7 @@
       <c r="K45" s="66"/>
     </row>
     <row r="46" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C46" s="127"/>
+      <c r="C46" s="142"/>
       <c r="D46" s="5" t="s">
         <v>24</v>
       </c>
@@ -4766,10 +4799,10 @@
       <c r="K46" s="66"/>
     </row>
     <row r="47" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C47" s="118" t="s">
+      <c r="C47" s="126" t="s">
         <v>2</v>
       </c>
-      <c r="D47" s="122" t="s">
+      <c r="D47" s="130" t="s">
         <v>5</v>
       </c>
       <c r="E47" s="29" t="s">
@@ -4793,8 +4826,8 @@
       <c r="K47" s="66"/>
     </row>
     <row r="48" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C48" s="117"/>
-      <c r="D48" s="117"/>
+      <c r="C48" s="127"/>
+      <c r="D48" s="127"/>
       <c r="E48" s="3" t="s">
         <v>17</v>
       </c>
@@ -4816,8 +4849,8 @@
       <c r="K48" s="66"/>
     </row>
     <row r="49" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C49" s="117"/>
-      <c r="D49" s="117"/>
+      <c r="C49" s="127"/>
+      <c r="D49" s="127"/>
       <c r="E49" s="3" t="s">
         <v>18</v>
       </c>
@@ -4839,8 +4872,8 @@
       <c r="K49" s="66"/>
     </row>
     <row r="50" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C50" s="117"/>
-      <c r="D50" s="121"/>
+      <c r="C50" s="127"/>
+      <c r="D50" s="129"/>
       <c r="E50" s="32" t="s">
         <v>26</v>
       </c>
@@ -4862,7 +4895,7 @@
       <c r="K50" s="66"/>
     </row>
     <row r="51" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C51" s="117"/>
+      <c r="C51" s="127"/>
       <c r="D51" s="17" t="s">
         <v>6</v>
       </c>
@@ -4875,7 +4908,7 @@
       <c r="K51" s="66"/>
     </row>
     <row r="52" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C52" s="127"/>
+      <c r="C52" s="142"/>
       <c r="D52" s="5" t="s">
         <v>24</v>
       </c>
@@ -4902,12 +4935,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C47:C52"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="D47:D50"/>
-    <mergeCell ref="D35:J35"/>
-    <mergeCell ref="D38:D39"/>
     <mergeCell ref="D6:J6"/>
     <mergeCell ref="C38:C41"/>
     <mergeCell ref="C42:C46"/>
@@ -4921,6 +4948,12 @@
     <mergeCell ref="D19:D20"/>
     <mergeCell ref="D22:D24"/>
     <mergeCell ref="D25:D28"/>
+    <mergeCell ref="C47:C52"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="D47:D50"/>
+    <mergeCell ref="D35:J35"/>
+    <mergeCell ref="D38:D39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4995,7 +5028,7 @@
     </row>
     <row r="5" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C5" s="66"/>
-      <c r="D5" s="108"/>
+      <c r="D5" s="123"/>
       <c r="E5" s="3"/>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
@@ -5008,7 +5041,7 @@
     </row>
     <row r="6" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C6" s="66"/>
-      <c r="D6" s="108"/>
+      <c r="D6" s="123"/>
       <c r="E6" s="3"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
@@ -5021,7 +5054,7 @@
     </row>
     <row r="7" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C7" s="66"/>
-      <c r="D7" s="108"/>
+      <c r="D7" s="123"/>
       <c r="E7" s="3"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
@@ -5034,7 +5067,7 @@
     </row>
     <row r="8" spans="3:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C8" s="66"/>
-      <c r="D8" s="109"/>
+      <c r="D8" s="124"/>
       <c r="E8" s="5"/>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
@@ -5047,7 +5080,7 @@
     </row>
     <row r="9" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C9" s="66"/>
-      <c r="D9" s="108"/>
+      <c r="D9" s="123"/>
       <c r="E9" s="3"/>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
@@ -5060,7 +5093,7 @@
     </row>
     <row r="10" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C10" s="66"/>
-      <c r="D10" s="108"/>
+      <c r="D10" s="123"/>
       <c r="E10" s="3"/>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
@@ -5073,7 +5106,7 @@
     </row>
     <row r="11" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C11" s="66"/>
-      <c r="D11" s="108"/>
+      <c r="D11" s="123"/>
       <c r="E11" s="3"/>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
@@ -5086,7 +5119,7 @@
     </row>
     <row r="12" spans="3:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C12" s="66"/>
-      <c r="D12" s="109"/>
+      <c r="D12" s="124"/>
       <c r="E12" s="5"/>
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
@@ -5099,74 +5132,74 @@
     </row>
     <row r="13" spans="3:29" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C13" s="66"/>
-      <c r="D13" s="128" t="s">
+      <c r="D13" s="143" t="s">
         <v>50</v>
       </c>
-      <c r="E13" s="128"/>
-      <c r="F13" s="128"/>
-      <c r="G13" s="128"/>
-      <c r="H13" s="128"/>
-      <c r="I13" s="128"/>
-      <c r="J13" s="128"/>
+      <c r="E13" s="143"/>
+      <c r="F13" s="143"/>
+      <c r="G13" s="143"/>
+      <c r="H13" s="143"/>
+      <c r="I13" s="143"/>
+      <c r="J13" s="143"/>
       <c r="K13" s="52"/>
       <c r="L13" s="66"/>
       <c r="M13" s="66"/>
     </row>
     <row r="14" spans="3:29" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C14" s="66"/>
-      <c r="D14" s="129"/>
-      <c r="E14" s="129"/>
-      <c r="F14" s="129"/>
-      <c r="G14" s="129"/>
-      <c r="H14" s="129"/>
-      <c r="I14" s="129"/>
-      <c r="J14" s="129"/>
+      <c r="D14" s="144"/>
+      <c r="E14" s="144"/>
+      <c r="F14" s="144"/>
+      <c r="G14" s="144"/>
+      <c r="H14" s="144"/>
+      <c r="I14" s="144"/>
+      <c r="J14" s="144"/>
       <c r="K14" s="52"/>
       <c r="L14" s="66"/>
-      <c r="M14" s="128" t="s">
+      <c r="M14" s="143" t="s">
         <v>51</v>
       </c>
-      <c r="N14" s="128"/>
-      <c r="O14" s="128"/>
-      <c r="P14" s="128"/>
-      <c r="Q14" s="128"/>
-      <c r="R14" s="128"/>
-      <c r="S14" s="128"/>
-      <c r="W14" s="128" t="s">
+      <c r="N14" s="143"/>
+      <c r="O14" s="143"/>
+      <c r="P14" s="143"/>
+      <c r="Q14" s="143"/>
+      <c r="R14" s="143"/>
+      <c r="S14" s="143"/>
+      <c r="W14" s="143" t="s">
         <v>52</v>
       </c>
-      <c r="X14" s="128"/>
-      <c r="Y14" s="128"/>
-      <c r="Z14" s="128"/>
-      <c r="AA14" s="128"/>
-      <c r="AB14" s="128"/>
-      <c r="AC14" s="128"/>
+      <c r="X14" s="143"/>
+      <c r="Y14" s="143"/>
+      <c r="Z14" s="143"/>
+      <c r="AA14" s="143"/>
+      <c r="AB14" s="143"/>
+      <c r="AC14" s="143"/>
     </row>
     <row r="15" spans="3:29" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C15" s="66"/>
-      <c r="D15" s="129"/>
-      <c r="E15" s="129"/>
-      <c r="F15" s="129"/>
-      <c r="G15" s="129"/>
-      <c r="H15" s="129"/>
-      <c r="I15" s="129"/>
-      <c r="J15" s="129"/>
+      <c r="D15" s="144"/>
+      <c r="E15" s="144"/>
+      <c r="F15" s="144"/>
+      <c r="G15" s="144"/>
+      <c r="H15" s="144"/>
+      <c r="I15" s="144"/>
+      <c r="J15" s="144"/>
       <c r="K15" s="52"/>
       <c r="L15" s="66"/>
-      <c r="M15" s="129"/>
-      <c r="N15" s="129"/>
-      <c r="O15" s="129"/>
-      <c r="P15" s="129"/>
-      <c r="Q15" s="129"/>
-      <c r="R15" s="129"/>
-      <c r="S15" s="129"/>
-      <c r="W15" s="129"/>
-      <c r="X15" s="129"/>
-      <c r="Y15" s="129"/>
-      <c r="Z15" s="129"/>
-      <c r="AA15" s="129"/>
-      <c r="AB15" s="129"/>
-      <c r="AC15" s="129"/>
+      <c r="M15" s="144"/>
+      <c r="N15" s="144"/>
+      <c r="O15" s="144"/>
+      <c r="P15" s="144"/>
+      <c r="Q15" s="144"/>
+      <c r="R15" s="144"/>
+      <c r="S15" s="144"/>
+      <c r="W15" s="144"/>
+      <c r="X15" s="144"/>
+      <c r="Y15" s="144"/>
+      <c r="Z15" s="144"/>
+      <c r="AA15" s="144"/>
+      <c r="AB15" s="144"/>
+      <c r="AC15" s="144"/>
     </row>
     <row r="16" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C16" s="66"/>
@@ -5179,24 +5212,24 @@
       <c r="J16" s="12"/>
       <c r="K16" s="52"/>
       <c r="L16" s="66"/>
-      <c r="M16" s="129"/>
-      <c r="N16" s="129"/>
-      <c r="O16" s="129"/>
-      <c r="P16" s="129"/>
-      <c r="Q16" s="129"/>
-      <c r="R16" s="129"/>
-      <c r="S16" s="129"/>
-      <c r="W16" s="129"/>
-      <c r="X16" s="129"/>
-      <c r="Y16" s="129"/>
-      <c r="Z16" s="129"/>
-      <c r="AA16" s="129"/>
-      <c r="AB16" s="129"/>
-      <c r="AC16" s="129"/>
+      <c r="M16" s="144"/>
+      <c r="N16" s="144"/>
+      <c r="O16" s="144"/>
+      <c r="P16" s="144"/>
+      <c r="Q16" s="144"/>
+      <c r="R16" s="144"/>
+      <c r="S16" s="144"/>
+      <c r="W16" s="144"/>
+      <c r="X16" s="144"/>
+      <c r="Y16" s="144"/>
+      <c r="Z16" s="144"/>
+      <c r="AA16" s="144"/>
+      <c r="AB16" s="144"/>
+      <c r="AC16" s="144"/>
     </row>
     <row r="17" spans="3:30" x14ac:dyDescent="0.2">
       <c r="C17" s="66"/>
-      <c r="D17" s="108"/>
+      <c r="D17" s="123"/>
       <c r="E17" s="3"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
@@ -5209,7 +5242,7 @@
     </row>
     <row r="18" spans="3:30" x14ac:dyDescent="0.2">
       <c r="C18" s="66"/>
-      <c r="D18" s="108"/>
+      <c r="D18" s="123"/>
       <c r="E18" s="3"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
@@ -5222,7 +5255,7 @@
     </row>
     <row r="19" spans="3:30" x14ac:dyDescent="0.2">
       <c r="C19" s="66"/>
-      <c r="D19" s="108"/>
+      <c r="D19" s="123"/>
       <c r="E19" s="3"/>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
@@ -5235,7 +5268,7 @@
     </row>
     <row r="20" spans="3:30" x14ac:dyDescent="0.2">
       <c r="C20" s="66"/>
-      <c r="D20" s="108"/>
+      <c r="D20" s="123"/>
       <c r="E20" s="3"/>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
@@ -6843,18 +6876,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95BB507F-C9F5-F04E-AC61-C149D982E15D}">
-  <dimension ref="J28:U52"/>
+  <dimension ref="J28:U70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H25" zoomScale="150" workbookViewId="0">
-      <selection activeCell="Q44" sqref="Q44"/>
+    <sheetView tabSelected="1" topLeftCell="E49" zoomScale="150" workbookViewId="0">
+      <selection activeCell="N68" sqref="N68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="10.83203125" customWidth="1"/>
     <col min="8" max="8" width="39.5" customWidth="1"/>
-    <col min="11" max="11" width="19.1640625" customWidth="1"/>
-    <col min="12" max="12" width="7.1640625" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" customWidth="1"/>
+    <col min="11" max="11" width="12.83203125" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" customWidth="1"/>
     <col min="13" max="13" width="10.5" customWidth="1"/>
     <col min="14" max="14" width="11.6640625" customWidth="1"/>
     <col min="18" max="18" width="12.6640625" customWidth="1"/>
@@ -6898,148 +6932,148 @@
       <c r="N30" s="66"/>
       <c r="O30" s="66"/>
       <c r="P30" s="66"/>
-      <c r="Q30" s="130" t="s">
+      <c r="Q30" s="108" t="s">
         <v>59</v>
       </c>
-      <c r="R30" s="130" t="s">
+      <c r="R30" s="108" t="s">
         <v>62</v>
       </c>
-      <c r="S30" s="130" t="s">
+      <c r="S30" s="108" t="s">
         <v>58</v>
       </c>
-      <c r="T30" s="130" t="s">
+      <c r="T30" s="108" t="s">
         <v>63</v>
       </c>
       <c r="U30" s="66"/>
     </row>
     <row r="31" spans="10:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J31" s="66"/>
-      <c r="K31" s="130" t="s">
+      <c r="K31" s="108" t="s">
         <v>59</v>
       </c>
-      <c r="L31" s="130" t="s">
+      <c r="L31" s="108" t="s">
         <v>62</v>
       </c>
-      <c r="M31" s="130" t="s">
+      <c r="M31" s="108" t="s">
         <v>58</v>
       </c>
-      <c r="N31" s="130" t="s">
+      <c r="N31" s="108" t="s">
         <v>63</v>
       </c>
       <c r="O31" s="66"/>
       <c r="P31" s="66"/>
-      <c r="Q31" s="142" t="s">
+      <c r="Q31" s="120" t="s">
         <v>64</v>
       </c>
-      <c r="R31" s="139" t="s">
+      <c r="R31" s="117" t="s">
         <v>65</v>
       </c>
-      <c r="S31" s="132">
+      <c r="S31" s="110">
         <v>4</v>
       </c>
-      <c r="T31" s="132">
+      <c r="T31" s="110">
         <v>54.021970000000003</v>
       </c>
       <c r="U31" s="66"/>
     </row>
     <row r="32" spans="10:21" x14ac:dyDescent="0.2">
       <c r="J32" s="66"/>
-      <c r="K32" s="131" t="s">
+      <c r="K32" s="146" t="s">
         <v>15</v>
       </c>
-      <c r="L32" s="139" t="s">
+      <c r="L32" s="117" t="s">
         <v>60</v>
       </c>
-      <c r="M32" s="132">
+      <c r="M32" s="110">
         <v>6.820417</v>
       </c>
-      <c r="N32" s="137">
+      <c r="N32" s="115">
         <v>25.528949999999998</v>
       </c>
       <c r="O32" s="66"/>
       <c r="P32" s="66"/>
-      <c r="Q32" s="143" t="s">
+      <c r="Q32" s="121" t="s">
         <v>5</v>
       </c>
-      <c r="R32" s="140" t="s">
+      <c r="R32" s="118" t="s">
         <v>65</v>
       </c>
-      <c r="S32" s="134">
+      <c r="S32" s="112">
         <v>5</v>
       </c>
-      <c r="T32" s="134">
+      <c r="T32" s="112">
         <v>59.862450000000003</v>
       </c>
       <c r="U32" s="66"/>
     </row>
     <row r="33" spans="10:21" x14ac:dyDescent="0.2">
       <c r="J33" s="66"/>
-      <c r="K33" s="133"/>
-      <c r="L33" s="140" t="s">
+      <c r="K33" s="147"/>
+      <c r="L33" s="118" t="s">
         <v>61</v>
       </c>
-      <c r="M33" s="134">
+      <c r="M33" s="112">
         <v>7.2917740000000002</v>
       </c>
-      <c r="N33" s="134">
+      <c r="N33" s="112">
         <v>28.326519999999999</v>
       </c>
       <c r="O33" s="66"/>
       <c r="P33" s="66"/>
-      <c r="Q33" s="144" t="s">
+      <c r="Q33" s="122" t="s">
         <v>6</v>
       </c>
-      <c r="R33" s="141" t="s">
+      <c r="R33" s="119" t="s">
         <v>65</v>
       </c>
-      <c r="S33" s="136">
+      <c r="S33" s="114">
         <v>9.2653459999999992</v>
       </c>
-      <c r="T33" s="136">
+      <c r="T33" s="114">
         <v>80.715180000000004</v>
       </c>
       <c r="U33" s="66"/>
     </row>
     <row r="34" spans="10:21" x14ac:dyDescent="0.2">
       <c r="J34" s="66"/>
-      <c r="K34" s="135" t="s">
+      <c r="K34" s="148" t="s">
         <v>5</v>
       </c>
-      <c r="L34" s="141" t="s">
+      <c r="L34" s="119" t="s">
         <v>60</v>
       </c>
-      <c r="M34" s="136">
+      <c r="M34" s="114">
         <v>5</v>
       </c>
-      <c r="N34" s="138">
+      <c r="N34" s="116">
         <v>36.09104</v>
       </c>
       <c r="O34" s="66"/>
       <c r="P34" s="66"/>
-      <c r="Q34" s="143" t="s">
+      <c r="Q34" s="121" t="s">
         <v>24</v>
       </c>
-      <c r="R34" s="140" t="s">
+      <c r="R34" s="118" t="s">
         <v>65</v>
       </c>
-      <c r="S34" s="134">
+      <c r="S34" s="112">
         <v>7.7588999999999997</v>
       </c>
-      <c r="T34" s="134">
+      <c r="T34" s="112">
         <v>92.156210000000002</v>
       </c>
       <c r="U34" s="66"/>
     </row>
     <row r="35" spans="10:21" x14ac:dyDescent="0.2">
       <c r="J35" s="66"/>
-      <c r="K35" s="133"/>
-      <c r="L35" s="140" t="s">
+      <c r="K35" s="147"/>
+      <c r="L35" s="118" t="s">
         <v>61</v>
       </c>
-      <c r="M35" s="134">
+      <c r="M35" s="112">
         <v>5.9688330000000001</v>
       </c>
-      <c r="N35" s="134">
+      <c r="N35" s="112">
         <v>50.782449999999997</v>
       </c>
       <c r="O35" s="66"/>
@@ -7052,16 +7086,16 @@
     </row>
     <row r="36" spans="10:21" x14ac:dyDescent="0.2">
       <c r="J36" s="66"/>
-      <c r="K36" s="135" t="s">
+      <c r="K36" s="148" t="s">
         <v>6</v>
       </c>
-      <c r="L36" s="141" t="s">
+      <c r="L36" s="119" t="s">
         <v>60</v>
       </c>
-      <c r="M36" s="136">
+      <c r="M36" s="114">
         <v>6.9876889999999996</v>
       </c>
-      <c r="N36" s="138">
+      <c r="N36" s="116">
         <v>70.550629999999998</v>
       </c>
       <c r="O36" s="66"/>
@@ -7074,44 +7108,44 @@
     </row>
     <row r="37" spans="10:21" x14ac:dyDescent="0.2">
       <c r="J37" s="66"/>
-      <c r="K37" s="133"/>
-      <c r="L37" s="140" t="s">
+      <c r="K37" s="147"/>
+      <c r="L37" s="118" t="s">
         <v>61</v>
       </c>
-      <c r="M37" s="134">
+      <c r="M37" s="112">
         <v>7.9859780000000002</v>
       </c>
-      <c r="N37" s="134">
+      <c r="N37" s="112">
         <v>79.455860000000001</v>
       </c>
       <c r="O37" s="66"/>
     </row>
     <row r="38" spans="10:21" x14ac:dyDescent="0.2">
       <c r="J38" s="66"/>
-      <c r="K38" s="135" t="s">
+      <c r="K38" s="148" t="s">
         <v>12</v>
       </c>
-      <c r="L38" s="141" t="s">
+      <c r="L38" s="119" t="s">
         <v>60</v>
       </c>
-      <c r="M38" s="136">
+      <c r="M38" s="114">
         <v>12.85126</v>
       </c>
-      <c r="N38" s="138">
+      <c r="N38" s="116">
         <v>63.976089999999999</v>
       </c>
       <c r="O38" s="66"/>
     </row>
     <row r="39" spans="10:21" x14ac:dyDescent="0.2">
       <c r="J39" s="66"/>
-      <c r="K39" s="133"/>
-      <c r="L39" s="140" t="s">
+      <c r="K39" s="147"/>
+      <c r="L39" s="118" t="s">
         <v>61</v>
       </c>
-      <c r="M39" s="134">
+      <c r="M39" s="112">
         <v>12.693714</v>
       </c>
-      <c r="N39" s="134">
+      <c r="N39" s="112">
         <v>83.763069999999999</v>
       </c>
       <c r="O39" s="66"/>
@@ -7124,140 +7158,367 @@
       <c r="N40" s="66"/>
       <c r="O40" s="66"/>
     </row>
-    <row r="43" spans="10:21" x14ac:dyDescent="0.2">
-      <c r="J43" s="145" t="s">
+    <row r="42" spans="10:21" x14ac:dyDescent="0.2">
+      <c r="K42" s="145" t="s">
         <v>67</v>
       </c>
-      <c r="K43" s="145"/>
-      <c r="L43" s="145"/>
-      <c r="M43" s="145"/>
-    </row>
-    <row r="44" spans="10:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J44" s="130" t="s">
+      <c r="L42" s="145"/>
+      <c r="M42" s="145"/>
+      <c r="N42" s="145"/>
+    </row>
+    <row r="43" spans="10:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K43" s="108" t="s">
         <v>59</v>
       </c>
-      <c r="K44" s="130" t="s">
+      <c r="L43" s="108" t="s">
         <v>62</v>
       </c>
-      <c r="L44" s="130" t="s">
+      <c r="M43" s="108" t="s">
         <v>58</v>
       </c>
-      <c r="M44" s="130" t="s">
+      <c r="N43" s="108" t="s">
         <v>63</v>
       </c>
     </row>
+    <row r="44" spans="10:21" x14ac:dyDescent="0.2">
+      <c r="K44" s="109" t="s">
+        <v>15</v>
+      </c>
+      <c r="L44" s="117" t="s">
+        <v>60</v>
+      </c>
+      <c r="M44" s="110">
+        <v>7.8456219999999997</v>
+      </c>
+      <c r="N44" s="115">
+        <v>29.234929999999999</v>
+      </c>
+    </row>
     <row r="45" spans="10:21" x14ac:dyDescent="0.2">
-      <c r="J45" s="131" t="s">
-        <v>15</v>
-      </c>
-      <c r="K45" s="139" t="s">
+      <c r="K45" s="111"/>
+      <c r="L45" s="118" t="s">
+        <v>61</v>
+      </c>
+      <c r="M45" s="112">
+        <v>7.0123470000000001</v>
+      </c>
+      <c r="N45" s="112">
+        <v>45.306550000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="10:21" x14ac:dyDescent="0.2">
+      <c r="K46" s="113" t="s">
+        <v>5</v>
+      </c>
+      <c r="L46" s="119" t="s">
         <v>60</v>
       </c>
-      <c r="L45">
-        <v>7.8456219999999997</v>
-      </c>
-      <c r="M45">
-        <v>29.234929999999999</v>
-      </c>
-    </row>
-    <row r="46" spans="10:21" x14ac:dyDescent="0.2">
-      <c r="J46" s="133"/>
-      <c r="K46" s="140" t="s">
+      <c r="M46" s="114">
+        <v>6.5228169999999999</v>
+      </c>
+      <c r="N46" s="116">
+        <v>42.06091</v>
+      </c>
+    </row>
+    <row r="47" spans="10:21" x14ac:dyDescent="0.2">
+      <c r="K47" s="111"/>
+      <c r="L47" s="118" t="s">
         <v>61</v>
       </c>
-      <c r="L46">
-        <v>7.0123470000000001</v>
-      </c>
-      <c r="M46">
-        <v>45.306550000000001</v>
-      </c>
-    </row>
-    <row r="47" spans="10:21" x14ac:dyDescent="0.2">
-      <c r="J47" s="135" t="s">
+      <c r="M47" s="112">
+        <v>5.9688330000000001</v>
+      </c>
+      <c r="N47" s="112">
+        <v>50.782449999999997</v>
+      </c>
+    </row>
+    <row r="48" spans="10:21" x14ac:dyDescent="0.2">
+      <c r="K48" s="113" t="s">
+        <v>6</v>
+      </c>
+      <c r="L48" s="119" t="s">
+        <v>60</v>
+      </c>
+      <c r="M48" s="114">
+        <v>6.3269760000000002</v>
+      </c>
+      <c r="N48" s="116">
+        <v>83.92165</v>
+      </c>
+    </row>
+    <row r="49" spans="10:15" x14ac:dyDescent="0.2">
+      <c r="K49" s="111"/>
+      <c r="L49" s="118" t="s">
+        <v>61</v>
+      </c>
+      <c r="M49" s="112">
+        <v>7.9859780000000002</v>
+      </c>
+      <c r="N49" s="112">
+        <v>79.455860000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="10:15" x14ac:dyDescent="0.2">
+      <c r="K50" s="113" t="s">
+        <v>12</v>
+      </c>
+      <c r="L50" s="119" t="s">
+        <v>60</v>
+      </c>
+      <c r="M50" s="114">
+        <v>11.056463000000001</v>
+      </c>
+      <c r="N50" s="116">
+        <v>82.390469999999993</v>
+      </c>
+    </row>
+    <row r="51" spans="10:15" x14ac:dyDescent="0.2">
+      <c r="K51" s="111"/>
+      <c r="L51" s="118" t="s">
+        <v>61</v>
+      </c>
+      <c r="M51" s="112">
+        <v>12.693714</v>
+      </c>
+      <c r="N51" s="112">
+        <v>83.763069999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="10:15" x14ac:dyDescent="0.2">
+      <c r="J53" s="66"/>
+      <c r="K53" s="66"/>
+      <c r="L53" s="66"/>
+      <c r="M53" s="66"/>
+      <c r="N53" s="66"/>
+      <c r="O53" s="66"/>
+    </row>
+    <row r="54" spans="10:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J54" s="66"/>
+      <c r="K54" s="108" t="s">
+        <v>59</v>
+      </c>
+      <c r="L54" s="108" t="s">
+        <v>62</v>
+      </c>
+      <c r="M54" s="108" t="s">
+        <v>58</v>
+      </c>
+      <c r="N54" s="108" t="s">
+        <v>63</v>
+      </c>
+      <c r="O54" s="66"/>
+    </row>
+    <row r="55" spans="10:15" x14ac:dyDescent="0.2">
+      <c r="J55" s="66"/>
+      <c r="K55" s="149" t="s">
+        <v>25</v>
+      </c>
+      <c r="L55" s="110" t="s">
+        <v>60</v>
+      </c>
+      <c r="M55" s="158">
+        <v>6.820417</v>
+      </c>
+      <c r="N55" s="158">
+        <v>25.528949999999998</v>
+      </c>
+      <c r="O55" s="66"/>
+    </row>
+    <row r="56" spans="10:15" x14ac:dyDescent="0.2">
+      <c r="J56" s="66"/>
+      <c r="K56" s="150"/>
+      <c r="L56" s="157" t="s">
+        <v>61</v>
+      </c>
+      <c r="M56" s="159">
+        <v>7.2917740000000002</v>
+      </c>
+      <c r="N56" s="159">
+        <v>28.326519999999999</v>
+      </c>
+      <c r="O56" s="66"/>
+    </row>
+    <row r="57" spans="10:15" x14ac:dyDescent="0.2">
+      <c r="J57" s="66"/>
+      <c r="K57" s="151"/>
+      <c r="L57" s="112" t="s">
+        <v>68</v>
+      </c>
+      <c r="M57" s="160">
+        <v>8.1715710000000001</v>
+      </c>
+      <c r="N57" s="154">
+        <v>23.440470000000001</v>
+      </c>
+      <c r="O57" s="66"/>
+    </row>
+    <row r="58" spans="10:15" x14ac:dyDescent="0.2">
+      <c r="J58" s="66"/>
+      <c r="K58" s="152" t="s">
         <v>5</v>
       </c>
-      <c r="K47" s="141" t="s">
+      <c r="L58" s="114" t="s">
         <v>60</v>
       </c>
-      <c r="L47">
-        <v>6.5228169999999999</v>
-      </c>
-      <c r="M47">
-        <v>42.06091</v>
-      </c>
-    </row>
-    <row r="48" spans="10:21" x14ac:dyDescent="0.2">
-      <c r="J48" s="133"/>
-      <c r="K48" s="140" t="s">
+      <c r="M58" s="161">
+        <v>5</v>
+      </c>
+      <c r="N58" s="161">
+        <v>36.09104</v>
+      </c>
+      <c r="O58" s="66"/>
+    </row>
+    <row r="59" spans="10:15" x14ac:dyDescent="0.2">
+      <c r="J59" s="66"/>
+      <c r="K59" s="150"/>
+      <c r="L59" s="157" t="s">
         <v>61</v>
       </c>
-      <c r="L48">
-        <v>5.9688330000000001</v>
-      </c>
-      <c r="M48">
-        <v>50.782449999999997</v>
-      </c>
-    </row>
-    <row r="49" spans="10:13" x14ac:dyDescent="0.2">
-      <c r="J49" s="135" t="s">
+      <c r="M59" s="159">
+        <v>5.6870779999999996</v>
+      </c>
+      <c r="N59" s="159">
+        <v>38.273609999999998</v>
+      </c>
+      <c r="O59" s="66"/>
+    </row>
+    <row r="60" spans="10:15" x14ac:dyDescent="0.2">
+      <c r="J60" s="66"/>
+      <c r="K60" s="151"/>
+      <c r="L60" s="112" t="s">
+        <v>68</v>
+      </c>
+      <c r="M60" s="160">
+        <v>6.6245799999999999</v>
+      </c>
+      <c r="N60" s="154">
+        <v>34.143740000000001</v>
+      </c>
+      <c r="O60" s="66"/>
+    </row>
+    <row r="61" spans="10:15" x14ac:dyDescent="0.2">
+      <c r="J61" s="66"/>
+      <c r="K61" s="152" t="s">
         <v>6</v>
       </c>
-      <c r="K49" s="141" t="s">
+      <c r="L61" s="114" t="s">
         <v>60</v>
       </c>
-      <c r="L49">
-        <v>6.3269760000000002</v>
-      </c>
-      <c r="M49">
-        <v>83.92165</v>
-      </c>
-    </row>
-    <row r="50" spans="10:13" x14ac:dyDescent="0.2">
-      <c r="J50" s="133"/>
-      <c r="K50" s="140" t="s">
+      <c r="M61" s="161">
+        <v>6.9876889999999996</v>
+      </c>
+      <c r="N61" s="161">
+        <v>70.550629999999998</v>
+      </c>
+      <c r="O61" s="66"/>
+    </row>
+    <row r="62" spans="10:15" x14ac:dyDescent="0.2">
+      <c r="J62" s="66"/>
+      <c r="K62" s="150"/>
+      <c r="L62" s="157" t="s">
         <v>61</v>
       </c>
-      <c r="L50">
-        <v>7.9859780000000002</v>
-      </c>
-      <c r="M50">
-        <v>79.455860000000001</v>
-      </c>
-    </row>
-    <row r="51" spans="10:13" x14ac:dyDescent="0.2">
-      <c r="J51" s="135" t="s">
-        <v>12</v>
-      </c>
-      <c r="K51" s="141" t="s">
+      <c r="M62" s="159">
+        <v>5.6009580000000003</v>
+      </c>
+      <c r="N62" s="159">
+        <v>70.076509999999999</v>
+      </c>
+      <c r="O62" s="66"/>
+    </row>
+    <row r="63" spans="10:15" x14ac:dyDescent="0.2">
+      <c r="J63" s="66"/>
+      <c r="K63" s="151"/>
+      <c r="L63" s="112" t="s">
+        <v>68</v>
+      </c>
+      <c r="M63" s="160">
+        <v>8.2312200000000004</v>
+      </c>
+      <c r="N63" s="154">
+        <v>69.124020000000002</v>
+      </c>
+      <c r="O63" s="66"/>
+    </row>
+    <row r="64" spans="10:15" x14ac:dyDescent="0.2">
+      <c r="J64" s="66"/>
+      <c r="K64" s="152" t="s">
+        <v>24</v>
+      </c>
+      <c r="L64" s="114" t="s">
         <v>60</v>
       </c>
-      <c r="L51">
-        <v>11.056463000000001</v>
-      </c>
-      <c r="M51">
-        <v>82.390469999999993</v>
-      </c>
-    </row>
-    <row r="52" spans="10:13" x14ac:dyDescent="0.2">
-      <c r="J52" s="133"/>
-      <c r="K52" s="140" t="s">
+      <c r="M64" s="161">
+        <v>12.85126</v>
+      </c>
+      <c r="N64" s="155">
+        <v>63.976089999999999</v>
+      </c>
+      <c r="O64" s="66"/>
+    </row>
+    <row r="65" spans="10:15" x14ac:dyDescent="0.2">
+      <c r="J65" s="66"/>
+      <c r="K65" s="150"/>
+      <c r="L65" s="157" t="s">
         <v>61</v>
       </c>
-      <c r="L52">
-        <v>12.693714</v>
-      </c>
-      <c r="M52">
-        <v>83.763069999999999</v>
-      </c>
+      <c r="M65" s="159">
+        <v>12.997923999999999</v>
+      </c>
+      <c r="N65" s="156">
+        <v>61.583039999999997</v>
+      </c>
+      <c r="O65" s="66"/>
+    </row>
+    <row r="66" spans="10:15" x14ac:dyDescent="0.2">
+      <c r="J66" s="66"/>
+      <c r="K66" s="151"/>
+      <c r="L66" s="112" t="s">
+        <v>68</v>
+      </c>
+      <c r="M66" s="160">
+        <v>14.149485</v>
+      </c>
+      <c r="N66" s="153">
+        <v>61.850610000000003</v>
+      </c>
+      <c r="O66" s="66"/>
+    </row>
+    <row r="67" spans="10:15" x14ac:dyDescent="0.2">
+      <c r="J67" s="66"/>
+      <c r="K67" s="66"/>
+      <c r="L67" s="66"/>
+      <c r="M67" s="66"/>
+      <c r="N67" s="66"/>
+      <c r="O67" s="66"/>
+    </row>
+    <row r="68" spans="10:15" x14ac:dyDescent="0.2">
+      <c r="J68" s="66"/>
+      <c r="K68" s="66"/>
+      <c r="L68" s="66"/>
+      <c r="M68" s="66"/>
+      <c r="N68" s="66"/>
+      <c r="O68" s="66"/>
+    </row>
+    <row r="69" spans="10:15" x14ac:dyDescent="0.2">
+      <c r="J69" s="66"/>
+      <c r="K69" s="66"/>
+      <c r="L69" s="66"/>
+      <c r="M69" s="66"/>
+      <c r="N69" s="66"/>
+      <c r="O69" s="66"/>
+    </row>
+    <row r="70" spans="10:15" x14ac:dyDescent="0.2">
+      <c r="O70" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="J45:J46"/>
-    <mergeCell ref="J47:J48"/>
-    <mergeCell ref="J49:J50"/>
-    <mergeCell ref="J51:J52"/>
+    <mergeCell ref="K55:K57"/>
+    <mergeCell ref="K58:K60"/>
+    <mergeCell ref="K61:K63"/>
+    <mergeCell ref="K64:K66"/>
     <mergeCell ref="K29:N29"/>
-    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="K42:N42"/>
     <mergeCell ref="K32:K33"/>
     <mergeCell ref="K34:K35"/>
     <mergeCell ref="K36:K37"/>

</xml_diff>